<commit_message>
Fix cell types in data.xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/hb16606_bristol_ac_uk/Documents/Documents/SPE/Green-Credentials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hb16606\OneDrive - University of Bristol\Documents\SPE\Green-Credentials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFBF31D5-3A61-4285-ACCC-A949CF96641E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{EFBF31D5-3A61-4285-ACCC-A949CF96641E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{40418A72-4656-4CA8-AD08-CE8562C8082B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{0C7B78C3-690B-478C-8020-AF23CEA86F9E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1" xr2:uid="{0C7B78C3-690B-478C-8020-AF23CEA86F9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Waste" sheetId="6" r:id="rId1"/>
@@ -995,7 +995,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1061,12 +1061,6 @@
     <xf numFmtId="3" fontId="2" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1080,9 +1074,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="7" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1302,6 +1293,27 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1621,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11E648A-DDD9-4DEC-A8DC-7148C1AF4BEC}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1630,126 +1642,126 @@
     <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="38.25">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:4" ht="25.5">
+      <c r="A1" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="67" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="76">
+      <c r="B2" s="73">
         <v>165.41</v>
       </c>
-      <c r="C2" s="76">
+      <c r="C2" s="73">
         <v>149.13</v>
       </c>
-      <c r="D2" s="77">
+      <c r="D2" s="74">
         <v>0.9</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="76">
+      <c r="B3" s="73">
         <v>125.85</v>
       </c>
-      <c r="C3" s="76">
+      <c r="C3" s="73">
         <v>112.18</v>
       </c>
-      <c r="D3" s="77">
+      <c r="D3" s="74">
         <v>0.89</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="76">
+      <c r="B4" s="73">
         <v>153.4</v>
       </c>
-      <c r="C4" s="76">
+      <c r="C4" s="73">
         <v>137.69999999999999</v>
       </c>
-      <c r="D4" s="77">
+      <c r="D4" s="74">
         <v>0.9</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="76">
+      <c r="B5" s="73">
         <v>145.47999999999999</v>
       </c>
-      <c r="C5" s="76">
+      <c r="C5" s="73">
         <v>126.15</v>
       </c>
-      <c r="D5" s="77">
+      <c r="D5" s="74">
         <v>0.87</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="76">
+      <c r="B6" s="73">
         <v>170.45</v>
       </c>
-      <c r="C6" s="76">
+      <c r="C6" s="73">
         <v>152.08000000000001</v>
       </c>
-      <c r="D6" s="77">
+      <c r="D6" s="74">
         <v>0.89</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="81">
+      <c r="B7" s="78">
         <v>154.35</v>
       </c>
-      <c r="C7" s="82">
+      <c r="C7" s="79">
         <v>138.79</v>
       </c>
-      <c r="D7" s="77">
+      <c r="D7" s="74">
         <v>0.9</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="81">
+      <c r="B8" s="78">
         <v>164.28</v>
       </c>
-      <c r="C8" s="81">
+      <c r="C8" s="78">
         <v>147.88</v>
       </c>
-      <c r="D8" s="77">
+      <c r="D8" s="74">
         <v>0.9</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="85">
+      <c r="B9" s="82">
         <v>161.86000000000001</v>
       </c>
-      <c r="C9" s="85">
+      <c r="C9" s="82">
         <v>142.47999999999999</v>
       </c>
       <c r="D9" s="20">
@@ -1757,13 +1769,13 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="85">
+      <c r="B10" s="82">
         <v>147.34</v>
       </c>
-      <c r="C10" s="85">
+      <c r="C10" s="82">
         <v>131.63999999999999</v>
       </c>
       <c r="D10" s="20">
@@ -1771,42 +1783,42 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="85"/>
-      <c r="C11" s="85"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="91"/>
-      <c r="C12" s="91"/>
-      <c r="D12" s="90"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="87"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="75" t="s">
+      <c r="A13" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="91"/>
-      <c r="C13" s="91"/>
-      <c r="D13" s="90"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="87"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="97" t="s">
+      <c r="A14" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="98">
+      <c r="B14" s="95">
         <f>SUM(B2:B13)</f>
         <v>1388.4199999999998</v>
       </c>
-      <c r="C14" s="98">
+      <c r="C14" s="95">
         <f>SUM(C2:C13)</f>
         <v>1238.0299999999997</v>
       </c>
-      <c r="D14" s="99">
+      <c r="D14" s="96">
         <f>AVERAGE(D2:D13)</f>
         <v>0.8911111111111113</v>
       </c>
@@ -1820,8 +1832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7AF804-493F-4EDB-83A6-FDA04192F147}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1848,21 +1860,21 @@
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="109">
         <v>5476</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="109">
         <v>6150</v>
       </c>
       <c r="D2" s="17">
-        <f>(C2-B2)/B2</f>
+        <f t="shared" ref="D2:D14" si="0">(C2-B2)/B2</f>
         <v>0.12308254200146092</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="112">
         <v>8273</v>
       </c>
       <c r="F2" s="20">
-        <f>(E2-C2)/E2</f>
+        <f t="shared" ref="F2:F10" si="1">(E2-C2)/E2</f>
         <v>0.25661791369515291</v>
       </c>
     </row>
@@ -1870,21 +1882,21 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="109">
         <v>6035</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="109">
         <v>6071</v>
       </c>
       <c r="D3" s="17">
-        <f>(C3-B3)/B3</f>
+        <f t="shared" si="0"/>
         <v>5.9652029826014917E-3</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="112">
         <v>7349</v>
       </c>
       <c r="F3" s="20">
-        <f>(E3-C3)/E3</f>
+        <f t="shared" si="1"/>
         <v>0.17390121104912232</v>
       </c>
     </row>
@@ -1892,21 +1904,21 @@
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="109">
         <v>5333</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="109">
         <v>5579</v>
       </c>
       <c r="D4" s="17">
-        <f>(C4-B4)/B4</f>
+        <f t="shared" si="0"/>
         <v>4.6127882992687046E-2</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="112">
         <v>5620</v>
       </c>
       <c r="F4" s="20">
-        <f>(E4-C4)/E4</f>
+        <f t="shared" si="1"/>
         <v>7.2953736654804268E-3</v>
       </c>
     </row>
@@ -1914,21 +1926,21 @@
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="109">
         <v>7399</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="109">
         <v>5734</v>
       </c>
       <c r="D5" s="17">
-        <f>(C5-B5)/B5</f>
+        <f t="shared" si="0"/>
         <v>-0.2250304095147993</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="112">
         <v>8615</v>
       </c>
       <c r="F5" s="20">
-        <f>(E5-C5)/E5</f>
+        <f t="shared" si="1"/>
         <v>0.33441671503192105</v>
       </c>
     </row>
@@ -1936,21 +1948,21 @@
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="109">
         <v>6641</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="109">
         <v>6577</v>
       </c>
       <c r="D6" s="17">
-        <f>(C6-B6)/B6</f>
+        <f t="shared" si="0"/>
         <v>-9.6371028459569345E-3</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="113">
         <v>10387</v>
       </c>
       <c r="F6" s="20">
-        <f>(E6-C6)/E6</f>
+        <f t="shared" si="1"/>
         <v>0.36680465967074227</v>
       </c>
     </row>
@@ -1958,21 +1970,21 @@
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="109">
         <v>5986</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="109">
         <v>7009</v>
       </c>
       <c r="D7" s="17">
-        <f>(C7-B7)/B7</f>
+        <f t="shared" si="0"/>
         <v>0.17089876378215837</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="113">
         <v>8235</v>
       </c>
       <c r="F7" s="20">
-        <f>(E7-C7)/E7</f>
+        <f t="shared" si="1"/>
         <v>0.14887674559805708</v>
       </c>
     </row>
@@ -1980,21 +1992,21 @@
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="109">
         <v>6849</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="109">
         <v>6729</v>
       </c>
       <c r="D8" s="17">
-        <f>(C8-B8)/B8</f>
+        <f t="shared" si="0"/>
         <v>-1.7520805957074025E-2</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="112">
         <v>7634</v>
       </c>
       <c r="F8" s="20">
-        <f>(E8-C8)/E8</f>
+        <f t="shared" si="1"/>
         <v>0.11854859837568771</v>
       </c>
     </row>
@@ -2002,21 +2014,21 @@
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="109">
         <v>6278</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="109">
         <v>8567</v>
       </c>
       <c r="D9" s="17">
-        <f>(C9-B9)/B9</f>
+        <f t="shared" si="0"/>
         <v>0.36460656259955398</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="112">
         <v>8694</v>
       </c>
       <c r="F9" s="20">
-        <f>(E9-C9)/E9</f>
+        <f t="shared" si="1"/>
         <v>1.4607775477340695E-2</v>
       </c>
     </row>
@@ -2024,21 +2036,21 @@
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="109">
         <v>6368</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="109">
         <v>8328</v>
       </c>
       <c r="D10" s="17">
-        <f>(C10-B10)/B10</f>
+        <f t="shared" si="0"/>
         <v>0.30778894472361806</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="112">
         <v>8007</v>
       </c>
       <c r="F10" s="20">
-        <f>(E10-C10)/E10</f>
+        <f t="shared" si="1"/>
         <v>-4.0089921318846013E-2</v>
       </c>
     </row>
@@ -2046,104 +2058,104 @@
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="109">
         <v>5649</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="109">
         <v>8404</v>
       </c>
       <c r="D11" s="17">
-        <f>(C11-B11)/B11</f>
+        <f t="shared" si="0"/>
         <v>0.48769693751106391</v>
       </c>
-      <c r="E11" s="18"/>
+      <c r="E11" s="112"/>
       <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="109">
         <v>7325</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="109">
         <v>8556</v>
       </c>
       <c r="D12" s="17">
-        <f>(C12-B12)/B12</f>
+        <f t="shared" si="0"/>
         <v>0.16805460750853243</v>
       </c>
-      <c r="E12" s="18"/>
+      <c r="E12" s="112"/>
       <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="110">
         <v>11037</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="110">
         <v>8881</v>
       </c>
-      <c r="D13" s="27">
-        <f>(C13-B13)/B13</f>
+      <c r="D13" s="25">
+        <f t="shared" si="0"/>
         <v>-0.19534293739240735</v>
       </c>
-      <c r="E13" s="18"/>
+      <c r="E13" s="112"/>
       <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="34">
+      <c r="B14" s="111">
         <v>69339</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C14" s="111">
         <v>77704</v>
       </c>
-      <c r="D14" s="35">
-        <f>(C14-B14)/B14</f>
+      <c r="D14" s="32">
+        <f t="shared" si="0"/>
         <v>0.12063917852867795</v>
       </c>
-      <c r="E14" s="36">
+      <c r="E14" s="33">
         <f>SUM(E2:E13)</f>
         <v>72814</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F14" s="34">
         <f>AVERAGE(F2:F13)</f>
         <v>0.1534421190271843</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="60">
-      <c r="A15" s="42"/>
-      <c r="B15" s="42" t="s">
+      <c r="A15" s="39"/>
+      <c r="B15" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="49"/>
-      <c r="B16" s="50">
+      <c r="A16" s="46"/>
+      <c r="B16" s="47">
         <v>81734</v>
       </c>
-      <c r="C16" s="50">
+      <c r="C16" s="47">
         <v>77704</v>
       </c>
-      <c r="D16" s="51">
+      <c r="D16" s="48">
         <f>(C16-B16)/B16</f>
         <v>-4.9306286245626052E-2</v>
       </c>
-      <c r="E16" s="52"/>
-      <c r="F16" s="53"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2162,25 +2174,25 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7" ht="51">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="65" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2195,18 +2207,18 @@
         <v>224</v>
       </c>
       <c r="D2" s="20">
-        <f>(C2-B2)/B2</f>
+        <f t="shared" ref="D2:D14" si="0">(C2-B2)/B2</f>
         <v>-0.81594083812654072</v>
       </c>
       <c r="E2" s="18">
         <v>1493</v>
       </c>
       <c r="F2" s="20">
-        <f>(E2-C2)/C2</f>
+        <f t="shared" ref="F2:F7" si="1">(E2-C2)/C2</f>
         <v>5.6651785714285712</v>
       </c>
       <c r="G2" s="20">
-        <f>(E2-B2)/B2</f>
+        <f t="shared" ref="G2:G7" si="2">(E2-B2)/B2</f>
         <v>0.22678718159408381</v>
       </c>
     </row>
@@ -2221,18 +2233,18 @@
         <v>221</v>
       </c>
       <c r="D3" s="20">
-        <f>(C3-B3)/B3</f>
+        <f t="shared" si="0"/>
         <v>-0.85443767495471756</v>
       </c>
       <c r="E3" s="18">
         <v>1326</v>
       </c>
       <c r="F3" s="20">
-        <f>(E3-C3)/C3</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="G3" s="20">
-        <f>(E3-B3)/B3</f>
+        <f t="shared" si="2"/>
         <v>-0.12662604972830563</v>
       </c>
     </row>
@@ -2247,18 +2259,18 @@
         <v>203</v>
       </c>
       <c r="D4" s="20">
-        <f>(C4-B4)/B4</f>
+        <f t="shared" si="0"/>
         <v>-0.83131128469336879</v>
       </c>
       <c r="E4" s="18">
         <v>1014</v>
       </c>
       <c r="F4" s="20">
-        <f>(E4-C4)/C4</f>
+        <f t="shared" si="1"/>
         <v>3.9950738916256157</v>
       </c>
       <c r="G4" s="20">
-        <f>(E4-B4)/B4</f>
+        <f t="shared" si="2"/>
         <v>-0.15738740235998011</v>
       </c>
     </row>
@@ -2273,18 +2285,18 @@
         <v>1516</v>
       </c>
       <c r="D5" s="20">
-        <f>(C5-B5)/B5</f>
+        <f t="shared" si="0"/>
         <v>7.6704545454545456E-2</v>
       </c>
       <c r="E5" s="18">
         <v>2664</v>
       </c>
       <c r="F5" s="20">
-        <f>(E5-C5)/C5</f>
+        <f t="shared" si="1"/>
         <v>0.75725593667546176</v>
       </c>
       <c r="G5" s="20">
-        <f>(E5-B5)/B5</f>
+        <f t="shared" si="2"/>
         <v>0.89204545454545459</v>
       </c>
     </row>
@@ -2299,18 +2311,18 @@
         <v>1739</v>
       </c>
       <c r="D6" s="20">
-        <f>(C6-B6)/B6</f>
+        <f t="shared" si="0"/>
         <v>0.37579113924050633</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="23">
         <v>3212</v>
       </c>
       <c r="F6" s="20">
-        <f>(E6-C6)/C6</f>
+        <f t="shared" si="1"/>
         <v>0.84703852788959177</v>
       </c>
       <c r="G6" s="20">
-        <f>(E6-B6)/B6</f>
+        <f t="shared" si="2"/>
         <v>1.5411392405063291</v>
       </c>
     </row>
@@ -2325,18 +2337,18 @@
         <v>1853</v>
       </c>
       <c r="D7" s="20">
-        <f>(C7-B7)/B7</f>
+        <f t="shared" si="0"/>
         <v>0.62686567164179108</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="23">
         <v>2547</v>
       </c>
-      <c r="F7" s="80">
-        <f>(E7-C7)/C7</f>
+      <c r="F7" s="77">
+        <f t="shared" si="1"/>
         <v>0.37452779276848353</v>
       </c>
       <c r="G7" s="20">
-        <f>(E7-B7)/B7</f>
+        <f t="shared" si="2"/>
         <v>1.2361720807726075</v>
       </c>
     </row>
@@ -2351,11 +2363,11 @@
         <v>2137</v>
       </c>
       <c r="D8" s="20">
-        <f>(C8-B8)/B8</f>
+        <f t="shared" si="0"/>
         <v>-0.14383012820512819</v>
       </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="83"/>
+      <c r="F8" s="80"/>
       <c r="G8" s="20"/>
     </row>
     <row r="9" spans="1:7">
@@ -2369,11 +2381,11 @@
         <v>2842</v>
       </c>
       <c r="D9" s="20">
-        <f>(C9-B9)/B9</f>
+        <f t="shared" si="0"/>
         <v>0.23672758920800696</v>
       </c>
       <c r="E9" s="18"/>
-      <c r="F9" s="83"/>
+      <c r="F9" s="80"/>
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:7">
@@ -2387,12 +2399,12 @@
         <v>3066</v>
       </c>
       <c r="D10" s="20">
-        <f>(C10-B10)/B10</f>
+        <f t="shared" si="0"/>
         <v>0.35483870967741937</v>
       </c>
       <c r="E10" s="18"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="87"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="84"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
@@ -2405,12 +2417,12 @@
         <v>3142</v>
       </c>
       <c r="D11" s="20">
-        <f>(C11-B11)/B11</f>
+        <f t="shared" si="0"/>
         <v>0.3945849977807368</v>
       </c>
       <c r="E11" s="18"/>
-      <c r="F11" s="83"/>
-      <c r="G11" s="77"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="74"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
@@ -2423,89 +2435,89 @@
         <v>3341</v>
       </c>
       <c r="D12" s="20">
-        <f>(C12-B12)/B12</f>
+        <f t="shared" si="0"/>
         <v>0.1433949349760438</v>
       </c>
       <c r="E12" s="18"/>
-      <c r="F12" s="83"/>
-      <c r="G12" s="90"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="87"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="23">
         <v>4402</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="23">
         <v>3233</v>
       </c>
-      <c r="D13" s="93">
-        <f>(C13-B13)/B13</f>
+      <c r="D13" s="90">
+        <f t="shared" si="0"/>
         <v>-0.26556110858700593</v>
       </c>
       <c r="E13" s="18"/>
-      <c r="F13" s="94"/>
-      <c r="G13" s="90"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="87"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="95" t="s">
+      <c r="A14" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="36">
+      <c r="B14" s="33">
         <f>SUM(B2:B13)</f>
         <v>24383.65</v>
       </c>
-      <c r="C14" s="36">
+      <c r="C14" s="33">
         <f>SUM(C2:C13)</f>
         <v>23517</v>
       </c>
-      <c r="D14" s="37">
-        <f>(C14-B14)/B14</f>
+      <c r="D14" s="34">
+        <f t="shared" si="0"/>
         <v>-3.554225884968007E-2</v>
       </c>
-      <c r="E14" s="36">
+      <c r="E14" s="33">
         <f>SUM(E2:E13)</f>
         <v>12256</v>
       </c>
-      <c r="F14" s="96">
+      <c r="F14" s="93">
         <f>AVERAGE(F2:F13)</f>
         <v>2.7731791200646203</v>
       </c>
-      <c r="G14" s="96">
+      <c r="G14" s="93">
         <f>AVERAGE(G2:G13)</f>
         <v>0.60202175088836485</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="60">
-      <c r="A15" s="103"/>
-      <c r="B15" s="104" t="s">
+      <c r="A15" s="100"/>
+      <c r="B15" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="104" t="s">
+      <c r="C15" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="103"/>
-      <c r="F15" s="103"/>
+      <c r="E15" s="100"/>
+      <c r="F15" s="100"/>
       <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="103"/>
-      <c r="B16" s="108">
+      <c r="A16" s="100"/>
+      <c r="B16" s="105">
         <v>23383</v>
       </c>
-      <c r="C16" s="108">
+      <c r="C16" s="105">
         <v>23517</v>
       </c>
-      <c r="D16" s="109">
+      <c r="D16" s="106">
         <f>(C16-B16)/B16</f>
         <v>5.7306590257879654E-3</v>
       </c>
-      <c r="E16" s="103"/>
-      <c r="F16" s="103"/>
+      <c r="E16" s="100"/>
+      <c r="F16" s="100"/>
       <c r="G16" s="14"/>
     </row>
   </sheetData>
@@ -2531,7 +2543,7 @@
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="51">
+    <row r="1" spans="1:14" ht="38.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2804,10 +2816,10 @@
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="26">
         <v>380207</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="27">
         <v>415125</v>
       </c>
       <c r="D13" s="17">
@@ -2817,53 +2829,53 @@
       <c r="E13" s="18"/>
       <c r="F13" s="19"/>
       <c r="G13" s="6"/>
-      <c r="N13" s="31"/>
+      <c r="N13" s="28"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="34">
+      <c r="B14" s="31">
         <f>SUM(B2:B13)</f>
         <v>4290970.29</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C14" s="31">
         <f>SUM(C2:C13)</f>
         <v>4264736</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="32">
         <f t="shared" si="0"/>
         <v>-6.1138363183586703E-3</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="31">
         <f>SUM(E2:E13)</f>
         <v>2570130</v>
       </c>
-      <c r="F14" s="35">
+      <c r="F14" s="32">
         <f>AVERAGE(F2:F13)</f>
         <v>-6.4872217433595183E-2</v>
       </c>
       <c r="G14" s="6"/>
       <c r="N14" s="6"/>
     </row>
-    <row r="15" spans="1:14" ht="38.25">
-      <c r="A15" s="38"/>
+    <row r="15" spans="1:14" ht="25.5">
+      <c r="A15" s="35"/>
       <c r="B15" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="41"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="38"/>
       <c r="G15" s="6"/>
       <c r="N15" s="6"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="38"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="15">
         <v>4382326</v>
       </c>
@@ -2881,19 +2893,19 @@
       <c r="N16" s="6"/>
     </row>
     <row r="17" spans="1:25">
-      <c r="A17" s="55"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="60"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="56"/>
+      <c r="M17" s="57"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
@@ -2908,19 +2920,19 @@
       <c r="Y17" s="14"/>
     </row>
     <row r="18" spans="1:25">
-      <c r="A18" s="61"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
+      <c r="A18" s="58"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="63"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="56"/>
+      <c r="M18" s="60"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
@@ -2937,7 +2949,7 @@
     <row r="19" spans="1:25">
       <c r="G19" s="6"/>
       <c r="O19" s="6"/>
-      <c r="T19" s="44"/>
+      <c r="T19" s="41"/>
       <c r="U19" s="14"/>
       <c r="V19" s="14"/>
       <c r="W19" s="14"/>
@@ -2946,8 +2958,8 @@
     </row>
     <row r="20" spans="1:25">
       <c r="G20" s="6"/>
-      <c r="O20" s="74"/>
-      <c r="T20" s="78"/>
+      <c r="O20" s="71"/>
+      <c r="T20" s="75"/>
       <c r="U20" s="14"/>
       <c r="V20" s="14"/>
       <c r="W20" s="14"/>
@@ -2956,8 +2968,8 @@
     </row>
     <row r="21" spans="1:25">
       <c r="G21" s="6"/>
-      <c r="O21" s="74"/>
-      <c r="T21" s="78"/>
+      <c r="O21" s="71"/>
+      <c r="T21" s="75"/>
       <c r="U21" s="14"/>
       <c r="V21" s="14"/>
       <c r="W21" s="14"/>
@@ -2966,8 +2978,8 @@
     </row>
     <row r="22" spans="1:25">
       <c r="G22" s="6"/>
-      <c r="O22" s="74"/>
-      <c r="T22" s="78"/>
+      <c r="O22" s="71"/>
+      <c r="T22" s="75"/>
       <c r="U22" s="14"/>
       <c r="V22" s="14"/>
       <c r="W22" s="14"/>
@@ -2976,8 +2988,8 @@
     </row>
     <row r="23" spans="1:25">
       <c r="G23" s="6"/>
-      <c r="O23" s="74"/>
-      <c r="T23" s="78"/>
+      <c r="O23" s="71"/>
+      <c r="T23" s="75"/>
       <c r="U23" s="14"/>
       <c r="V23" s="14"/>
       <c r="W23" s="14"/>
@@ -2986,8 +2998,8 @@
     </row>
     <row r="24" spans="1:25">
       <c r="G24" s="6"/>
-      <c r="O24" s="74"/>
-      <c r="T24" s="78"/>
+      <c r="O24" s="71"/>
+      <c r="T24" s="75"/>
       <c r="U24" s="14"/>
       <c r="V24" s="14"/>
       <c r="W24" s="14"/>
@@ -2996,8 +3008,8 @@
     </row>
     <row r="25" spans="1:25">
       <c r="G25" s="6"/>
-      <c r="O25" s="74"/>
-      <c r="T25" s="78"/>
+      <c r="O25" s="71"/>
+      <c r="T25" s="75"/>
       <c r="U25" s="14"/>
       <c r="V25" s="14"/>
       <c r="W25" s="14"/>
@@ -3006,8 +3018,8 @@
     </row>
     <row r="26" spans="1:25">
       <c r="G26" s="6"/>
-      <c r="O26" s="74"/>
-      <c r="T26" s="84"/>
+      <c r="O26" s="71"/>
+      <c r="T26" s="81"/>
       <c r="U26" s="14"/>
       <c r="V26" s="14"/>
       <c r="W26" s="14"/>
@@ -3016,8 +3028,8 @@
     </row>
     <row r="27" spans="1:25">
       <c r="G27" s="6"/>
-      <c r="O27" s="74"/>
-      <c r="T27" s="86"/>
+      <c r="O27" s="71"/>
+      <c r="T27" s="83"/>
       <c r="U27" s="14"/>
       <c r="V27" s="14"/>
       <c r="W27" s="14"/>
@@ -3027,7 +3039,7 @@
     <row r="28" spans="1:25">
       <c r="G28" s="6"/>
       <c r="O28" s="6"/>
-      <c r="T28" s="44"/>
+      <c r="T28" s="41"/>
       <c r="U28" s="14"/>
       <c r="V28" s="14"/>
       <c r="W28" s="14"/>
@@ -3035,9 +3047,9 @@
       <c r="Y28" s="14"/>
     </row>
     <row r="29" spans="1:25">
-      <c r="G29" s="55"/>
+      <c r="G29" s="52"/>
       <c r="O29" s="6"/>
-      <c r="T29" s="88"/>
+      <c r="T29" s="85"/>
       <c r="U29" s="14"/>
       <c r="V29" s="14"/>
       <c r="W29" s="14"/>
@@ -3045,9 +3057,9 @@
       <c r="Y29" s="14"/>
     </row>
     <row r="30" spans="1:25">
-      <c r="G30" s="89"/>
+      <c r="G30" s="86"/>
       <c r="O30" s="14"/>
-      <c r="T30" s="92"/>
+      <c r="T30" s="89"/>
       <c r="U30" s="14"/>
       <c r="V30" s="14"/>
       <c r="W30" s="14"/>
@@ -3055,9 +3067,9 @@
       <c r="Y30" s="14"/>
     </row>
     <row r="31" spans="1:25">
-      <c r="G31" s="89"/>
+      <c r="G31" s="86"/>
       <c r="O31" s="14"/>
-      <c r="T31" s="92"/>
+      <c r="T31" s="89"/>
       <c r="U31" s="14"/>
       <c r="V31" s="14"/>
       <c r="W31" s="14"/>
@@ -3065,9 +3077,9 @@
       <c r="Y31" s="14"/>
     </row>
     <row r="32" spans="1:25">
-      <c r="G32" s="89"/>
+      <c r="G32" s="86"/>
       <c r="O32" s="14"/>
-      <c r="T32" s="92"/>
+      <c r="T32" s="89"/>
       <c r="U32" s="14"/>
       <c r="V32" s="14"/>
       <c r="W32" s="14"/>
@@ -3075,13 +3087,13 @@
       <c r="Y32" s="14"/>
     </row>
     <row r="33" spans="1:25">
-      <c r="A33" s="38"/>
-      <c r="B33" s="58"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="100"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="102"/>
-      <c r="G33" s="89"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="97"/>
+      <c r="E33" s="98"/>
+      <c r="F33" s="99"/>
+      <c r="G33" s="86"/>
       <c r="O33" s="14"/>
       <c r="P33" s="14"/>
       <c r="Q33" s="14"/>
@@ -3095,13 +3107,13 @@
       <c r="Y33" s="14"/>
     </row>
     <row r="34" spans="1:25">
-      <c r="A34" s="38"/>
-      <c r="B34" s="59"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="105"/>
-      <c r="E34" s="106"/>
-      <c r="F34" s="107"/>
-      <c r="G34" s="89"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="102"/>
+      <c r="E34" s="103"/>
+      <c r="F34" s="104"/>
+      <c r="G34" s="86"/>
       <c r="O34" s="14"/>
       <c r="P34" s="14"/>
       <c r="Q34" s="14"/>
@@ -3136,21 +3148,21 @@
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="51">
+    <row r="1" spans="1:6" ht="38.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="F1" s="62" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3158,21 +3170,21 @@
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="72">
+      <c r="B2" s="69">
         <v>166018</v>
       </c>
-      <c r="C2" s="72">
+      <c r="C2" s="69">
         <v>154290</v>
       </c>
-      <c r="D2" s="73">
-        <f>(C2-B2)/B2</f>
+      <c r="D2" s="70">
+        <f t="shared" ref="D2:D14" si="0">(C2-B2)/B2</f>
         <v>-7.0642942331554409E-2</v>
       </c>
       <c r="E2" s="18">
         <v>137349</v>
       </c>
       <c r="F2" s="19">
-        <f>(E2-C2)/C2</f>
+        <f t="shared" ref="F2:F9" si="1">(E2-C2)/C2</f>
         <v>-0.10979972778533929</v>
       </c>
     </row>
@@ -3180,21 +3192,21 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="79">
+      <c r="B3" s="76">
         <v>153234</v>
       </c>
-      <c r="C3" s="72">
+      <c r="C3" s="69">
         <v>139138</v>
       </c>
-      <c r="D3" s="73">
-        <f>(C3-B3)/B3</f>
+      <c r="D3" s="70">
+        <f t="shared" si="0"/>
         <v>-9.199002832269601E-2</v>
       </c>
       <c r="E3" s="18">
         <v>126757</v>
       </c>
       <c r="F3" s="19">
-        <f>(E3-C3)/C3</f>
+        <f t="shared" si="1"/>
         <v>-8.8983599016803458E-2</v>
       </c>
     </row>
@@ -3202,21 +3214,21 @@
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="72">
+      <c r="B4" s="69">
         <v>149129</v>
       </c>
-      <c r="C4" s="72">
+      <c r="C4" s="69">
         <v>139609</v>
       </c>
-      <c r="D4" s="73">
-        <f>(C4-B4)/B4</f>
+      <c r="D4" s="70">
+        <f t="shared" si="0"/>
         <v>-6.3837348872452709E-2</v>
       </c>
       <c r="E4" s="18">
         <v>117550</v>
       </c>
       <c r="F4" s="19">
-        <f>(E4-C4)/C4</f>
+        <f t="shared" si="1"/>
         <v>-0.15800557270663065</v>
       </c>
     </row>
@@ -3224,21 +3236,21 @@
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="72">
+      <c r="B5" s="69">
         <v>146506</v>
       </c>
-      <c r="C5" s="72">
+      <c r="C5" s="69">
         <v>126227</v>
       </c>
-      <c r="D5" s="73">
-        <f>(C5-B5)/B5</f>
+      <c r="D5" s="70">
+        <f t="shared" si="0"/>
         <v>-0.13841753921341104</v>
       </c>
       <c r="E5" s="18">
         <v>113477</v>
       </c>
       <c r="F5" s="19">
-        <f>(E5-C5)/C5</f>
+        <f t="shared" si="1"/>
         <v>-0.10100850055851759</v>
       </c>
     </row>
@@ -3246,21 +3258,21 @@
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="72">
+      <c r="B6" s="69">
         <v>122937</v>
       </c>
-      <c r="C6" s="72">
+      <c r="C6" s="69">
         <v>128749</v>
       </c>
-      <c r="D6" s="73">
-        <f>(C6-B6)/B6</f>
+      <c r="D6" s="70">
+        <f t="shared" si="0"/>
         <v>4.7276247183516758E-2</v>
       </c>
       <c r="E6" s="18">
         <v>108336</v>
       </c>
       <c r="F6" s="19">
-        <f>(E6-C6)/C6</f>
+        <f t="shared" si="1"/>
         <v>-0.15854880426255738</v>
       </c>
     </row>
@@ -3268,21 +3280,21 @@
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="72">
+      <c r="B7" s="69">
         <v>113710</v>
       </c>
-      <c r="C7" s="72">
+      <c r="C7" s="69">
         <v>125671</v>
       </c>
-      <c r="D7" s="73">
-        <f>(C7-B7)/B7</f>
+      <c r="D7" s="70">
+        <f t="shared" si="0"/>
         <v>0.10518863776272976</v>
       </c>
       <c r="E7" s="18">
         <v>98523</v>
       </c>
       <c r="F7" s="19">
-        <f>(E7-C7)/C7</f>
+        <f t="shared" si="1"/>
         <v>-0.21602438112213637</v>
       </c>
     </row>
@@ -3290,21 +3302,21 @@
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="72">
+      <c r="B8" s="69">
         <v>117122</v>
       </c>
-      <c r="C8" s="72">
+      <c r="C8" s="69">
         <v>147302</v>
       </c>
-      <c r="D8" s="73">
-        <f>(C8-B8)/B8</f>
+      <c r="D8" s="70">
+        <f t="shared" si="0"/>
         <v>0.25768002595584094</v>
       </c>
       <c r="E8" s="18">
         <v>103029</v>
       </c>
       <c r="F8" s="19">
-        <f>(E8-C8)/C8</f>
+        <f t="shared" si="1"/>
         <v>-0.30055939498445372</v>
       </c>
     </row>
@@ -3312,21 +3324,21 @@
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="72">
+      <c r="B9" s="69">
         <v>126623</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="69">
         <v>145461</v>
       </c>
-      <c r="D9" s="73">
-        <f>(C9-B9)/B9</f>
+      <c r="D9" s="70">
+        <f t="shared" si="0"/>
         <v>0.14877233993824188</v>
       </c>
       <c r="E9" s="18">
         <v>115694</v>
       </c>
       <c r="F9" s="19">
-        <f>(E9-C9)/C9</f>
+        <f t="shared" si="1"/>
         <v>-0.20463904414241618</v>
       </c>
     </row>
@@ -3334,14 +3346,14 @@
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="72">
+      <c r="B10" s="69">
         <v>122360</v>
       </c>
-      <c r="C10" s="72">
+      <c r="C10" s="69">
         <v>149470</v>
       </c>
-      <c r="D10" s="73">
-        <f>(C10-B10)/B10</f>
+      <c r="D10" s="70">
+        <f t="shared" si="0"/>
         <v>0.22155933311539719</v>
       </c>
       <c r="E10" s="18"/>
@@ -3351,14 +3363,14 @@
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="72">
+      <c r="B11" s="69">
         <v>132280</v>
       </c>
-      <c r="C11" s="72">
+      <c r="C11" s="69">
         <v>165507</v>
       </c>
-      <c r="D11" s="73">
-        <f>(C11-B11)/B11</f>
+      <c r="D11" s="70">
+        <f t="shared" si="0"/>
         <v>0.25118687632295134</v>
       </c>
       <c r="E11" s="18"/>
@@ -3368,14 +3380,14 @@
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="72">
+      <c r="B12" s="69">
         <v>128303</v>
       </c>
-      <c r="C12" s="72">
+      <c r="C12" s="69">
         <v>162736</v>
       </c>
-      <c r="D12" s="73">
-        <f>(C12-B12)/B12</f>
+      <c r="D12" s="70">
+        <f t="shared" si="0"/>
         <v>0.2683725244148617</v>
       </c>
       <c r="E12" s="18"/>
@@ -3385,40 +3397,40 @@
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="72">
+      <c r="B13" s="69">
         <v>132120</v>
       </c>
-      <c r="C13" s="72">
+      <c r="C13" s="69">
         <v>165619</v>
       </c>
-      <c r="D13" s="73">
-        <f>(C13-B13)/B13</f>
+      <c r="D13" s="70">
+        <f t="shared" si="0"/>
         <v>0.25354980320920373</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="19"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="34">
+      <c r="B14" s="31">
         <f>SUM(B2:B13)</f>
         <v>1610342</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C14" s="31">
         <f>SUM(C2:C13)</f>
         <v>1749779</v>
       </c>
-      <c r="D14" s="35">
-        <f>(C14-B14)/B14</f>
+      <c r="D14" s="32">
+        <f t="shared" si="0"/>
         <v>8.6588438977558801E-2</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="31">
         <f>SUM(E2:E13)</f>
         <v>920715</v>
       </c>
-      <c r="F14" s="35">
+      <c r="F14" s="32">
         <f>AVERAGE(F2:F13)</f>
         <v>-0.16719612807235684</v>
       </c>
@@ -3445,7 +3457,7 @@
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="51">
+    <row r="1" spans="1:11" ht="38.25">
       <c r="A1" s="1"/>
       <c r="B1" s="11" t="s">
         <v>8</v>
@@ -3479,14 +3491,14 @@
         <v>40365</v>
       </c>
       <c r="D2" s="17">
-        <f>(C2-B2)/B2</f>
+        <f t="shared" ref="D2:D14" si="0">(C2-B2)/B2</f>
         <v>0.67282293688279304</v>
       </c>
       <c r="E2" s="18">
         <v>41888</v>
       </c>
       <c r="F2" s="20">
-        <f>(E2-C2)/C2</f>
+        <f t="shared" ref="F2:F9" si="1">(E2-C2)/C2</f>
         <v>3.773070729592469E-2</v>
       </c>
       <c r="G2" s="14"/>
@@ -3506,23 +3518,23 @@
         <v>37545</v>
       </c>
       <c r="D3" s="17">
-        <f>(C3-B3)/B3</f>
+        <f t="shared" si="0"/>
         <v>-0.21967033487771195</v>
       </c>
       <c r="E3" s="22">
         <v>42788</v>
       </c>
       <c r="F3" s="20">
-        <f>(E3-C3)/C3</f>
+        <f t="shared" si="1"/>
         <v>0.13964575842322546</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="108"/>
+      <c r="K3" s="108"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
@@ -3535,14 +3547,14 @@
         <v>25781.81</v>
       </c>
       <c r="D4" s="17">
-        <f>(C4-B4)/B4</f>
+        <f t="shared" si="0"/>
         <v>-7.3694825846982515E-6</v>
       </c>
       <c r="E4" s="22">
         <v>45023</v>
       </c>
       <c r="F4" s="20">
-        <f>(E4-C4)/C4</f>
+        <f t="shared" si="1"/>
         <v>0.74630873472421055</v>
       </c>
       <c r="G4" s="14"/>
@@ -3562,14 +3574,14 @@
         <v>25781.81</v>
       </c>
       <c r="D5" s="17">
-        <f>(C5-B5)/B5</f>
+        <f t="shared" si="0"/>
         <v>-0.27485976356125169</v>
       </c>
       <c r="E5" s="22">
         <v>25839</v>
       </c>
       <c r="F5" s="20">
-        <f>(E5-C5)/C5</f>
+        <f t="shared" si="1"/>
         <v>2.2182306052212272E-3</v>
       </c>
       <c r="G5" s="14"/>
@@ -3589,14 +3601,14 @@
         <v>13432.28</v>
       </c>
       <c r="D6" s="17">
-        <f>(C6-B6)/B6</f>
+        <f t="shared" si="0"/>
         <v>-0.14596388606307217</v>
       </c>
       <c r="E6" s="22">
         <v>12769</v>
       </c>
       <c r="F6" s="20">
-        <f>(E6-C6)/C6</f>
+        <f t="shared" si="1"/>
         <v>-4.9379554327336879E-2</v>
       </c>
       <c r="G6" s="14"/>
@@ -3616,14 +3628,14 @@
         <v>15430.56</v>
       </c>
       <c r="D7" s="17">
-        <f>(C7-B7)/B7</f>
+        <f t="shared" si="0"/>
         <v>2.3020281751619143E-3</v>
       </c>
       <c r="E7" s="22">
         <v>10444</v>
       </c>
       <c r="F7" s="20">
-        <f>(E7-C7)/C7</f>
+        <f t="shared" si="1"/>
         <v>-0.32316131106064844</v>
       </c>
       <c r="G7" s="14"/>
@@ -3643,14 +3655,14 @@
         <v>7210.53</v>
       </c>
       <c r="D8" s="17">
-        <f>(C8-B8)/B8</f>
+        <f t="shared" si="0"/>
         <v>-0.20482736869036638</v>
       </c>
       <c r="E8" s="18">
         <v>8021</v>
       </c>
       <c r="F8" s="20">
-        <f>(E8-C8)/C8</f>
+        <f t="shared" si="1"/>
         <v>0.11240089147399709</v>
       </c>
       <c r="G8" s="14"/>
@@ -3670,14 +3682,14 @@
         <v>7045.99</v>
       </c>
       <c r="D9" s="17">
-        <f>(C9-B9)/B9</f>
+        <f t="shared" si="0"/>
         <v>-0.41720512820512823</v>
       </c>
       <c r="E9" s="18">
         <v>11379</v>
       </c>
       <c r="F9" s="20">
-        <f>(E9-C9)/C9</f>
+        <f t="shared" si="1"/>
         <v>0.61496113392156393</v>
       </c>
       <c r="G9" s="14"/>
@@ -3687,17 +3699,17 @@
       <c r="K9" s="14"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="23">
         <v>15191</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="23">
         <v>23032</v>
       </c>
-      <c r="D10" s="27">
-        <f>(C10-B10)/B10</f>
+      <c r="D10" s="25">
+        <f t="shared" si="0"/>
         <v>0.51616088473438215</v>
       </c>
       <c r="E10" s="18"/>
@@ -3709,17 +3721,17 @@
       <c r="K10" s="14"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="23">
         <v>17892</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="23">
         <v>36770</v>
       </c>
-      <c r="D11" s="27">
-        <f>(C11-B11)/B11</f>
+      <c r="D11" s="25">
+        <f t="shared" si="0"/>
         <v>1.0551084283478649</v>
       </c>
       <c r="E11" s="18"/>
@@ -3731,17 +3743,17 @@
       <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="23">
         <v>41103</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="23">
         <v>40381</v>
       </c>
-      <c r="D12" s="27">
-        <f>(C12-B12)/B12</f>
+      <c r="D12" s="25">
+        <f t="shared" si="0"/>
         <v>-1.7565627813055009E-2</v>
       </c>
       <c r="E12" s="18"/>
@@ -3756,14 +3768,14 @@
       <c r="A13" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="26">
         <v>31826.36</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="29">
         <v>34355</v>
       </c>
       <c r="D13" s="17">
-        <f>(C13-B13)/B13</f>
+        <f t="shared" si="0"/>
         <v>7.9451121648847031E-2</v>
       </c>
       <c r="E13" s="18"/>
@@ -3775,26 +3787,26 @@
       <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="34">
+      <c r="B14" s="31">
         <f>SUM(B2:B13)</f>
         <v>291873.75</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C14" s="31">
         <f>SUM(C2:C13)</f>
         <v>307130.98</v>
       </c>
-      <c r="D14" s="35">
-        <f>(C14-B14)/B14</f>
+      <c r="D14" s="32">
+        <f t="shared" si="0"/>
         <v>5.2273388751129489E-2</v>
       </c>
-      <c r="E14" s="36">
+      <c r="E14" s="33">
         <f>SUM(E2:E13)</f>
         <v>198151</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F14" s="34">
         <f>AVERAGE(F2:F13)</f>
         <v>0.16009057388201969</v>
       </c>
@@ -3804,19 +3816,19 @@
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:11" ht="38.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45" t="s">
+    <row r="15" spans="1:11" ht="25.5">
+      <c r="A15" s="41"/>
+      <c r="B15" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="D15" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="47"/>
-      <c r="F15" s="48"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="45"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -3824,19 +3836,19 @@
       <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="44"/>
-      <c r="B16" s="54">
+      <c r="A16" s="41"/>
+      <c r="B16" s="51">
         <v>331445.11</v>
       </c>
-      <c r="C16" s="54">
+      <c r="C16" s="51">
         <v>272775.98</v>
       </c>
       <c r="D16" s="20">
         <f>(C16-B16)/C16</f>
         <v>-0.2150817311700246</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="48"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="45"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>

</xml_diff>

<commit_message>
added pulling water from excel
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hb16606\OneDrive - University of Bristol\Documents\SPE\Green-Credentials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janhe\SPE\Green-Credentials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{EFBF31D5-3A61-4285-ACCC-A949CF96641E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{40418A72-4656-4CA8-AD08-CE8562C8082B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D994D5-F568-4C43-97DE-FE4145BC6807}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1" xr2:uid="{0C7B78C3-690B-478C-8020-AF23CEA86F9E}"/>
+    <workbookView xWindow="-11184" yWindow="2388" windowWidth="17328" windowHeight="9462" firstSheet="1" activeTab="5" xr2:uid="{0C7B78C3-690B-478C-8020-AF23CEA86F9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Waste" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <author>HEAVEN, Beth</author>
   </authors>
   <commentList>
-    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{D79F2548-EA04-49ED-8076-0A96154B2C54}">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{D79F2548-EA04-49ED-8076-0A96154B2C54}">
       <text>
         <r>
           <rPr>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{227B656D-9F89-4FD1-BCD5-3FC6F1AC3235}">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{227B656D-9F89-4FD1-BCD5-3FC6F1AC3235}">
       <text>
         <r>
           <rPr>
@@ -89,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{88A1BF4D-6C55-4D8C-9D70-55676554A30D}">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{88A1BF4D-6C55-4D8C-9D70-55676554A30D}">
       <text>
         <r>
           <rPr>
@@ -113,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{E6162AF4-AF00-419C-99CF-427F81597654}">
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{E6162AF4-AF00-419C-99CF-427F81597654}">
       <text>
         <r>
           <rPr>
@@ -137,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{5EB881B7-1BFE-4854-87AA-BE35FBE94D3B}">
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{5EB881B7-1BFE-4854-87AA-BE35FBE94D3B}">
       <text>
         <r>
           <rPr>
@@ -161,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{C15B1364-3085-4DA6-B888-9C68FF64D757}">
+    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{C15B1364-3085-4DA6-B888-9C68FF64D757}">
       <text>
         <r>
           <rPr>
@@ -349,7 +349,7 @@
     <author>HEAVEN, Beth</author>
   </authors>
   <commentList>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{DD55B405-E7CD-4A86-A2E0-2644AA8DE715}">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{DD55B405-E7CD-4A86-A2E0-2644AA8DE715}">
       <text>
         <r>
           <rPr>
@@ -373,7 +373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{215953B0-5C77-41E4-8C5E-62DD8096597D}">
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{215953B0-5C77-41E4-8C5E-62DD8096597D}">
       <text>
         <r>
           <rPr>
@@ -465,7 +465,7 @@
     <author>HEAVEN, Beth</author>
   </authors>
   <commentList>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{C238EF34-BAEC-4A74-BCF0-0DBD760F5F4D}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{C238EF34-BAEC-4A74-BCF0-0DBD760F5F4D}">
       <text>
         <r>
           <rPr>
@@ -489,7 +489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{D4AB3E5F-0F79-4D7A-B18C-1E7084A5DBCD}">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{D4AB3E5F-0F79-4D7A-B18C-1E7084A5DBCD}">
       <text>
         <r>
           <rPr>
@@ -513,7 +513,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{3B3B2EC9-3D9C-42CF-BCED-C2C7B0C0CF4E}">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{3B3B2EC9-3D9C-42CF-BCED-C2C7B0C0CF4E}">
       <text>
         <r>
           <rPr>
@@ -537,7 +537,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{89B4EEC3-A23F-40A8-AB11-09CFDEFF559B}">
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{89B4EEC3-A23F-40A8-AB11-09CFDEFF559B}">
       <text>
         <r>
           <rPr>
@@ -561,7 +561,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{F87BE9C1-248B-46AB-BF2A-281738FC0E7A}">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{F87BE9C1-248B-46AB-BF2A-281738FC0E7A}">
       <text>
         <r>
           <rPr>
@@ -995,19 +995,16 @@
       <alignment horizontal="right"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1015,38 +1012,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1055,33 +1046,27 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1097,22 +1082,19 @@
     <xf numFmtId="9" fontId="8" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1124,59 +1106,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1184,7 +1139,7 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1196,55 +1151,40 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="10" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="10" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="11" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1253,7 +1193,7 @@
     <xf numFmtId="9" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1267,52 +1207,37 @@
     </xf>
     <xf numFmtId="4" fontId="8" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="8" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1637,188 +1562,188 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:4" ht="24.6">
+      <c r="A1" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="52" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="73">
+      <c r="B2" s="57">
         <v>165.41</v>
       </c>
-      <c r="C2" s="73">
+      <c r="C2" s="57">
         <v>149.13</v>
       </c>
-      <c r="D2" s="74">
+      <c r="D2" s="17">
         <v>0.9</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="73">
+      <c r="B3" s="57">
         <v>125.85</v>
       </c>
-      <c r="C3" s="73">
+      <c r="C3" s="57">
         <v>112.18</v>
       </c>
-      <c r="D3" s="74">
+      <c r="D3" s="17">
         <v>0.89</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="73">
+      <c r="B4" s="57">
         <v>153.4</v>
       </c>
-      <c r="C4" s="73">
+      <c r="C4" s="57">
         <v>137.69999999999999</v>
       </c>
-      <c r="D4" s="74">
+      <c r="D4" s="17">
         <v>0.9</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="73">
+      <c r="B5" s="57">
         <v>145.47999999999999</v>
       </c>
-      <c r="C5" s="73">
+      <c r="C5" s="57">
         <v>126.15</v>
       </c>
-      <c r="D5" s="74">
+      <c r="D5" s="17">
         <v>0.87</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="73">
+      <c r="B6" s="57">
         <v>170.45</v>
       </c>
-      <c r="C6" s="73">
+      <c r="C6" s="57">
         <v>152.08000000000001</v>
       </c>
-      <c r="D6" s="74">
+      <c r="D6" s="17">
         <v>0.89</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="78">
+      <c r="B7" s="60">
         <v>154.35</v>
       </c>
-      <c r="C7" s="79">
+      <c r="C7" s="61">
         <v>138.79</v>
       </c>
-      <c r="D7" s="74">
+      <c r="D7" s="17">
         <v>0.9</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="78">
+      <c r="B8" s="60">
         <v>164.28</v>
       </c>
-      <c r="C8" s="78">
+      <c r="C8" s="60">
         <v>147.88</v>
       </c>
-      <c r="D8" s="74">
+      <c r="D8" s="17">
         <v>0.9</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="82">
+      <c r="B9" s="60">
         <v>161.86000000000001</v>
       </c>
-      <c r="C9" s="82">
+      <c r="C9" s="60">
         <v>142.47999999999999</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="17">
         <v>0.88</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="82">
+      <c r="B10" s="60">
         <v>147.34</v>
       </c>
-      <c r="C10" s="82">
+      <c r="C10" s="60">
         <v>131.63999999999999</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="17">
         <v>0.89</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="72" t="s">
+      <c r="A11" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="82"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="20"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="17"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="72" t="s">
+      <c r="A12" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="88"/>
-      <c r="D12" s="87"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="67"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="87"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="67"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="95">
+      <c r="B14" s="75">
         <f>SUM(B2:B13)</f>
         <v>1388.4199999999998</v>
       </c>
-      <c r="C14" s="95">
+      <c r="C14" s="75">
         <f>SUM(C2:C13)</f>
         <v>1238.0299999999997</v>
       </c>
-      <c r="D14" s="96">
+      <c r="D14" s="76">
         <f>AVERAGE(D2:D13)</f>
         <v>0.8911111111111113</v>
       </c>
@@ -1832,27 +1757,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7AF804-493F-4EDB-83A6-FDA04192F147}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="51">
+    <row r="1" spans="1:6" ht="49.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1860,21 +1785,21 @@
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="109">
+      <c r="B2" s="83">
         <v>5476</v>
       </c>
-      <c r="C2" s="109">
+      <c r="C2" s="83">
         <v>6150</v>
       </c>
-      <c r="D2" s="17">
-        <f t="shared" ref="D2:D14" si="0">(C2-B2)/B2</f>
+      <c r="D2" s="83">
+        <v>8273</v>
+      </c>
+      <c r="E2" s="16">
+        <f>(C2-B2)/B2</f>
         <v>0.12308254200146092</v>
       </c>
-      <c r="E2" s="112">
-        <v>8273</v>
-      </c>
-      <c r="F2" s="20">
-        <f t="shared" ref="F2:F10" si="1">(E2-C2)/E2</f>
+      <c r="F2" s="17">
+        <f>(D2-C2)/D2</f>
         <v>0.25661791369515291</v>
       </c>
     </row>
@@ -1882,21 +1807,21 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="109">
+      <c r="B3" s="83">
         <v>6035</v>
       </c>
-      <c r="C3" s="109">
+      <c r="C3" s="83">
         <v>6071</v>
       </c>
-      <c r="D3" s="17">
-        <f t="shared" si="0"/>
+      <c r="D3" s="83">
+        <v>7349</v>
+      </c>
+      <c r="E3" s="16">
+        <f>(C3-B3)/B3</f>
         <v>5.9652029826014917E-3</v>
       </c>
-      <c r="E3" s="112">
-        <v>7349</v>
-      </c>
-      <c r="F3" s="20">
-        <f t="shared" si="1"/>
+      <c r="F3" s="17">
+        <f>(D3-C3)/D3</f>
         <v>0.17390121104912232</v>
       </c>
     </row>
@@ -1904,21 +1829,21 @@
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="109">
+      <c r="B4" s="83">
         <v>5333</v>
       </c>
-      <c r="C4" s="109">
+      <c r="C4" s="83">
         <v>5579</v>
       </c>
-      <c r="D4" s="17">
-        <f t="shared" si="0"/>
+      <c r="D4" s="83">
+        <v>5620</v>
+      </c>
+      <c r="E4" s="16">
+        <f>(C4-B4)/B4</f>
         <v>4.6127882992687046E-2</v>
       </c>
-      <c r="E4" s="112">
-        <v>5620</v>
-      </c>
-      <c r="F4" s="20">
-        <f t="shared" si="1"/>
+      <c r="F4" s="17">
+        <f>(D4-C4)/D4</f>
         <v>7.2953736654804268E-3</v>
       </c>
     </row>
@@ -1926,21 +1851,21 @@
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="109">
+      <c r="B5" s="83">
         <v>7399</v>
       </c>
-      <c r="C5" s="109">
+      <c r="C5" s="83">
         <v>5734</v>
       </c>
-      <c r="D5" s="17">
-        <f t="shared" si="0"/>
+      <c r="D5" s="83">
+        <v>8615</v>
+      </c>
+      <c r="E5" s="16">
+        <f>(C5-B5)/B5</f>
         <v>-0.2250304095147993</v>
       </c>
-      <c r="E5" s="112">
-        <v>8615</v>
-      </c>
-      <c r="F5" s="20">
-        <f t="shared" si="1"/>
+      <c r="F5" s="17">
+        <f>(D5-C5)/D5</f>
         <v>0.33441671503192105</v>
       </c>
     </row>
@@ -1948,21 +1873,21 @@
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="109">
+      <c r="B6" s="83">
         <v>6641</v>
       </c>
-      <c r="C6" s="109">
+      <c r="C6" s="83">
         <v>6577</v>
       </c>
-      <c r="D6" s="17">
-        <f t="shared" si="0"/>
+      <c r="D6" s="86">
+        <v>10387</v>
+      </c>
+      <c r="E6" s="16">
+        <f>(C6-B6)/B6</f>
         <v>-9.6371028459569345E-3</v>
       </c>
-      <c r="E6" s="113">
-        <v>10387</v>
-      </c>
-      <c r="F6" s="20">
-        <f t="shared" si="1"/>
+      <c r="F6" s="17">
+        <f>(D6-C6)/D6</f>
         <v>0.36680465967074227</v>
       </c>
     </row>
@@ -1970,21 +1895,21 @@
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="109">
+      <c r="B7" s="83">
         <v>5986</v>
       </c>
-      <c r="C7" s="109">
+      <c r="C7" s="83">
         <v>7009</v>
       </c>
-      <c r="D7" s="17">
-        <f t="shared" si="0"/>
+      <c r="D7" s="86">
+        <v>8235</v>
+      </c>
+      <c r="E7" s="16">
+        <f>(C7-B7)/B7</f>
         <v>0.17089876378215837</v>
       </c>
-      <c r="E7" s="113">
-        <v>8235</v>
-      </c>
-      <c r="F7" s="20">
-        <f t="shared" si="1"/>
+      <c r="F7" s="17">
+        <f>(D7-C7)/D7</f>
         <v>0.14887674559805708</v>
       </c>
     </row>
@@ -1992,21 +1917,21 @@
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="109">
+      <c r="B8" s="83">
         <v>6849</v>
       </c>
-      <c r="C8" s="109">
+      <c r="C8" s="83">
         <v>6729</v>
       </c>
-      <c r="D8" s="17">
-        <f t="shared" si="0"/>
+      <c r="D8" s="83">
+        <v>7634</v>
+      </c>
+      <c r="E8" s="16">
+        <f>(C8-B8)/B8</f>
         <v>-1.7520805957074025E-2</v>
       </c>
-      <c r="E8" s="112">
-        <v>7634</v>
-      </c>
-      <c r="F8" s="20">
-        <f t="shared" si="1"/>
+      <c r="F8" s="17">
+        <f>(D8-C8)/D8</f>
         <v>0.11854859837568771</v>
       </c>
     </row>
@@ -2014,21 +1939,21 @@
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="109">
+      <c r="B9" s="83">
         <v>6278</v>
       </c>
-      <c r="C9" s="109">
+      <c r="C9" s="83">
         <v>8567</v>
       </c>
-      <c r="D9" s="17">
-        <f t="shared" si="0"/>
+      <c r="D9" s="83">
+        <v>8694</v>
+      </c>
+      <c r="E9" s="16">
+        <f>(C9-B9)/B9</f>
         <v>0.36460656259955398</v>
       </c>
-      <c r="E9" s="112">
-        <v>8694</v>
-      </c>
-      <c r="F9" s="20">
-        <f t="shared" si="1"/>
+      <c r="F9" s="17">
+        <f>(D9-C9)/D9</f>
         <v>1.4607775477340695E-2</v>
       </c>
     </row>
@@ -2036,21 +1961,21 @@
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="109">
+      <c r="B10" s="83">
         <v>6368</v>
       </c>
-      <c r="C10" s="109">
+      <c r="C10" s="83">
         <v>8328</v>
       </c>
-      <c r="D10" s="17">
-        <f t="shared" si="0"/>
+      <c r="D10" s="83">
+        <v>8007</v>
+      </c>
+      <c r="E10" s="16">
+        <f>(C10-B10)/B10</f>
         <v>0.30778894472361806</v>
       </c>
-      <c r="E10" s="112">
-        <v>8007</v>
-      </c>
-      <c r="F10" s="20">
-        <f t="shared" si="1"/>
+      <c r="F10" s="17">
+        <f>(D10-C10)/D10</f>
         <v>-4.0089921318846013E-2</v>
       </c>
     </row>
@@ -2058,104 +1983,104 @@
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="109">
+      <c r="B11" s="83">
         <v>5649</v>
       </c>
-      <c r="C11" s="109">
+      <c r="C11" s="83">
         <v>8404</v>
       </c>
-      <c r="D11" s="17">
-        <f t="shared" si="0"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="16">
+        <f>(C11-B11)/B11</f>
         <v>0.48769693751106391</v>
       </c>
-      <c r="E11" s="112"/>
-      <c r="F11" s="20"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="109">
+      <c r="B12" s="83">
         <v>7325</v>
       </c>
-      <c r="C12" s="109">
+      <c r="C12" s="83">
         <v>8556</v>
       </c>
-      <c r="D12" s="17">
-        <f t="shared" si="0"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="16">
+        <f>(C12-B12)/B12</f>
         <v>0.16805460750853243</v>
       </c>
-      <c r="E12" s="112"/>
-      <c r="F12" s="20"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="110">
+      <c r="B13" s="84">
         <v>11037</v>
       </c>
-      <c r="C13" s="110">
+      <c r="C13" s="84">
         <v>8881</v>
       </c>
-      <c r="D13" s="25">
-        <f t="shared" si="0"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="21">
+        <f>(C13-B13)/B13</f>
         <v>-0.19534293739240735</v>
       </c>
-      <c r="E13" s="112"/>
-      <c r="F13" s="20"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="111">
+      <c r="B14" s="85">
         <v>69339</v>
       </c>
-      <c r="C14" s="111">
+      <c r="C14" s="85">
         <v>77704</v>
       </c>
-      <c r="D14" s="32">
-        <f t="shared" si="0"/>
+      <c r="D14" s="28">
+        <f>SUM(D2:D13)</f>
+        <v>72814</v>
+      </c>
+      <c r="E14" s="27">
+        <f>(C14-B14)/B14</f>
         <v>0.12063917852867795</v>
       </c>
-      <c r="E14" s="33">
-        <f>SUM(E2:E13)</f>
-        <v>72814</v>
-      </c>
-      <c r="F14" s="34">
+      <c r="F14" s="29">
         <f>AVERAGE(F2:F13)</f>
         <v>0.1534421190271843</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="60">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39" t="s">
+    <row r="15" spans="1:6" ht="43.2">
+      <c r="A15" s="33"/>
+      <c r="B15" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="33"/>
+      <c r="E15" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
+      <c r="F15" s="33"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="46"/>
-      <c r="B16" s="47">
+      <c r="A16" s="34"/>
+      <c r="B16" s="39">
         <v>81734</v>
       </c>
-      <c r="C16" s="47">
+      <c r="C16" s="39">
         <v>77704</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="33"/>
+      <c r="E16" s="40">
         <f>(C16-B16)/B16</f>
         <v>-4.9306286245626052E-2</v>
       </c>
-      <c r="E16" s="49"/>
-      <c r="F16" s="50"/>
+      <c r="F16" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2168,31 +2093,31 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="51">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:7" ht="49.2">
+      <c r="A1" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="F1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="65" t="s">
+      <c r="G1" s="50" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2200,24 +2125,24 @@
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="18">
         <v>1217</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="18">
         <v>224</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="17">
         <f t="shared" ref="D2:D14" si="0">(C2-B2)/B2</f>
         <v>-0.81594083812654072</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="14">
         <v>1493</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="17">
         <f t="shared" ref="F2:F7" si="1">(E2-C2)/C2</f>
         <v>5.6651785714285712</v>
       </c>
-      <c r="G2" s="20">
+      <c r="G2" s="17">
         <f t="shared" ref="G2:G7" si="2">(E2-B2)/B2</f>
         <v>0.22678718159408381</v>
       </c>
@@ -2226,24 +2151,24 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="18">
         <v>1518.25</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="18">
         <v>221</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="17">
         <f t="shared" si="0"/>
         <v>-0.85443767495471756</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="14">
         <v>1326</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="17">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="17">
         <f t="shared" si="2"/>
         <v>-0.12662604972830563</v>
       </c>
@@ -2252,24 +2177,24 @@
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="18">
         <v>1203.4000000000001</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="18">
         <v>203</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="17">
         <f t="shared" si="0"/>
         <v>-0.83131128469336879</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="14">
         <v>1014</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="17">
         <f t="shared" si="1"/>
         <v>3.9950738916256157</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="17">
         <f t="shared" si="2"/>
         <v>-0.15738740235998011</v>
       </c>
@@ -2278,24 +2203,24 @@
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="14">
         <v>1408</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="14">
         <v>1516</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="17">
         <f t="shared" si="0"/>
         <v>7.6704545454545456E-2</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="14">
         <v>2664</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="17">
         <f t="shared" si="1"/>
         <v>0.75725593667546176</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="17">
         <f t="shared" si="2"/>
         <v>0.89204545454545459</v>
       </c>
@@ -2304,24 +2229,24 @@
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="14">
         <v>1264</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="14">
         <v>1739</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="17">
         <f t="shared" si="0"/>
         <v>0.37579113924050633</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="19">
         <v>3212</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="17">
         <f t="shared" si="1"/>
         <v>0.84703852788959177</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="17">
         <f t="shared" si="2"/>
         <v>1.5411392405063291</v>
       </c>
@@ -2330,24 +2255,24 @@
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="14">
         <v>1139</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="14">
         <v>1853</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="17">
         <f t="shared" si="0"/>
         <v>0.62686567164179108</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="19">
         <v>2547</v>
       </c>
-      <c r="F7" s="77">
+      <c r="F7" s="59">
         <f t="shared" si="1"/>
         <v>0.37452779276848353</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="17">
         <f t="shared" si="2"/>
         <v>1.2361720807726075</v>
       </c>
@@ -2356,169 +2281,169 @@
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="14">
         <v>2496</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="14">
         <v>2137</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="17">
         <f t="shared" si="0"/>
         <v>-0.14383012820512819</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="20"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="14">
         <v>2298</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="14">
         <v>2842</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="17">
         <f t="shared" si="0"/>
         <v>0.23672758920800696</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="20"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="17"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="14">
         <v>2263</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="14">
         <v>3066</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="17">
         <f t="shared" si="0"/>
         <v>0.35483870967741937</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="84"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="65"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="14">
         <v>2253</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="14">
         <v>3142</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="17">
         <f t="shared" si="0"/>
         <v>0.3945849977807368</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="74"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="17"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="14">
         <v>2922</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="14">
         <v>3341</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="17">
         <f t="shared" si="0"/>
         <v>0.1433949349760438</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="87"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="67"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="19">
         <v>4402</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="19">
         <v>3233</v>
       </c>
-      <c r="D13" s="90">
+      <c r="D13" s="70">
         <f t="shared" si="0"/>
         <v>-0.26556110858700593</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="91"/>
-      <c r="G13" s="87"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="92" t="s">
+      <c r="A14" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="28">
         <f>SUM(B2:B13)</f>
         <v>24383.65</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="28">
         <f>SUM(C2:C13)</f>
         <v>23517</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="29">
         <f t="shared" si="0"/>
         <v>-3.554225884968007E-2</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="28">
         <f>SUM(E2:E13)</f>
         <v>12256</v>
       </c>
-      <c r="F14" s="93">
+      <c r="F14" s="73">
         <f>AVERAGE(F2:F13)</f>
         <v>2.7731791200646203</v>
       </c>
-      <c r="G14" s="93">
+      <c r="G14" s="73">
         <f>AVERAGE(G2:G13)</f>
         <v>0.60202175088836485</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="60">
-      <c r="A15" s="100"/>
-      <c r="B15" s="101" t="s">
+    <row r="15" spans="1:7" ht="43.2">
+      <c r="A15" s="79"/>
+      <c r="B15" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="101" t="s">
+      <c r="C15" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="100"/>
-      <c r="F15" s="100"/>
-      <c r="G15" s="14"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="100"/>
-      <c r="B16" s="105">
+      <c r="A16" s="79"/>
+      <c r="B16" s="81">
         <v>23383</v>
       </c>
-      <c r="C16" s="105">
+      <c r="C16" s="81">
         <v>23517</v>
       </c>
-      <c r="D16" s="106">
+      <c r="D16" s="82">
         <f>(C16-B16)/B16</f>
         <v>5.7306590257879654E-3</v>
       </c>
-      <c r="E16" s="100"/>
-      <c r="F16" s="100"/>
-      <c r="G16" s="14"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2531,19 +2456,19 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.41796875" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="38.25">
+    <row r="1" spans="1:14" ht="49.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2552,579 +2477,579 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="G1" s="5"/>
+      <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="14">
         <v>394931</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="15">
         <v>381400</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="14">
+        <v>358709</v>
+      </c>
+      <c r="E2" s="16">
         <f>(C2-B2)/B2</f>
         <v>-3.4261681154429506E-2</v>
       </c>
-      <c r="E2" s="18">
-        <v>358709</v>
-      </c>
-      <c r="F2" s="19">
-        <f>(E2-C2)/C2</f>
+      <c r="F2" s="16">
+        <f>(D2-C2)/C2</f>
         <v>-5.9493969585736758E-2</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="N2" s="6"/>
+      <c r="G2" s="5"/>
+      <c r="N2" s="5"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="1">
         <v>367833</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="15">
         <v>338378</v>
       </c>
-      <c r="D3" s="17">
-        <f t="shared" ref="D3:D14" si="0">(C3-B3)/B3</f>
+      <c r="D3" s="14">
+        <v>320011</v>
+      </c>
+      <c r="E3" s="16">
+        <f>(C3-B3)/B3</f>
         <v>-8.0077100205799917E-2</v>
       </c>
-      <c r="E3" s="18">
-        <v>320011</v>
-      </c>
-      <c r="F3" s="19">
-        <f t="shared" ref="F3:F9" si="1">(E3-C3)/C3</f>
+      <c r="F3" s="16">
+        <f>(D3-C3)/C3</f>
         <v>-5.4279533539414504E-2</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="N3" s="6"/>
+      <c r="G3" s="5"/>
+      <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <v>371467</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <v>354957</v>
       </c>
-      <c r="D4" s="17">
-        <f t="shared" si="0"/>
+      <c r="D4" s="14">
+        <v>323736</v>
+      </c>
+      <c r="E4" s="16">
+        <f>(C4-B4)/B4</f>
         <v>-4.4445401610371853E-2</v>
       </c>
-      <c r="E4" s="18">
-        <v>323736</v>
-      </c>
-      <c r="F4" s="19">
-        <f t="shared" si="1"/>
+      <c r="F4" s="16">
+        <f>(D4-C4)/C4</f>
         <v>-8.7957132835808277E-2</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="N4" s="6"/>
+      <c r="G4" s="5"/>
+      <c r="N4" s="5"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>368871</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <v>329975</v>
       </c>
-      <c r="D5" s="17">
-        <f t="shared" si="0"/>
+      <c r="D5" s="14">
+        <v>307995</v>
+      </c>
+      <c r="E5" s="16">
+        <f>(C5-B5)/B5</f>
         <v>-0.10544607735495606</v>
       </c>
-      <c r="E5" s="18">
-        <v>307995</v>
-      </c>
-      <c r="F5" s="19">
-        <f t="shared" si="1"/>
+      <c r="F5" s="16">
+        <f>(D5-C5)/C5</f>
         <v>-6.6611106902038031E-2</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="N5" s="6"/>
+      <c r="G5" s="5"/>
+      <c r="N5" s="5"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>334319</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="15">
         <v>333225</v>
       </c>
-      <c r="D6" s="17">
-        <f t="shared" si="0"/>
+      <c r="D6" s="14">
+        <v>305855</v>
+      </c>
+      <c r="E6" s="16">
+        <f>(C6-B6)/B6</f>
         <v>-3.2723237387046506E-3</v>
       </c>
-      <c r="E6" s="18">
-        <v>305855</v>
-      </c>
-      <c r="F6" s="19">
-        <f t="shared" si="1"/>
+      <c r="F6" s="16">
+        <f>(D6-C6)/C6</f>
         <v>-8.2136694425688342E-2</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="N6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>324600</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="15">
         <v>319566</v>
       </c>
-      <c r="D7" s="17">
-        <f t="shared" si="0"/>
+      <c r="D7" s="14">
+        <v>289224</v>
+      </c>
+      <c r="E7" s="16">
+        <f>(C7-B7)/B7</f>
         <v>-1.5508317929759704E-2</v>
       </c>
-      <c r="E7" s="18">
-        <v>289224</v>
-      </c>
-      <c r="F7" s="19">
-        <f t="shared" si="1"/>
+      <c r="F7" s="16">
+        <f>(D7-C7)/C7</f>
         <v>-9.4947522577495724E-2</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="G7" s="5"/>
+      <c r="N7" s="5"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>333724</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="15">
         <v>345523</v>
       </c>
-      <c r="D8" s="17">
-        <f t="shared" si="0"/>
+      <c r="D8" s="14">
+        <v>327266</v>
+      </c>
+      <c r="E8" s="16">
+        <f>(C8-B8)/B8</f>
         <v>3.5355563279836029E-2</v>
       </c>
-      <c r="E8" s="18">
-        <v>327266</v>
-      </c>
-      <c r="F8" s="19">
-        <f t="shared" si="1"/>
+      <c r="F8" s="16">
+        <f>(D8-C8)/C8</f>
         <v>-5.2838740112814489E-2</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="N8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="N8" s="5"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>348860</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="15">
         <v>344469</v>
       </c>
-      <c r="D9" s="17">
-        <f t="shared" si="0"/>
+      <c r="D9" s="14">
+        <v>337334</v>
+      </c>
+      <c r="E9" s="16">
+        <f>(C9-B9)/B9</f>
         <v>-1.2586711001547899E-2</v>
       </c>
-      <c r="E9" s="18">
-        <v>337334</v>
-      </c>
-      <c r="F9" s="19">
-        <f t="shared" si="1"/>
+      <c r="F9" s="16">
+        <f>(D9-C9)/C9</f>
         <v>-2.0713039489765408E-2</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="N9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="N9" s="5"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <v>341996</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <v>342330</v>
       </c>
-      <c r="D10" s="17">
-        <f t="shared" si="0"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="16">
+        <f>(C10-B10)/B10</f>
         <v>9.7661960958607711E-4</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="6"/>
-      <c r="N10" s="6"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="5"/>
+      <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>354358.2</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <v>367756</v>
       </c>
-      <c r="D11" s="17">
-        <f t="shared" si="0"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="16">
+        <f>(C11-B11)/B11</f>
         <v>3.7808635442893625E-2</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="6"/>
-      <c r="N11" s="6"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="5"/>
+      <c r="N11" s="5"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>369804.09</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>392032</v>
       </c>
-      <c r="D12" s="17">
-        <f t="shared" si="0"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="16">
+        <f>(C12-B12)/B12</f>
         <v>6.0107258413502063E-2</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="6"/>
-      <c r="N12" s="6"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="5"/>
+      <c r="N12" s="5"/>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="22">
         <v>380207</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="23">
         <v>415125</v>
       </c>
-      <c r="D13" s="17">
-        <f t="shared" si="0"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="16">
+        <f>(C13-B13)/B13</f>
         <v>9.1839445354767277E-2</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="6"/>
-      <c r="N13" s="28"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="5"/>
+      <c r="N13" s="24"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="26">
         <f>SUM(B2:B13)</f>
         <v>4290970.29</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="26">
         <f>SUM(C2:C13)</f>
         <v>4264736</v>
       </c>
-      <c r="D14" s="32">
-        <f t="shared" si="0"/>
+      <c r="D14" s="26">
+        <f>SUM(D2:D13)</f>
+        <v>2570130</v>
+      </c>
+      <c r="E14" s="27">
+        <f>(C14-B14)/B14</f>
         <v>-6.1138363183586703E-3</v>
       </c>
-      <c r="E14" s="31">
-        <f>SUM(E2:E13)</f>
-        <v>2570130</v>
-      </c>
-      <c r="F14" s="32">
+      <c r="F14" s="27">
         <f>AVERAGE(F2:F13)</f>
         <v>-6.4872217433595183E-2</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="N14" s="6"/>
-    </row>
-    <row r="15" spans="1:14" ht="25.5">
-      <c r="A15" s="35"/>
-      <c r="B15" s="21" t="s">
+      <c r="G14" s="5"/>
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="1:14" ht="36.9">
+      <c r="A15" s="30"/>
+      <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="32"/>
+      <c r="E15" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="6"/>
-      <c r="N15" s="6"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="5"/>
+      <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="35"/>
-      <c r="B16" s="15">
+      <c r="A16" s="30"/>
+      <c r="B16" s="14">
         <v>4382326</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="14">
         <f>C14</f>
         <v>4264736</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="14"/>
+      <c r="E16" s="16">
         <f>(C16-B16)/C16</f>
         <v>-2.7572632866372033E-2</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="6"/>
-      <c r="N16" s="6"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="5"/>
+      <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:25">
-      <c r="A17" s="52"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="56"/>
-      <c r="M17" s="57"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
-      <c r="U17" s="14"/>
-      <c r="V17" s="14"/>
-      <c r="W17" s="14"/>
-      <c r="X17" s="14"/>
-      <c r="Y17" s="14"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
     </row>
     <row r="18" spans="1:25">
-      <c r="A18" s="58"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
-      <c r="W18" s="14"/>
-      <c r="X18" s="14"/>
-      <c r="Y18" s="14"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="13"/>
+      <c r="Y18" s="13"/>
     </row>
     <row r="19" spans="1:25">
-      <c r="G19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="T19" s="41"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-      <c r="W19" s="14"/>
-      <c r="X19" s="14"/>
-      <c r="Y19" s="14"/>
+      <c r="G19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="T19" s="35"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
     </row>
     <row r="20" spans="1:25">
-      <c r="G20" s="6"/>
-      <c r="O20" s="71"/>
-      <c r="T20" s="75"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="14"/>
-      <c r="W20" s="14"/>
-      <c r="X20" s="14"/>
-      <c r="Y20" s="14"/>
+      <c r="G20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="T20" s="35"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
     </row>
     <row r="21" spans="1:25">
-      <c r="G21" s="6"/>
-      <c r="O21" s="71"/>
-      <c r="T21" s="75"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="14"/>
-      <c r="W21" s="14"/>
-      <c r="X21" s="14"/>
-      <c r="Y21" s="14"/>
+      <c r="G21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
     </row>
     <row r="22" spans="1:25">
-      <c r="G22" s="6"/>
-      <c r="O22" s="71"/>
-      <c r="T22" s="75"/>
-      <c r="U22" s="14"/>
-      <c r="V22" s="14"/>
-      <c r="W22" s="14"/>
-      <c r="X22" s="14"/>
-      <c r="Y22" s="14"/>
+      <c r="G22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="T22" s="35"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
     </row>
     <row r="23" spans="1:25">
-      <c r="G23" s="6"/>
-      <c r="O23" s="71"/>
-      <c r="T23" s="75"/>
-      <c r="U23" s="14"/>
-      <c r="V23" s="14"/>
-      <c r="W23" s="14"/>
-      <c r="X23" s="14"/>
-      <c r="Y23" s="14"/>
+      <c r="G23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="T23" s="35"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
+      <c r="W23" s="13"/>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="13"/>
     </row>
     <row r="24" spans="1:25">
-      <c r="G24" s="6"/>
-      <c r="O24" s="71"/>
-      <c r="T24" s="75"/>
-      <c r="U24" s="14"/>
-      <c r="V24" s="14"/>
-      <c r="W24" s="14"/>
-      <c r="X24" s="14"/>
-      <c r="Y24" s="14"/>
+      <c r="G24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="T24" s="35"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13"/>
+      <c r="W24" s="13"/>
+      <c r="X24" s="13"/>
+      <c r="Y24" s="13"/>
     </row>
     <row r="25" spans="1:25">
-      <c r="G25" s="6"/>
-      <c r="O25" s="71"/>
-      <c r="T25" s="75"/>
-      <c r="U25" s="14"/>
-      <c r="V25" s="14"/>
-      <c r="W25" s="14"/>
-      <c r="X25" s="14"/>
-      <c r="Y25" s="14"/>
+      <c r="G25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="T25" s="35"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="13"/>
+      <c r="W25" s="13"/>
+      <c r="X25" s="13"/>
+      <c r="Y25" s="13"/>
     </row>
     <row r="26" spans="1:25">
-      <c r="G26" s="6"/>
-      <c r="O26" s="71"/>
-      <c r="T26" s="81"/>
-      <c r="U26" s="14"/>
-      <c r="V26" s="14"/>
-      <c r="W26" s="14"/>
-      <c r="X26" s="14"/>
-      <c r="Y26" s="14"/>
+      <c r="G26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="T26" s="63"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="13"/>
+      <c r="W26" s="13"/>
+      <c r="X26" s="13"/>
+      <c r="Y26" s="13"/>
     </row>
     <row r="27" spans="1:25">
-      <c r="G27" s="6"/>
-      <c r="O27" s="71"/>
-      <c r="T27" s="83"/>
-      <c r="U27" s="14"/>
-      <c r="V27" s="14"/>
-      <c r="W27" s="14"/>
-      <c r="X27" s="14"/>
-      <c r="Y27" s="14"/>
+      <c r="G27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="T27" s="64"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
+      <c r="W27" s="13"/>
+      <c r="X27" s="13"/>
+      <c r="Y27" s="13"/>
     </row>
     <row r="28" spans="1:25">
-      <c r="G28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="T28" s="41"/>
-      <c r="U28" s="14"/>
-      <c r="V28" s="14"/>
-      <c r="W28" s="14"/>
-      <c r="X28" s="14"/>
-      <c r="Y28" s="14"/>
+      <c r="G28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="T28" s="35"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="13"/>
+      <c r="W28" s="13"/>
+      <c r="X28" s="13"/>
+      <c r="Y28" s="13"/>
     </row>
     <row r="29" spans="1:25">
-      <c r="G29" s="52"/>
-      <c r="O29" s="6"/>
-      <c r="T29" s="85"/>
-      <c r="U29" s="14"/>
-      <c r="V29" s="14"/>
-      <c r="W29" s="14"/>
-      <c r="X29" s="14"/>
-      <c r="Y29" s="14"/>
+      <c r="G29" s="30"/>
+      <c r="O29" s="5"/>
+      <c r="T29" s="63"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="13"/>
+      <c r="W29" s="13"/>
+      <c r="X29" s="13"/>
+      <c r="Y29" s="13"/>
     </row>
     <row r="30" spans="1:25">
-      <c r="G30" s="86"/>
-      <c r="O30" s="14"/>
-      <c r="T30" s="89"/>
-      <c r="U30" s="14"/>
-      <c r="V30" s="14"/>
-      <c r="W30" s="14"/>
-      <c r="X30" s="14"/>
-      <c r="Y30" s="14"/>
+      <c r="G30" s="66"/>
+      <c r="O30" s="13"/>
+      <c r="T30" s="69"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="13"/>
+      <c r="W30" s="13"/>
+      <c r="X30" s="13"/>
+      <c r="Y30" s="13"/>
     </row>
     <row r="31" spans="1:25">
-      <c r="G31" s="86"/>
-      <c r="O31" s="14"/>
-      <c r="T31" s="89"/>
-      <c r="U31" s="14"/>
-      <c r="V31" s="14"/>
-      <c r="W31" s="14"/>
-      <c r="X31" s="14"/>
-      <c r="Y31" s="14"/>
+      <c r="G31" s="66"/>
+      <c r="O31" s="13"/>
+      <c r="T31" s="69"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="13"/>
+      <c r="W31" s="13"/>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="13"/>
     </row>
     <row r="32" spans="1:25">
-      <c r="G32" s="86"/>
-      <c r="O32" s="14"/>
-      <c r="T32" s="89"/>
-      <c r="U32" s="14"/>
-      <c r="V32" s="14"/>
-      <c r="W32" s="14"/>
-      <c r="X32" s="14"/>
-      <c r="Y32" s="14"/>
+      <c r="G32" s="66"/>
+      <c r="O32" s="13"/>
+      <c r="T32" s="69"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
+      <c r="W32" s="13"/>
+      <c r="X32" s="13"/>
+      <c r="Y32" s="13"/>
     </row>
     <row r="33" spans="1:25">
-      <c r="A33" s="35"/>
-      <c r="B33" s="55"/>
-      <c r="C33" s="55"/>
-      <c r="D33" s="97"/>
-      <c r="E33" s="98"/>
-      <c r="F33" s="99"/>
-      <c r="G33" s="86"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
-      <c r="T33" s="14"/>
-      <c r="U33" s="14"/>
-      <c r="V33" s="14"/>
-      <c r="W33" s="14"/>
-      <c r="X33" s="14"/>
-      <c r="Y33" s="14"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="66"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="13"/>
+      <c r="V33" s="13"/>
+      <c r="W33" s="13"/>
+      <c r="X33" s="13"/>
+      <c r="Y33" s="13"/>
     </row>
     <row r="34" spans="1:25">
-      <c r="A34" s="35"/>
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="102"/>
-      <c r="E34" s="103"/>
-      <c r="F34" s="104"/>
-      <c r="G34" s="86"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
-      <c r="T34" s="14"/>
-      <c r="U34" s="14"/>
-      <c r="V34" s="14"/>
-      <c r="W34" s="14"/>
-      <c r="X34" s="14"/>
-      <c r="Y34" s="14"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="66"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="13"/>
+      <c r="W34" s="13"/>
+      <c r="X34" s="13"/>
+      <c r="Y34" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3137,32 +3062,32 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F14"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26171875" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="38.25">
+    <row r="1" spans="1:6" ht="49.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="61" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="47" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3170,21 +3095,21 @@
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="69">
+      <c r="B2" s="54">
         <v>166018</v>
       </c>
-      <c r="C2" s="69">
+      <c r="C2" s="54">
         <v>154290</v>
       </c>
-      <c r="D2" s="70">
-        <f t="shared" ref="D2:D14" si="0">(C2-B2)/B2</f>
+      <c r="D2" s="14">
+        <v>137349</v>
+      </c>
+      <c r="E2" s="55">
+        <f>(C2-B2)/B2</f>
         <v>-7.0642942331554409E-2</v>
       </c>
-      <c r="E2" s="18">
-        <v>137349</v>
-      </c>
-      <c r="F2" s="19">
-        <f t="shared" ref="F2:F9" si="1">(E2-C2)/C2</f>
+      <c r="F2" s="16">
+        <f>(D2-C2)/C2</f>
         <v>-0.10979972778533929</v>
       </c>
     </row>
@@ -3192,21 +3117,21 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="76">
+      <c r="B3" s="58">
         <v>153234</v>
       </c>
-      <c r="C3" s="69">
+      <c r="C3" s="54">
         <v>139138</v>
       </c>
-      <c r="D3" s="70">
-        <f t="shared" si="0"/>
+      <c r="D3" s="14">
+        <v>126757</v>
+      </c>
+      <c r="E3" s="55">
+        <f>(C3-B3)/B3</f>
         <v>-9.199002832269601E-2</v>
       </c>
-      <c r="E3" s="18">
-        <v>126757</v>
-      </c>
-      <c r="F3" s="19">
-        <f t="shared" si="1"/>
+      <c r="F3" s="16">
+        <f>(D3-C3)/C3</f>
         <v>-8.8983599016803458E-2</v>
       </c>
     </row>
@@ -3214,21 +3139,21 @@
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="69">
+      <c r="B4" s="54">
         <v>149129</v>
       </c>
-      <c r="C4" s="69">
+      <c r="C4" s="54">
         <v>139609</v>
       </c>
-      <c r="D4" s="70">
-        <f t="shared" si="0"/>
+      <c r="D4" s="14">
+        <v>117550</v>
+      </c>
+      <c r="E4" s="55">
+        <f>(C4-B4)/B4</f>
         <v>-6.3837348872452709E-2</v>
       </c>
-      <c r="E4" s="18">
-        <v>117550</v>
-      </c>
-      <c r="F4" s="19">
-        <f t="shared" si="1"/>
+      <c r="F4" s="16">
+        <f>(D4-C4)/C4</f>
         <v>-0.15800557270663065</v>
       </c>
     </row>
@@ -3236,21 +3161,21 @@
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="69">
+      <c r="B5" s="54">
         <v>146506</v>
       </c>
-      <c r="C5" s="69">
+      <c r="C5" s="54">
         <v>126227</v>
       </c>
-      <c r="D5" s="70">
-        <f t="shared" si="0"/>
+      <c r="D5" s="14">
+        <v>113477</v>
+      </c>
+      <c r="E5" s="55">
+        <f>(C5-B5)/B5</f>
         <v>-0.13841753921341104</v>
       </c>
-      <c r="E5" s="18">
-        <v>113477</v>
-      </c>
-      <c r="F5" s="19">
-        <f t="shared" si="1"/>
+      <c r="F5" s="16">
+        <f>(D5-C5)/C5</f>
         <v>-0.10100850055851759</v>
       </c>
     </row>
@@ -3258,21 +3183,21 @@
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="69">
+      <c r="B6" s="54">
         <v>122937</v>
       </c>
-      <c r="C6" s="69">
+      <c r="C6" s="54">
         <v>128749</v>
       </c>
-      <c r="D6" s="70">
-        <f t="shared" si="0"/>
+      <c r="D6" s="14">
+        <v>108336</v>
+      </c>
+      <c r="E6" s="55">
+        <f>(C6-B6)/B6</f>
         <v>4.7276247183516758E-2</v>
       </c>
-      <c r="E6" s="18">
-        <v>108336</v>
-      </c>
-      <c r="F6" s="19">
-        <f t="shared" si="1"/>
+      <c r="F6" s="16">
+        <f>(D6-C6)/C6</f>
         <v>-0.15854880426255738</v>
       </c>
     </row>
@@ -3280,21 +3205,21 @@
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="69">
+      <c r="B7" s="54">
         <v>113710</v>
       </c>
-      <c r="C7" s="69">
+      <c r="C7" s="54">
         <v>125671</v>
       </c>
-      <c r="D7" s="70">
-        <f t="shared" si="0"/>
+      <c r="D7" s="14">
+        <v>98523</v>
+      </c>
+      <c r="E7" s="55">
+        <f>(C7-B7)/B7</f>
         <v>0.10518863776272976</v>
       </c>
-      <c r="E7" s="18">
-        <v>98523</v>
-      </c>
-      <c r="F7" s="19">
-        <f t="shared" si="1"/>
+      <c r="F7" s="16">
+        <f>(D7-C7)/C7</f>
         <v>-0.21602438112213637</v>
       </c>
     </row>
@@ -3302,21 +3227,21 @@
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="69">
+      <c r="B8" s="54">
         <v>117122</v>
       </c>
-      <c r="C8" s="69">
+      <c r="C8" s="54">
         <v>147302</v>
       </c>
-      <c r="D8" s="70">
-        <f t="shared" si="0"/>
+      <c r="D8" s="14">
+        <v>103029</v>
+      </c>
+      <c r="E8" s="55">
+        <f>(C8-B8)/B8</f>
         <v>0.25768002595584094</v>
       </c>
-      <c r="E8" s="18">
-        <v>103029</v>
-      </c>
-      <c r="F8" s="19">
-        <f t="shared" si="1"/>
+      <c r="F8" s="16">
+        <f>(D8-C8)/C8</f>
         <v>-0.30055939498445372</v>
       </c>
     </row>
@@ -3324,21 +3249,21 @@
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="69">
+      <c r="B9" s="54">
         <v>126623</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="54">
         <v>145461</v>
       </c>
-      <c r="D9" s="70">
-        <f t="shared" si="0"/>
+      <c r="D9" s="14">
+        <v>115694</v>
+      </c>
+      <c r="E9" s="55">
+        <f>(C9-B9)/B9</f>
         <v>0.14877233993824188</v>
       </c>
-      <c r="E9" s="18">
-        <v>115694</v>
-      </c>
-      <c r="F9" s="19">
-        <f t="shared" si="1"/>
+      <c r="F9" s="16">
+        <f>(D9-C9)/C9</f>
         <v>-0.20463904414241618</v>
       </c>
     </row>
@@ -3346,91 +3271,91 @@
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="69">
+      <c r="B10" s="54">
         <v>122360</v>
       </c>
-      <c r="C10" s="69">
+      <c r="C10" s="54">
         <v>149470</v>
       </c>
-      <c r="D10" s="70">
-        <f t="shared" si="0"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="55">
+        <f>(C10-B10)/B10</f>
         <v>0.22155933311539719</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
+      <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="69">
+      <c r="B11" s="54">
         <v>132280</v>
       </c>
-      <c r="C11" s="69">
+      <c r="C11" s="54">
         <v>165507</v>
       </c>
-      <c r="D11" s="70">
-        <f t="shared" si="0"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="55">
+        <f>(C11-B11)/B11</f>
         <v>0.25118687632295134</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19"/>
+      <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="69">
+      <c r="B12" s="54">
         <v>128303</v>
       </c>
-      <c r="C12" s="69">
+      <c r="C12" s="54">
         <v>162736</v>
       </c>
-      <c r="D12" s="70">
-        <f t="shared" si="0"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="55">
+        <f>(C12-B12)/B12</f>
         <v>0.2683725244148617</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="19"/>
+      <c r="F12" s="16"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="69">
+      <c r="B13" s="54">
         <v>132120</v>
       </c>
-      <c r="C13" s="69">
+      <c r="C13" s="54">
         <v>165619</v>
       </c>
-      <c r="D13" s="70">
-        <f t="shared" si="0"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="55">
+        <f>(C13-B13)/B13</f>
         <v>0.25354980320920373</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
+      <c r="F13" s="16"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="26">
         <f>SUM(B2:B13)</f>
         <v>1610342</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="26">
         <f>SUM(C2:C13)</f>
         <v>1749779</v>
       </c>
-      <c r="D14" s="32">
-        <f t="shared" si="0"/>
+      <c r="D14" s="26">
+        <f>SUM(D2:D13)</f>
+        <v>920715</v>
+      </c>
+      <c r="E14" s="27">
+        <f>(C14-B14)/B14</f>
         <v>8.6588438977558801E-2</v>
       </c>
-      <c r="E14" s="31">
-        <f>SUM(E2:E13)</f>
-        <v>920715</v>
-      </c>
-      <c r="F14" s="32">
+      <c r="F14" s="27">
         <f>AVERAGE(F2:F13)</f>
         <v>-0.16719612807235684</v>
       </c>
@@ -3445,421 +3370,416 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116C5861-0548-4071-B9F1-0FF3651A304B}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="2" max="3" width="14.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.578125" customWidth="1"/>
+    <col min="5" max="5" width="14.68359375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="38.25">
+    <row r="1" spans="1:11" ht="36.9">
       <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="14">
         <v>24129.87</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="14">
         <v>40365</v>
       </c>
-      <c r="D2" s="17">
-        <f t="shared" ref="D2:D14" si="0">(C2-B2)/B2</f>
+      <c r="D2" s="14">
+        <v>41888</v>
+      </c>
+      <c r="E2" s="16">
+        <f>(C2-B2)/B2</f>
         <v>0.67282293688279304</v>
       </c>
-      <c r="E2" s="18">
-        <v>41888</v>
-      </c>
-      <c r="F2" s="20">
-        <f t="shared" ref="F2:F9" si="1">(E2-C2)/C2</f>
+      <c r="F2" s="17">
+        <f>(D2-C2)/C2</f>
         <v>3.773070729592469E-2</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>48114.28</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>37545</v>
       </c>
-      <c r="D3" s="17">
-        <f t="shared" si="0"/>
+      <c r="D3" s="18">
+        <v>42788</v>
+      </c>
+      <c r="E3" s="16">
+        <f>(C3-B3)/B3</f>
         <v>-0.21967033487771195</v>
       </c>
-      <c r="E3" s="22">
-        <v>42788</v>
-      </c>
-      <c r="F3" s="20">
-        <f t="shared" si="1"/>
+      <c r="F3" s="17">
+        <f>(D3-C3)/C3</f>
         <v>0.13964575842322546</v>
       </c>
-      <c r="G3" s="107" t="s">
+      <c r="G3" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
-      <c r="K3" s="108"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <v>25782</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <v>25781.81</v>
       </c>
-      <c r="D4" s="17">
-        <f t="shared" si="0"/>
+      <c r="D4" s="18">
+        <v>45023</v>
+      </c>
+      <c r="E4" s="16">
+        <f>(C4-B4)/B4</f>
         <v>-7.3694825846982515E-6</v>
       </c>
-      <c r="E4" s="22">
-        <v>45023</v>
-      </c>
-      <c r="F4" s="20">
-        <f t="shared" si="1"/>
+      <c r="F4" s="17">
+        <f>(D4-C4)/C4</f>
         <v>0.74630873472421055</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>35554.239999999998</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>25781.81</v>
       </c>
-      <c r="D5" s="17">
-        <f t="shared" si="0"/>
+      <c r="D5" s="18">
+        <v>25839</v>
+      </c>
+      <c r="E5" s="16">
+        <f>(C5-B5)/B5</f>
         <v>-0.27485976356125169</v>
       </c>
-      <c r="E5" s="22">
-        <v>25839</v>
-      </c>
-      <c r="F5" s="20">
-        <f t="shared" si="1"/>
+      <c r="F5" s="17">
+        <f>(D5-C5)/C5</f>
         <v>2.2182306052212272E-3</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>15728</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>13432.28</v>
       </c>
-      <c r="D6" s="17">
-        <f t="shared" si="0"/>
+      <c r="D6" s="18">
+        <v>12769</v>
+      </c>
+      <c r="E6" s="16">
+        <f>(C6-B6)/B6</f>
         <v>-0.14596388606307217</v>
       </c>
-      <c r="E6" s="22">
-        <v>12769</v>
-      </c>
-      <c r="F6" s="20">
-        <f t="shared" si="1"/>
+      <c r="F6" s="17">
+        <f>(D6-C6)/C6</f>
         <v>-4.9379554327336879E-2</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>15395.12</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>15430.56</v>
       </c>
-      <c r="D7" s="17">
-        <f t="shared" si="0"/>
+      <c r="D7" s="18">
+        <v>10444</v>
+      </c>
+      <c r="E7" s="16">
+        <f>(C7-B7)/B7</f>
         <v>2.3020281751619143E-3</v>
       </c>
-      <c r="E7" s="22">
-        <v>10444</v>
-      </c>
-      <c r="F7" s="20">
-        <f t="shared" si="1"/>
+      <c r="F7" s="17">
+        <f>(D7-C7)/C7</f>
         <v>-0.32316131106064844</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>9067.8799999999992</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <v>7210.53</v>
       </c>
-      <c r="D8" s="17">
-        <f t="shared" si="0"/>
+      <c r="D8" s="14">
+        <v>8021</v>
+      </c>
+      <c r="E8" s="16">
+        <f>(C8-B8)/B8</f>
         <v>-0.20482736869036638</v>
       </c>
-      <c r="E8" s="18">
-        <v>8021</v>
-      </c>
-      <c r="F8" s="20">
-        <f t="shared" si="1"/>
+      <c r="F8" s="17">
+        <f>(D8-C8)/C8</f>
         <v>0.11240089147399709</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>12090</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <v>7045.99</v>
       </c>
-      <c r="D9" s="17">
-        <f t="shared" si="0"/>
+      <c r="D9" s="14">
+        <v>11379</v>
+      </c>
+      <c r="E9" s="16">
+        <f>(C9-B9)/B9</f>
         <v>-0.41720512820512823</v>
       </c>
-      <c r="E9" s="18">
-        <v>11379</v>
-      </c>
-      <c r="F9" s="20">
-        <f t="shared" si="1"/>
+      <c r="F9" s="17">
+        <f>(D9-C9)/C9</f>
         <v>0.61496113392156393</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="19">
         <v>15191</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="19">
         <v>23032</v>
       </c>
-      <c r="D10" s="25">
-        <f t="shared" si="0"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="21">
+        <f>(C10-B10)/B10</f>
         <v>0.51616088473438215</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B11" s="19">
         <v>17892</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="19">
         <v>36770</v>
       </c>
-      <c r="D11" s="25">
-        <f t="shared" si="0"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="21">
+        <f>(C11-B11)/B11</f>
         <v>1.0551084283478649</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="19">
         <v>41103</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="19">
         <v>40381</v>
       </c>
-      <c r="D12" s="25">
-        <f t="shared" si="0"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="21">
+        <f>(C12-B12)/B12</f>
         <v>-1.7565627813055009E-2</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="22">
         <v>31826.36</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="22">
         <v>34355</v>
       </c>
-      <c r="D13" s="17">
-        <f t="shared" si="0"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="16">
+        <f>(C13-B13)/B13</f>
         <v>7.9451121648847031E-2</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="26">
         <f>SUM(B2:B13)</f>
         <v>291873.75</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="26">
         <f>SUM(C2:C13)</f>
         <v>307130.98</v>
       </c>
-      <c r="D14" s="32">
-        <f t="shared" si="0"/>
+      <c r="D14" s="28">
+        <f>SUM(D2:D13)</f>
+        <v>198151</v>
+      </c>
+      <c r="E14" s="27">
+        <f>(C14-B14)/B14</f>
         <v>5.2273388751129489E-2</v>
       </c>
-      <c r="E14" s="33">
-        <f>SUM(E2:E13)</f>
-        <v>198151</v>
-      </c>
-      <c r="F14" s="34">
+      <c r="F14" s="29">
         <f>AVERAGE(F2:F13)</f>
         <v>0.16009057388201969</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-    </row>
-    <row r="15" spans="1:11" ht="25.5">
-      <c r="A15" s="41"/>
-      <c r="B15" s="42" t="s">
+      <c r="G14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+    </row>
+    <row r="15" spans="1:11" ht="24.6">
+      <c r="A15" s="35"/>
+      <c r="B15" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="36"/>
+      <c r="E15" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="44"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="41"/>
-      <c r="B16" s="51">
+      <c r="A16" s="35"/>
+      <c r="B16" s="42">
         <v>331445.11</v>
       </c>
-      <c r="C16" s="51">
+      <c r="C16" s="42">
         <v>272775.98</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="36"/>
+      <c r="E16" s="17">
         <f>(C16-B16)/C16</f>
         <v>-0.2150817311700246</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added all reading from excel functions
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janhe\SPE\Green-Credentials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D994D5-F568-4C43-97DE-FE4145BC6807}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C024069-0EF2-4668-ACA9-BD1C01341D23}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11184" yWindow="2388" windowWidth="17328" windowHeight="9462" firstSheet="1" activeTab="5" xr2:uid="{0C7B78C3-690B-478C-8020-AF23CEA86F9E}"/>
+    <workbookView xWindow="0" yWindow="2388" windowWidth="17328" windowHeight="9462" firstSheet="1" activeTab="3" xr2:uid="{0C7B78C3-690B-478C-8020-AF23CEA86F9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Waste" sheetId="6" r:id="rId1"/>
@@ -1795,11 +1795,11 @@
         <v>8273</v>
       </c>
       <c r="E2" s="16">
-        <f>(C2-B2)/B2</f>
+        <f t="shared" ref="E2:E14" si="0">(C2-B2)/B2</f>
         <v>0.12308254200146092</v>
       </c>
       <c r="F2" s="17">
-        <f>(D2-C2)/D2</f>
+        <f t="shared" ref="F2:F10" si="1">(D2-C2)/D2</f>
         <v>0.25661791369515291</v>
       </c>
     </row>
@@ -1817,11 +1817,11 @@
         <v>7349</v>
       </c>
       <c r="E3" s="16">
-        <f>(C3-B3)/B3</f>
+        <f t="shared" si="0"/>
         <v>5.9652029826014917E-3</v>
       </c>
       <c r="F3" s="17">
-        <f>(D3-C3)/D3</f>
+        <f t="shared" si="1"/>
         <v>0.17390121104912232</v>
       </c>
     </row>
@@ -1839,11 +1839,11 @@
         <v>5620</v>
       </c>
       <c r="E4" s="16">
-        <f>(C4-B4)/B4</f>
+        <f t="shared" si="0"/>
         <v>4.6127882992687046E-2</v>
       </c>
       <c r="F4" s="17">
-        <f>(D4-C4)/D4</f>
+        <f t="shared" si="1"/>
         <v>7.2953736654804268E-3</v>
       </c>
     </row>
@@ -1861,11 +1861,11 @@
         <v>8615</v>
       </c>
       <c r="E5" s="16">
-        <f>(C5-B5)/B5</f>
+        <f t="shared" si="0"/>
         <v>-0.2250304095147993</v>
       </c>
       <c r="F5" s="17">
-        <f>(D5-C5)/D5</f>
+        <f t="shared" si="1"/>
         <v>0.33441671503192105</v>
       </c>
     </row>
@@ -1883,11 +1883,11 @@
         <v>10387</v>
       </c>
       <c r="E6" s="16">
-        <f>(C6-B6)/B6</f>
+        <f t="shared" si="0"/>
         <v>-9.6371028459569345E-3</v>
       </c>
       <c r="F6" s="17">
-        <f>(D6-C6)/D6</f>
+        <f t="shared" si="1"/>
         <v>0.36680465967074227</v>
       </c>
     </row>
@@ -1905,11 +1905,11 @@
         <v>8235</v>
       </c>
       <c r="E7" s="16">
-        <f>(C7-B7)/B7</f>
+        <f t="shared" si="0"/>
         <v>0.17089876378215837</v>
       </c>
       <c r="F7" s="17">
-        <f>(D7-C7)/D7</f>
+        <f t="shared" si="1"/>
         <v>0.14887674559805708</v>
       </c>
     </row>
@@ -1927,11 +1927,11 @@
         <v>7634</v>
       </c>
       <c r="E8" s="16">
-        <f>(C8-B8)/B8</f>
+        <f t="shared" si="0"/>
         <v>-1.7520805957074025E-2</v>
       </c>
       <c r="F8" s="17">
-        <f>(D8-C8)/D8</f>
+        <f t="shared" si="1"/>
         <v>0.11854859837568771</v>
       </c>
     </row>
@@ -1949,11 +1949,11 @@
         <v>8694</v>
       </c>
       <c r="E9" s="16">
-        <f>(C9-B9)/B9</f>
+        <f t="shared" si="0"/>
         <v>0.36460656259955398</v>
       </c>
       <c r="F9" s="17">
-        <f>(D9-C9)/D9</f>
+        <f t="shared" si="1"/>
         <v>1.4607775477340695E-2</v>
       </c>
     </row>
@@ -1971,11 +1971,11 @@
         <v>8007</v>
       </c>
       <c r="E10" s="16">
-        <f>(C10-B10)/B10</f>
+        <f t="shared" si="0"/>
         <v>0.30778894472361806</v>
       </c>
       <c r="F10" s="17">
-        <f>(D10-C10)/D10</f>
+        <f t="shared" si="1"/>
         <v>-4.0089921318846013E-2</v>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D11" s="83"/>
       <c r="E11" s="16">
-        <f>(C11-B11)/B11</f>
+        <f t="shared" si="0"/>
         <v>0.48769693751106391</v>
       </c>
       <c r="F11" s="17"/>
@@ -2008,7 +2008,7 @@
       </c>
       <c r="D12" s="83"/>
       <c r="E12" s="16">
-        <f>(C12-B12)/B12</f>
+        <f t="shared" si="0"/>
         <v>0.16805460750853243</v>
       </c>
       <c r="F12" s="17"/>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="D13" s="83"/>
       <c r="E13" s="21">
-        <f>(C13-B13)/B13</f>
+        <f t="shared" si="0"/>
         <v>-0.19534293739240735</v>
       </c>
       <c r="F13" s="17"/>
@@ -2045,7 +2045,7 @@
         <v>72814</v>
       </c>
       <c r="E14" s="27">
-        <f>(C14-B14)/B14</f>
+        <f t="shared" si="0"/>
         <v>0.12063917852867795</v>
       </c>
       <c r="F14" s="29">
@@ -2455,8 +2455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BC1D0F-CAAD-431F-A14A-C9799CB6C71A}">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2502,11 +2502,11 @@
         <v>358709</v>
       </c>
       <c r="E2" s="16">
-        <f>(C2-B2)/B2</f>
+        <f t="shared" ref="E2:F9" si="0">(C2-B2)/B2</f>
         <v>-3.4261681154429506E-2</v>
       </c>
       <c r="F2" s="16">
-        <f>(D2-C2)/C2</f>
+        <f t="shared" si="0"/>
         <v>-5.9493969585736758E-2</v>
       </c>
       <c r="G2" s="5"/>
@@ -2526,11 +2526,11 @@
         <v>320011</v>
       </c>
       <c r="E3" s="16">
-        <f>(C3-B3)/B3</f>
+        <f t="shared" si="0"/>
         <v>-8.0077100205799917E-2</v>
       </c>
       <c r="F3" s="16">
-        <f>(D3-C3)/C3</f>
+        <f t="shared" si="0"/>
         <v>-5.4279533539414504E-2</v>
       </c>
       <c r="G3" s="5"/>
@@ -2550,11 +2550,11 @@
         <v>323736</v>
       </c>
       <c r="E4" s="16">
-        <f>(C4-B4)/B4</f>
+        <f t="shared" si="0"/>
         <v>-4.4445401610371853E-2</v>
       </c>
       <c r="F4" s="16">
-        <f>(D4-C4)/C4</f>
+        <f t="shared" si="0"/>
         <v>-8.7957132835808277E-2</v>
       </c>
       <c r="G4" s="5"/>
@@ -2574,11 +2574,11 @@
         <v>307995</v>
       </c>
       <c r="E5" s="16">
-        <f>(C5-B5)/B5</f>
+        <f t="shared" si="0"/>
         <v>-0.10544607735495606</v>
       </c>
       <c r="F5" s="16">
-        <f>(D5-C5)/C5</f>
+        <f t="shared" si="0"/>
         <v>-6.6611106902038031E-2</v>
       </c>
       <c r="G5" s="5"/>
@@ -2598,11 +2598,11 @@
         <v>305855</v>
       </c>
       <c r="E6" s="16">
-        <f>(C6-B6)/B6</f>
+        <f t="shared" si="0"/>
         <v>-3.2723237387046506E-3</v>
       </c>
       <c r="F6" s="16">
-        <f>(D6-C6)/C6</f>
+        <f t="shared" si="0"/>
         <v>-8.2136694425688342E-2</v>
       </c>
       <c r="G6" s="5"/>
@@ -2622,11 +2622,11 @@
         <v>289224</v>
       </c>
       <c r="E7" s="16">
-        <f>(C7-B7)/B7</f>
+        <f t="shared" si="0"/>
         <v>-1.5508317929759704E-2</v>
       </c>
       <c r="F7" s="16">
-        <f>(D7-C7)/C7</f>
+        <f t="shared" si="0"/>
         <v>-9.4947522577495724E-2</v>
       </c>
       <c r="G7" s="5"/>
@@ -2646,11 +2646,11 @@
         <v>327266</v>
       </c>
       <c r="E8" s="16">
-        <f>(C8-B8)/B8</f>
+        <f t="shared" si="0"/>
         <v>3.5355563279836029E-2</v>
       </c>
       <c r="F8" s="16">
-        <f>(D8-C8)/C8</f>
+        <f t="shared" si="0"/>
         <v>-5.2838740112814489E-2</v>
       </c>
       <c r="G8" s="5"/>
@@ -2670,11 +2670,11 @@
         <v>337334</v>
       </c>
       <c r="E9" s="16">
-        <f>(C9-B9)/B9</f>
+        <f t="shared" si="0"/>
         <v>-1.2586711001547899E-2</v>
       </c>
       <c r="F9" s="16">
-        <f>(D9-C9)/C9</f>
+        <f t="shared" si="0"/>
         <v>-2.0713039489765408E-2</v>
       </c>
       <c r="G9" s="5"/>
@@ -3105,11 +3105,11 @@
         <v>137349</v>
       </c>
       <c r="E2" s="55">
-        <f>(C2-B2)/B2</f>
+        <f t="shared" ref="E2:F9" si="0">(C2-B2)/B2</f>
         <v>-7.0642942331554409E-2</v>
       </c>
       <c r="F2" s="16">
-        <f>(D2-C2)/C2</f>
+        <f t="shared" si="0"/>
         <v>-0.10979972778533929</v>
       </c>
     </row>
@@ -3127,11 +3127,11 @@
         <v>126757</v>
       </c>
       <c r="E3" s="55">
-        <f>(C3-B3)/B3</f>
+        <f t="shared" si="0"/>
         <v>-9.199002832269601E-2</v>
       </c>
       <c r="F3" s="16">
-        <f>(D3-C3)/C3</f>
+        <f t="shared" si="0"/>
         <v>-8.8983599016803458E-2</v>
       </c>
     </row>
@@ -3149,11 +3149,11 @@
         <v>117550</v>
       </c>
       <c r="E4" s="55">
-        <f>(C4-B4)/B4</f>
+        <f t="shared" si="0"/>
         <v>-6.3837348872452709E-2</v>
       </c>
       <c r="F4" s="16">
-        <f>(D4-C4)/C4</f>
+        <f t="shared" si="0"/>
         <v>-0.15800557270663065</v>
       </c>
     </row>
@@ -3171,11 +3171,11 @@
         <v>113477</v>
       </c>
       <c r="E5" s="55">
-        <f>(C5-B5)/B5</f>
+        <f t="shared" si="0"/>
         <v>-0.13841753921341104</v>
       </c>
       <c r="F5" s="16">
-        <f>(D5-C5)/C5</f>
+        <f t="shared" si="0"/>
         <v>-0.10100850055851759</v>
       </c>
     </row>
@@ -3193,11 +3193,11 @@
         <v>108336</v>
       </c>
       <c r="E6" s="55">
-        <f>(C6-B6)/B6</f>
+        <f t="shared" si="0"/>
         <v>4.7276247183516758E-2</v>
       </c>
       <c r="F6" s="16">
-        <f>(D6-C6)/C6</f>
+        <f t="shared" si="0"/>
         <v>-0.15854880426255738</v>
       </c>
     </row>
@@ -3215,11 +3215,11 @@
         <v>98523</v>
       </c>
       <c r="E7" s="55">
-        <f>(C7-B7)/B7</f>
+        <f t="shared" si="0"/>
         <v>0.10518863776272976</v>
       </c>
       <c r="F7" s="16">
-        <f>(D7-C7)/C7</f>
+        <f t="shared" si="0"/>
         <v>-0.21602438112213637</v>
       </c>
     </row>
@@ -3237,11 +3237,11 @@
         <v>103029</v>
       </c>
       <c r="E8" s="55">
-        <f>(C8-B8)/B8</f>
+        <f t="shared" si="0"/>
         <v>0.25768002595584094</v>
       </c>
       <c r="F8" s="16">
-        <f>(D8-C8)/C8</f>
+        <f t="shared" si="0"/>
         <v>-0.30055939498445372</v>
       </c>
     </row>
@@ -3259,11 +3259,11 @@
         <v>115694</v>
       </c>
       <c r="E9" s="55">
-        <f>(C9-B9)/B9</f>
+        <f t="shared" si="0"/>
         <v>0.14877233993824188</v>
       </c>
       <c r="F9" s="16">
-        <f>(D9-C9)/C9</f>
+        <f t="shared" si="0"/>
         <v>-0.20463904414241618</v>
       </c>
     </row>
@@ -3370,7 +3370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116C5861-0548-4071-B9F1-0FF3651A304B}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -3419,11 +3419,11 @@
         <v>41888</v>
       </c>
       <c r="E2" s="16">
-        <f>(C2-B2)/B2</f>
+        <f t="shared" ref="E2:F9" si="0">(C2-B2)/B2</f>
         <v>0.67282293688279304</v>
       </c>
       <c r="F2" s="17">
-        <f>(D2-C2)/C2</f>
+        <f t="shared" si="0"/>
         <v>3.773070729592469E-2</v>
       </c>
       <c r="G2" s="13"/>
@@ -3446,11 +3446,11 @@
         <v>42788</v>
       </c>
       <c r="E3" s="16">
-        <f>(C3-B3)/B3</f>
+        <f t="shared" si="0"/>
         <v>-0.21967033487771195</v>
       </c>
       <c r="F3" s="17">
-        <f>(D3-C3)/C3</f>
+        <f t="shared" si="0"/>
         <v>0.13964575842322546</v>
       </c>
       <c r="G3" s="87" t="s">
@@ -3475,11 +3475,11 @@
         <v>45023</v>
       </c>
       <c r="E4" s="16">
-        <f>(C4-B4)/B4</f>
+        <f t="shared" si="0"/>
         <v>-7.3694825846982515E-6</v>
       </c>
       <c r="F4" s="17">
-        <f>(D4-C4)/C4</f>
+        <f t="shared" si="0"/>
         <v>0.74630873472421055</v>
       </c>
       <c r="G4" s="13"/>
@@ -3502,11 +3502,11 @@
         <v>25839</v>
       </c>
       <c r="E5" s="16">
-        <f>(C5-B5)/B5</f>
+        <f t="shared" si="0"/>
         <v>-0.27485976356125169</v>
       </c>
       <c r="F5" s="17">
-        <f>(D5-C5)/C5</f>
+        <f t="shared" si="0"/>
         <v>2.2182306052212272E-3</v>
       </c>
       <c r="G5" s="13"/>
@@ -3529,11 +3529,11 @@
         <v>12769</v>
       </c>
       <c r="E6" s="16">
-        <f>(C6-B6)/B6</f>
+        <f t="shared" si="0"/>
         <v>-0.14596388606307217</v>
       </c>
       <c r="F6" s="17">
-        <f>(D6-C6)/C6</f>
+        <f t="shared" si="0"/>
         <v>-4.9379554327336879E-2</v>
       </c>
       <c r="G6" s="13"/>
@@ -3556,11 +3556,11 @@
         <v>10444</v>
       </c>
       <c r="E7" s="16">
-        <f>(C7-B7)/B7</f>
+        <f t="shared" si="0"/>
         <v>2.3020281751619143E-3</v>
       </c>
       <c r="F7" s="17">
-        <f>(D7-C7)/C7</f>
+        <f t="shared" si="0"/>
         <v>-0.32316131106064844</v>
       </c>
       <c r="G7" s="13"/>
@@ -3583,11 +3583,11 @@
         <v>8021</v>
       </c>
       <c r="E8" s="16">
-        <f>(C8-B8)/B8</f>
+        <f t="shared" si="0"/>
         <v>-0.20482736869036638</v>
       </c>
       <c r="F8" s="17">
-        <f>(D8-C8)/C8</f>
+        <f t="shared" si="0"/>
         <v>0.11240089147399709</v>
       </c>
       <c r="G8" s="13"/>
@@ -3610,11 +3610,11 @@
         <v>11379</v>
       </c>
       <c r="E9" s="16">
-        <f>(C9-B9)/B9</f>
+        <f t="shared" si="0"/>
         <v>-0.41720512820512823</v>
       </c>
       <c r="F9" s="17">
-        <f>(D9-C9)/C9</f>
+        <f t="shared" si="0"/>
         <v>0.61496113392156393</v>
       </c>
       <c r="G9" s="13"/>

</xml_diff>

<commit_message>
getting last month now depends on a specific cell in data (elec table)
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janhe\SPE\Green-Credentials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Green-Credentials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C024069-0EF2-4668-ACA9-BD1C01341D23}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D518D5-0013-48C0-808B-C89DF4E3EA55}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2388" windowWidth="17328" windowHeight="9462" firstSheet="1" activeTab="3" xr2:uid="{0C7B78C3-690B-478C-8020-AF23CEA86F9E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{0C7B78C3-690B-478C-8020-AF23CEA86F9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Waste" sheetId="6" r:id="rId1"/>
@@ -759,8 +759,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -989,7 +989,7 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="right"/>
@@ -1118,7 +1118,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
@@ -1164,7 +1164,7 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1177,7 +1177,7 @@
     <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1567,7 +1567,7 @@
     <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24.6">
+    <row r="1" spans="1:4" ht="26.4">
       <c r="A1" s="51" t="s">
         <v>40</v>
       </c>
@@ -1763,7 +1763,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="49.2">
+    <row r="1" spans="1:6" ht="52.8">
       <c r="A1" s="1"/>
       <c r="B1" s="6" t="s">
         <v>5</v>
@@ -2053,7 +2053,7 @@
         <v>0.1534421190271843</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="43.2">
+    <row r="15" spans="1:6" ht="57.6">
       <c r="A15" s="33"/>
       <c r="B15" s="33" t="s">
         <v>28</v>
@@ -2098,7 +2098,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="49.2">
+    <row r="1" spans="1:7" ht="66">
       <c r="A1" s="37" t="s">
         <v>35</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>0.60202175088836485</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="43.2">
+    <row r="15" spans="1:7" ht="57.6">
       <c r="A15" s="79"/>
       <c r="B15" s="80" t="s">
         <v>44</v>
@@ -2456,19 +2456,19 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.41796875" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="49.2">
+    <row r="1" spans="1:14" ht="52.8">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2485,7 +2485,10 @@
       <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" s="5">
+        <f>COUNTA(D2:D13)</f>
+        <v>8</v>
+      </c>
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14">
@@ -2783,7 +2786,7 @@
       <c r="G14" s="5"/>
       <c r="N14" s="5"/>
     </row>
-    <row r="15" spans="1:14" ht="36.9">
+    <row r="15" spans="1:14" ht="52.8">
       <c r="A15" s="30"/>
       <c r="B15" s="1" t="s">
         <v>25</v>
@@ -3067,13 +3070,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26171875" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="49.2">
+    <row r="1" spans="1:6" ht="52.8">
       <c r="A1" s="1"/>
       <c r="B1" s="20" t="s">
         <v>32</v>
@@ -3376,13 +3379,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.578125" customWidth="1"/>
-    <col min="5" max="5" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.578125" customWidth="1"/>
+    <col min="2" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="36.9">
+    <row r="1" spans="1:11" ht="39.6">
       <c r="A1" s="1"/>
       <c r="B1" s="10" t="s">
         <v>8</v>
@@ -3737,7 +3740,7 @@
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="1:11" ht="24.6">
+    <row r="15" spans="1:11" ht="26.4">
       <c r="A15" s="35"/>
       <c r="B15" s="36" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
actual push of the previous commit
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janhe\SPE\Green-Credentials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Green-Credentials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE780D2-09E8-470A-9D49-9E73A6231A47}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD323F4-0117-459A-97C4-37A93D432EFF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2388" windowWidth="17328" windowHeight="9462" firstSheet="1" activeTab="5" xr2:uid="{0C7B78C3-690B-478C-8020-AF23CEA86F9E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{0C7B78C3-690B-478C-8020-AF23CEA86F9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Waste" sheetId="6" r:id="rId1"/>
@@ -686,7 +686,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="52">
   <si>
     <t>Elec 2017 (kWh)</t>
   </si>
@@ -836,6 +836,12 @@
   </si>
   <si>
     <t>Gas 2019 (kWh)</t>
+  </si>
+  <si>
+    <t>Additional comments:</t>
+  </si>
+  <si>
+    <t>This is a test.</t>
   </si>
 </sst>
 </file>
@@ -843,8 +849,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -891,12 +897,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Futura ND Book"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
@@ -934,6 +934,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1073,251 +1080,354 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="right"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="10" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="10" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="11" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="8" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="11" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1636,193 +1746,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11E648A-DDD9-4DEC-A8DC-7148C1AF4BEC}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="N2" sqref="N2:N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="1" max="3" width="8.88671875" style="21"/>
+    <col min="4" max="4" width="12" style="21" customWidth="1"/>
+    <col min="5" max="11" width="8.88671875" style="21"/>
+    <col min="12" max="12" width="9.33203125" style="21" customWidth="1"/>
+    <col min="13" max="13" width="17.21875" style="21" customWidth="1"/>
+    <col min="14" max="14" width="32.44140625" style="21" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="36.9">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:14" ht="39.6">
+      <c r="A1" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="30" t="s">
         <v>38</v>
       </c>
       <c r="M1">
         <f>COUNTA(C2:C13)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="54" t="s">
+      <c r="N1" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="55">
+      <c r="B2" s="33">
         <v>136.19999999999999</v>
       </c>
-      <c r="C2" s="55">
+      <c r="C2" s="33">
         <v>122.19</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="6">
         <f>C2/B2</f>
         <v>0.89713656387665208</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="54" t="s">
+      <c r="N2" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="55">
+      <c r="B3" s="33">
         <v>138.19999999999999</v>
       </c>
-      <c r="C3" s="55">
+      <c r="C3" s="33">
         <v>124.62</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="6">
         <f t="shared" ref="D3:D13" si="0">C3/B3</f>
         <v>0.90173661360347335</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="54" t="s">
+      <c r="N3" s="23"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="15" t="e">
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="54" t="s">
+      <c r="N4" s="23"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="15" t="e">
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="54" t="s">
+      <c r="N5" s="23"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="15" t="e">
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="54" t="s">
+      <c r="N6" s="23"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="15" t="e">
+      <c r="B7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="54" t="s">
+      <c r="N7" s="23"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="15" t="e">
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="54" t="s">
+      <c r="N8" s="23"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="15" t="e">
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="54" t="s">
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="15" t="e">
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="54" t="s">
+      <c r="N10" s="23"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="15" t="e">
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="54" t="s">
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="85"/>
-      <c r="C12" s="85"/>
-      <c r="D12" s="15" t="e">
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="54" t="s">
+      <c r="N12" s="23"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="15" t="e">
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="71" t="s">
+      <c r="N13" s="23"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="72">
+      <c r="B14" s="38">
         <f>SUM(B2:B13)</f>
         <v>274.39999999999998</v>
       </c>
-      <c r="C14" s="72">
+      <c r="C14" s="38">
         <f>SUM(C2:C13)</f>
         <v>246.81</v>
       </c>
-      <c r="D14" s="73" t="e">
+      <c r="D14" s="39" t="e">
         <f>AVERAGE(D2:D13)</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="N14" s="23"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="N15" s="23"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="N16" s="23"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="CBRqd0wM120iM1ikX3ylqN4nz96YDbgvObD55ZquG3G/W/y4uuRDigSoLJF7t/ppJXrxd3LdZ4g3aFZHPil/zg==" saltValue="3ZljL6AByAn88Mzez6OPMw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="N2:N16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1830,325 +1974,355 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7AF804-493F-4EDB-83A6-FDA04192F147}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="12" width="8.88671875" style="21"/>
+    <col min="13" max="13" width="14.6640625" style="21" customWidth="1"/>
+    <col min="14" max="14" width="32.21875" style="21" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="21"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="61.5">
-      <c r="A1" s="1"/>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:14" ht="79.2">
+      <c r="A1" s="19"/>
+      <c r="B1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="43" t="s">
         <v>45</v>
       </c>
       <c r="M1">
         <f>COUNTA(D2:D13)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="1" t="s">
+      <c r="N1" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="80">
+      <c r="B2" s="44">
         <v>6150</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="4">
         <v>8273</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="4">
         <v>8065</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="5">
         <f t="shared" ref="E2:E14" si="0">(C2-B2)/B2</f>
         <v>0.34520325203252034</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="6">
         <f t="shared" ref="F2:F10" si="1">(D2-C2)/D2</f>
         <v>-2.579045257284563E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="1" t="s">
+      <c r="N2" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="80">
+      <c r="B3" s="44">
         <v>6071</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="4">
         <v>7349</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="4">
         <v>6895</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="5">
         <f t="shared" si="0"/>
         <v>0.21050897710426619</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="6">
         <f t="shared" si="1"/>
         <v>-6.5844815083393765E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="1" t="s">
+      <c r="N3" s="23"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="80">
+      <c r="B4" s="44">
         <v>5579</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="4">
         <v>5620</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="14">
+      <c r="D4" s="4"/>
+      <c r="E4" s="5">
         <f t="shared" si="0"/>
         <v>7.3489872737049653E-3</v>
       </c>
-      <c r="F4" s="15" t="e">
+      <c r="F4" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="1" t="s">
+      <c r="N4" s="23"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="80">
+      <c r="B5" s="44">
         <v>5734</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="4">
         <v>8615</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="14">
+      <c r="D5" s="4"/>
+      <c r="E5" s="5">
         <f t="shared" si="0"/>
         <v>0.50244157656086497</v>
       </c>
-      <c r="F5" s="15" t="e">
+      <c r="F5" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="1" t="s">
+      <c r="N5" s="23"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="80">
+      <c r="B6" s="44">
         <v>6577</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="8">
         <v>10387</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="14">
+      <c r="D6" s="4"/>
+      <c r="E6" s="5">
         <f t="shared" si="0"/>
         <v>0.57929147027520145</v>
       </c>
-      <c r="F6" s="15" t="e">
+      <c r="F6" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="1" t="s">
+      <c r="N6" s="23"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="80">
+      <c r="B7" s="44">
         <v>7009</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="8">
         <v>8235</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="14">
+      <c r="D7" s="4"/>
+      <c r="E7" s="5">
         <f t="shared" si="0"/>
         <v>0.17491796261948922</v>
       </c>
-      <c r="F7" s="15" t="e">
+      <c r="F7" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="1" t="s">
+      <c r="N7" s="23"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="80">
+      <c r="B8" s="44">
         <v>6729</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="4">
         <v>7634</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="14">
+      <c r="D8" s="4"/>
+      <c r="E8" s="5">
         <f t="shared" si="0"/>
         <v>0.13449249517015902</v>
       </c>
-      <c r="F8" s="15" t="e">
+      <c r="F8" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="1" t="s">
+      <c r="N8" s="23"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="80">
+      <c r="B9" s="44">
         <v>8567</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="4">
         <v>8694</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="14">
+      <c r="D9" s="4"/>
+      <c r="E9" s="5">
         <f t="shared" si="0"/>
         <v>1.4824325901715887E-2</v>
       </c>
-      <c r="F9" s="15" t="e">
+      <c r="F9" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="1" t="s">
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="80">
+      <c r="B10" s="44">
         <v>8328</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="4">
         <v>7729</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="14">
+      <c r="D10" s="4"/>
+      <c r="E10" s="5">
         <f t="shared" si="0"/>
         <v>-7.1926032660902972E-2</v>
       </c>
-      <c r="F10" s="15" t="e">
+      <c r="F10" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="1" t="s">
+      <c r="N10" s="23"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="80">
+      <c r="B11" s="44">
         <v>8404</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="4">
         <v>8881</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="14">
+      <c r="D11" s="4"/>
+      <c r="E11" s="5">
         <f t="shared" si="0"/>
         <v>5.6758686339838174E-2</v>
       </c>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="1" t="s">
+      <c r="F11" s="6"/>
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="80">
+      <c r="B12" s="44">
         <v>8556</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="4">
         <v>8520</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="14">
+      <c r="D12" s="4"/>
+      <c r="E12" s="5">
         <f t="shared" si="0"/>
         <v>-4.2075736325385693E-3</v>
       </c>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="1" t="s">
+      <c r="F12" s="6"/>
+      <c r="N12" s="23"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="81">
+      <c r="B13" s="45">
         <v>8881</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="4">
         <v>6912</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="19">
+      <c r="D13" s="4"/>
+      <c r="E13" s="9">
         <f t="shared" si="0"/>
         <v>-0.22170926697443982</v>
       </c>
-      <c r="F13" s="15"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="23" t="s">
+      <c r="F13" s="6"/>
+      <c r="N13" s="23"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="82">
+      <c r="B14" s="46">
         <v>77704</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="12">
         <f>SUM(C2:C13)</f>
         <v>96849</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="12">
         <f>SUM(D2:D13)</f>
         <v>14960</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="13">
         <f t="shared" si="0"/>
         <v>0.24638371255019045</v>
       </c>
-      <c r="F14" s="27" t="e">
+      <c r="F14" s="14" t="e">
         <f>AVERAGE(F2:F13)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="43.2">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31" t="s">
+      <c r="N14" s="23"/>
+    </row>
+    <row r="15" spans="1:14" ht="57.6">
+      <c r="A15" s="47"/>
+      <c r="B15" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32" t="s">
+      <c r="D15" s="47"/>
+      <c r="E15" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="31"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="32"/>
-      <c r="B16" s="37">
+      <c r="F15" s="47"/>
+      <c r="N15" s="23"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="48"/>
+      <c r="B16" s="49">
         <v>81734</v>
       </c>
-      <c r="C16" s="37">
+      <c r="C16" s="49">
         <v>77704</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="38">
+      <c r="D16" s="47"/>
+      <c r="E16" s="50">
         <f>(C16-B16)/B16</f>
         <v>-4.9306286245626052E-2</v>
       </c>
-      <c r="F16" s="39"/>
+      <c r="F16" s="51"/>
+      <c r="N16" s="23"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="0U9HAsuYDx6Zuz7v5FnTeLJl3cv9OpiztPU3WvhzSoG1SBmxutKbkiu7C+DEzQ9p8VgS1OtdOEnoN0W1LL+rMA==" saltValue="eI13n4kNKH4QIf54y6oqxQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="N2:N16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -2156,366 +2330,396 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E42DFC87-E78F-46DC-B128-C26135CB7DA1}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="12" width="8.88671875" style="21"/>
+    <col min="13" max="13" width="15.5546875" style="21" customWidth="1"/>
+    <col min="14" max="14" width="33.109375" style="21" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="21"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="49.2">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:14" ht="66">
+      <c r="A1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="54" t="s">
         <v>36</v>
       </c>
       <c r="M1">
         <f>COUNTA(E2:E13)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="1" t="s">
+      <c r="N1" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="7">
         <v>1217</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="7">
         <v>224</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="6">
         <f t="shared" ref="D2:D14" si="0">(C2-B2)/B2</f>
         <v>-0.81594083812654072</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="4">
         <v>1493</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="6">
         <f t="shared" ref="F2:F7" si="1">(E2-C2)/C2</f>
         <v>5.6651785714285712</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="6">
         <f t="shared" ref="G2:G7" si="2">(E2-B2)/B2</f>
         <v>0.22678718159408381</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="1" t="s">
+      <c r="N2" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="7">
         <v>1518.25</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="7">
         <v>221</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="6">
         <f t="shared" si="0"/>
         <v>-0.85443767495471756</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="4">
         <v>1326</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="6">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="6">
         <f t="shared" si="2"/>
         <v>-0.12662604972830563</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="1" t="s">
+      <c r="N3" s="23"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="7">
         <v>1203.4000000000001</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="7">
         <v>203</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="6">
         <f t="shared" si="0"/>
         <v>-0.83131128469336879</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="4">
         <v>1014</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="6">
         <f t="shared" si="1"/>
         <v>3.9950738916256157</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="6">
         <f t="shared" si="2"/>
         <v>-0.15738740235998011</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="1" t="s">
+      <c r="N4" s="23"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="4">
         <v>1408</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="4">
         <v>1516</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="6">
         <f t="shared" si="0"/>
         <v>7.6704545454545456E-2</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="4">
         <v>2664</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="6">
         <f t="shared" si="1"/>
         <v>0.75725593667546176</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="6">
         <f t="shared" si="2"/>
         <v>0.89204545454545459</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="1" t="s">
+      <c r="N5" s="23"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="4">
         <v>1264</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="4">
         <v>1739</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="6">
         <f t="shared" si="0"/>
         <v>0.37579113924050633</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="8">
         <v>3212</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="6">
         <f t="shared" si="1"/>
         <v>0.84703852788959177</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="6">
         <f t="shared" si="2"/>
         <v>1.5411392405063291</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="1" t="s">
+      <c r="N6" s="23"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="4">
         <v>1139</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="4">
         <v>1853</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="6">
         <f t="shared" si="0"/>
         <v>0.62686567164179108</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="8">
         <v>2547</v>
       </c>
-      <c r="F7" s="57">
+      <c r="F7" s="55">
         <f t="shared" si="1"/>
         <v>0.37452779276848353</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="6">
         <f t="shared" si="2"/>
         <v>1.2361720807726075</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="1" t="s">
+      <c r="N7" s="23"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="4">
         <v>2496</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="4">
         <v>2137</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="6">
         <f t="shared" si="0"/>
         <v>-0.14383012820512819</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="15"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="1" t="s">
+      <c r="E8" s="4"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="6"/>
+      <c r="N8" s="23"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="4">
         <v>2298</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="4">
         <v>2842</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="6">
         <f t="shared" si="0"/>
         <v>0.23672758920800696</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="1" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="6"/>
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="4">
         <v>2263</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="4">
         <v>3066</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="6">
         <f t="shared" si="0"/>
         <v>0.35483870967741937</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="63"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="1" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="57"/>
+      <c r="N10" s="23"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="4">
         <v>2253</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="4">
         <v>3142</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="6">
         <f t="shared" si="0"/>
         <v>0.3945849977807368</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="15"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="1" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="6"/>
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="4">
         <v>2922</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="4">
         <v>3341</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="6">
         <f t="shared" si="0"/>
         <v>0.1433949349760438</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="65"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="1" t="s">
+      <c r="E12" s="4"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="58"/>
+      <c r="N12" s="23"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="8">
         <v>4402</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="8">
         <v>3233</v>
       </c>
-      <c r="D13" s="67">
+      <c r="D13" s="59">
         <f t="shared" si="0"/>
         <v>-0.26556110858700593</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="65"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="69" t="s">
+      <c r="E13" s="4"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="58"/>
+      <c r="N13" s="23"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="12">
         <f>SUM(B2:B13)</f>
         <v>24383.65</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="12">
         <f>SUM(C2:C13)</f>
         <v>23517</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="14">
         <f t="shared" si="0"/>
         <v>-3.554225884968007E-2</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="12">
         <f>SUM(E2:E13)</f>
         <v>12256</v>
       </c>
-      <c r="F14" s="70">
+      <c r="F14" s="62">
         <f>AVERAGE(F2:F13)</f>
         <v>2.7731791200646203</v>
       </c>
-      <c r="G14" s="70">
+      <c r="G14" s="62">
         <f>AVERAGE(G2:G13)</f>
         <v>0.60202175088836485</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="43.2">
-      <c r="A15" s="76"/>
-      <c r="B15" s="77" t="s">
+      <c r="N14" s="23"/>
+    </row>
+    <row r="15" spans="1:14" ht="57.6">
+      <c r="A15" s="63"/>
+      <c r="B15" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="77" t="s">
+      <c r="C15" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="11"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="76"/>
-      <c r="B16" s="78">
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="20"/>
+      <c r="N15" s="23"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="63"/>
+      <c r="B16" s="65">
         <v>23383</v>
       </c>
-      <c r="C16" s="78">
+      <c r="C16" s="65">
         <v>23517</v>
       </c>
-      <c r="D16" s="79">
+      <c r="D16" s="66">
         <f>(C16-B16)/B16</f>
         <v>5.7306590257879654E-3</v>
       </c>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="11"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="20"/>
+      <c r="N16" s="23"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="7DGr32luiVPnv71tQFu2CttWFgcsz+Vf7h08yNzVidP8H7KqcD+dIpuVeY+ZqNjQ9x3MKKt2f1165hfLPTu21Q==" saltValue="vFcumXZvguZZajLz2jBpyg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="N2:N16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -2526,594 +2730,607 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.5234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.20703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.41796875" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="21"/>
+    <col min="6" max="6" width="12" style="21" customWidth="1"/>
+    <col min="7" max="12" width="8.88671875" style="21"/>
+    <col min="13" max="13" width="14.77734375" style="21" customWidth="1"/>
+    <col min="14" max="14" width="33.5546875" style="21" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="61.5">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:14" ht="79.2">
+      <c r="A1" s="19"/>
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="4"/>
+      <c r="G1" s="69"/>
       <c r="M1">
         <f>COUNTA(D2:D13)</f>
         <v>2</v>
       </c>
-      <c r="N1" s="4"/>
+      <c r="N1" s="22" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="70">
         <v>381400</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="4">
         <v>358709</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="4">
         <v>292117</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="5">
         <f t="shared" ref="E2:F9" si="0">(C2-B2)/B2</f>
         <v>-5.9493969585736758E-2</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="5">
         <f t="shared" si="0"/>
         <v>-0.18564351605340262</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="G2" s="69"/>
+      <c r="N2" s="23" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="70">
         <v>338378</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="4">
         <v>320011</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="4">
         <v>257282</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="5">
         <f t="shared" si="0"/>
         <v>-5.4279533539414504E-2</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="5">
         <f t="shared" si="0"/>
         <v>-0.19602138676482997</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="G3" s="69"/>
+      <c r="N3" s="23"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="70">
         <v>354957</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="4">
         <v>323736</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="14">
+      <c r="D4" s="4"/>
+      <c r="E4" s="5">
         <f t="shared" si="0"/>
         <v>-8.7957132835808277E-2</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="5">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="N4" s="4"/>
+      <c r="G4" s="69"/>
+      <c r="N4" s="23"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="70">
         <v>329975</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="4">
         <v>307995</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="14">
+      <c r="D5" s="4"/>
+      <c r="E5" s="5">
         <f t="shared" si="0"/>
         <v>-6.6611106902038031E-2</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="5">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="G5" s="69"/>
+      <c r="N5" s="23"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="70">
         <v>333225</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="4">
         <v>305855</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="14">
+      <c r="D6" s="4"/>
+      <c r="E6" s="5">
         <f t="shared" si="0"/>
         <v>-8.2136694425688342E-2</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="5">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="G6" s="69"/>
+      <c r="N6" s="23"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="70">
         <v>319566</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="4">
         <v>289224</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="14">
+      <c r="D7" s="4"/>
+      <c r="E7" s="5">
         <f t="shared" si="0"/>
         <v>-9.4947522577495724E-2</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="5">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="N7" s="4"/>
+      <c r="G7" s="69"/>
+      <c r="N7" s="23"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="70">
         <v>345523</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="4">
         <v>304267</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="14">
+      <c r="D8" s="4"/>
+      <c r="E8" s="5">
         <f t="shared" si="0"/>
         <v>-0.11940160278765813</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="5">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="N8" s="4"/>
+      <c r="G8" s="69"/>
+      <c r="N8" s="23"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="70">
         <v>344469</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="4">
         <v>314709</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="14">
+      <c r="D9" s="4"/>
+      <c r="E9" s="5">
         <f t="shared" si="0"/>
         <v>-8.6393840955209328E-2</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="5">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="N9" s="4"/>
+      <c r="G9" s="69"/>
+      <c r="N9" s="23"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="4">
         <v>342330</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="4">
         <v>300248</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="14">
+      <c r="D10" s="4"/>
+      <c r="E10" s="5">
         <f>(C10-B10)/B10</f>
         <v>-0.12292816872608302</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="69"/>
+      <c r="N10" s="23"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="4">
         <v>367756</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="4">
         <v>303597</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="14">
+      <c r="D11" s="4"/>
+      <c r="E11" s="5">
         <f>(C11-B11)/B11</f>
         <v>-0.17446078378055016</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="4"/>
-      <c r="N11" s="4"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="69"/>
+      <c r="N11" s="23"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="4">
         <v>392032</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="4">
         <v>300258</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="14">
+      <c r="D12" s="4"/>
+      <c r="E12" s="5">
         <f>(C12-B12)/B12</f>
         <v>-0.23409823687862216</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="4"/>
-      <c r="N12" s="4"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="69"/>
+      <c r="N12" s="23"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="71">
         <v>415125</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="4">
         <v>316760</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="14">
+      <c r="D13" s="4"/>
+      <c r="E13" s="5">
         <f>(C13-B13)/B13</f>
         <v>-0.23695272508280638</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="4"/>
-      <c r="N13" s="22"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="69"/>
+      <c r="N13" s="23"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="11">
         <f>SUM(B2:B13)</f>
         <v>4264736</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="11">
         <f>SUM(C2:C13)</f>
         <v>3745369</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="11">
         <f>SUM(D2:D13)</f>
         <v>549399</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="13">
         <f>(C14-B14)/B14</f>
         <v>-0.12178174686545662</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="13">
         <f>AVERAGE(F2:F13)</f>
         <v>-0.79770811285227905</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="N14" s="4"/>
-    </row>
-    <row r="15" spans="1:14" ht="36.9">
-      <c r="A15" s="28"/>
-      <c r="B15" s="1" t="s">
+      <c r="G14" s="69"/>
+      <c r="N14" s="23"/>
+    </row>
+    <row r="15" spans="1:14" ht="52.8">
+      <c r="A15" s="72"/>
+      <c r="B15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="29" t="s">
+      <c r="D15" s="73"/>
+      <c r="E15" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="4"/>
-      <c r="N15" s="4"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="69"/>
+      <c r="M15" s="75"/>
+      <c r="N15" s="23"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="28"/>
-      <c r="B16" s="12">
+      <c r="A16" s="72"/>
+      <c r="B16" s="4">
         <v>4382326</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="4">
         <f>C14</f>
         <v>3745369</v>
       </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="14">
+      <c r="D16" s="4"/>
+      <c r="E16" s="5">
         <f>(C16-B16)/C16</f>
         <v>-0.17006521920804066</v>
       </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="4"/>
-      <c r="N16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="69"/>
+      <c r="M16" s="76"/>
+      <c r="N16" s="23"/>
     </row>
     <row r="17" spans="1:25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="11"/>
+      <c r="A17" s="72"/>
+      <c r="B17" s="72"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
+      <c r="K17" s="75"/>
+      <c r="L17" s="78"/>
+      <c r="N17" s="69"/>
+      <c r="O17" s="69"/>
+      <c r="P17" s="69"/>
+      <c r="Q17" s="69"/>
+      <c r="R17" s="69"/>
+      <c r="S17" s="69"/>
+      <c r="T17" s="69"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="20"/>
+      <c r="W17" s="20"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="20"/>
     </row>
     <row r="18" spans="1:25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="44"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="11"/>
-      <c r="V18" s="11"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="11"/>
+      <c r="A18" s="72"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="78"/>
+      <c r="K18" s="75"/>
+      <c r="L18" s="78"/>
+      <c r="N18" s="69"/>
+      <c r="O18" s="69"/>
+      <c r="P18" s="69"/>
+      <c r="Q18" s="69"/>
+      <c r="R18" s="69"/>
+      <c r="S18" s="69"/>
+      <c r="T18" s="69"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="20"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="20"/>
     </row>
     <row r="19" spans="1:25">
-      <c r="G19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="T19" s="33"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="11"/>
-      <c r="W19" s="11"/>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="11"/>
+      <c r="G19" s="69"/>
+      <c r="O19" s="69"/>
+      <c r="T19" s="28"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="20"/>
+      <c r="X19" s="20"/>
+      <c r="Y19" s="20"/>
     </row>
     <row r="20" spans="1:25">
-      <c r="G20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="T20" s="33"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11"/>
-      <c r="W20" s="11"/>
-      <c r="X20" s="11"/>
-      <c r="Y20" s="11"/>
+      <c r="G20" s="69"/>
+      <c r="O20" s="69"/>
+      <c r="T20" s="28"/>
+      <c r="U20" s="20"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="20"/>
     </row>
     <row r="21" spans="1:25">
-      <c r="G21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="T21" s="33"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
-      <c r="X21" s="11"/>
-      <c r="Y21" s="11"/>
+      <c r="G21" s="69"/>
+      <c r="O21" s="69"/>
+      <c r="T21" s="28"/>
+      <c r="U21" s="20"/>
+      <c r="V21" s="20"/>
+      <c r="W21" s="20"/>
+      <c r="X21" s="20"/>
+      <c r="Y21" s="20"/>
     </row>
     <row r="22" spans="1:25">
-      <c r="G22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="T22" s="33"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="11"/>
-      <c r="Y22" s="11"/>
+      <c r="G22" s="69"/>
+      <c r="O22" s="69"/>
+      <c r="T22" s="28"/>
+      <c r="U22" s="20"/>
+      <c r="V22" s="20"/>
+      <c r="W22" s="20"/>
+      <c r="X22" s="20"/>
+      <c r="Y22" s="20"/>
     </row>
     <row r="23" spans="1:25">
-      <c r="G23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="T23" s="33"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
-      <c r="Y23" s="11"/>
+      <c r="G23" s="69"/>
+      <c r="O23" s="69"/>
+      <c r="T23" s="28"/>
+      <c r="U23" s="20"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="20"/>
+      <c r="X23" s="20"/>
+      <c r="Y23" s="20"/>
     </row>
     <row r="24" spans="1:25">
-      <c r="G24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="T24" s="33"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="11"/>
+      <c r="G24" s="69"/>
+      <c r="O24" s="69"/>
+      <c r="T24" s="28"/>
+      <c r="U24" s="20"/>
+      <c r="V24" s="20"/>
+      <c r="W24" s="20"/>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="20"/>
     </row>
     <row r="25" spans="1:25">
-      <c r="G25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="T25" s="33"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11"/>
-      <c r="Y25" s="11"/>
+      <c r="G25" s="69"/>
+      <c r="O25" s="69"/>
+      <c r="T25" s="28"/>
+      <c r="U25" s="20"/>
+      <c r="V25" s="20"/>
+      <c r="W25" s="20"/>
+      <c r="X25" s="20"/>
+      <c r="Y25" s="20"/>
     </row>
     <row r="26" spans="1:25">
-      <c r="G26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="T26" s="61"/>
-      <c r="U26" s="11"/>
-      <c r="V26" s="11"/>
-      <c r="W26" s="11"/>
-      <c r="X26" s="11"/>
-      <c r="Y26" s="11"/>
+      <c r="G26" s="69"/>
+      <c r="O26" s="69"/>
+      <c r="T26" s="79"/>
+      <c r="U26" s="20"/>
+      <c r="V26" s="20"/>
+      <c r="W26" s="20"/>
+      <c r="X26" s="20"/>
+      <c r="Y26" s="20"/>
     </row>
     <row r="27" spans="1:25">
-      <c r="G27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="T27" s="62"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
+      <c r="G27" s="69"/>
+      <c r="O27" s="69"/>
+      <c r="T27" s="80"/>
+      <c r="U27" s="20"/>
+      <c r="V27" s="20"/>
+      <c r="W27" s="20"/>
+      <c r="X27" s="20"/>
+      <c r="Y27" s="20"/>
     </row>
     <row r="28" spans="1:25">
-      <c r="G28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="T28" s="33"/>
-      <c r="U28" s="11"/>
-      <c r="V28" s="11"/>
-      <c r="W28" s="11"/>
-      <c r="X28" s="11"/>
-      <c r="Y28" s="11"/>
+      <c r="G28" s="69"/>
+      <c r="O28" s="69"/>
+      <c r="T28" s="28"/>
+      <c r="U28" s="20"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="20"/>
+      <c r="X28" s="20"/>
+      <c r="Y28" s="20"/>
     </row>
     <row r="29" spans="1:25">
-      <c r="G29" s="28"/>
-      <c r="O29" s="4"/>
-      <c r="T29" s="61"/>
-      <c r="U29" s="11"/>
-      <c r="V29" s="11"/>
-      <c r="W29" s="11"/>
-      <c r="X29" s="11"/>
-      <c r="Y29" s="11"/>
+      <c r="G29" s="72"/>
+      <c r="O29" s="69"/>
+      <c r="T29" s="79"/>
+      <c r="U29" s="20"/>
+      <c r="V29" s="20"/>
+      <c r="W29" s="20"/>
+      <c r="X29" s="20"/>
+      <c r="Y29" s="20"/>
     </row>
     <row r="30" spans="1:25">
-      <c r="G30" s="64"/>
-      <c r="O30" s="11"/>
-      <c r="T30" s="66"/>
-      <c r="U30" s="11"/>
-      <c r="V30" s="11"/>
-      <c r="W30" s="11"/>
-      <c r="X30" s="11"/>
-      <c r="Y30" s="11"/>
+      <c r="G30" s="81"/>
+      <c r="O30" s="20"/>
+      <c r="T30" s="82"/>
+      <c r="U30" s="20"/>
+      <c r="V30" s="20"/>
+      <c r="W30" s="20"/>
+      <c r="X30" s="20"/>
+      <c r="Y30" s="20"/>
     </row>
     <row r="31" spans="1:25">
-      <c r="G31" s="64"/>
-      <c r="O31" s="11"/>
-      <c r="T31" s="66"/>
-      <c r="U31" s="11"/>
-      <c r="V31" s="11"/>
-      <c r="W31" s="11"/>
-      <c r="X31" s="11"/>
-      <c r="Y31" s="11"/>
+      <c r="G31" s="81"/>
+      <c r="O31" s="20"/>
+      <c r="T31" s="82"/>
+      <c r="U31" s="20"/>
+      <c r="V31" s="20"/>
+      <c r="W31" s="20"/>
+      <c r="X31" s="20"/>
+      <c r="Y31" s="20"/>
     </row>
     <row r="32" spans="1:25">
-      <c r="G32" s="64"/>
-      <c r="O32" s="11"/>
-      <c r="T32" s="66"/>
-      <c r="U32" s="11"/>
-      <c r="V32" s="11"/>
-      <c r="W32" s="11"/>
-      <c r="X32" s="11"/>
-      <c r="Y32" s="11"/>
+      <c r="G32" s="81"/>
+      <c r="O32" s="20"/>
+      <c r="T32" s="82"/>
+      <c r="U32" s="20"/>
+      <c r="V32" s="20"/>
+      <c r="W32" s="20"/>
+      <c r="X32" s="20"/>
+      <c r="Y32" s="20"/>
     </row>
     <row r="33" spans="1:25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="64"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="11"/>
-      <c r="U33" s="11"/>
-      <c r="V33" s="11"/>
-      <c r="W33" s="11"/>
-      <c r="X33" s="11"/>
-      <c r="Y33" s="11"/>
+      <c r="A33" s="72"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="83"/>
+      <c r="E33" s="84"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="81"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="20"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="20"/>
+      <c r="S33" s="20"/>
+      <c r="T33" s="20"/>
+      <c r="U33" s="20"/>
+      <c r="V33" s="20"/>
+      <c r="W33" s="20"/>
+      <c r="X33" s="20"/>
+      <c r="Y33" s="20"/>
     </row>
     <row r="34" spans="1:25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="64"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="11"/>
-      <c r="S34" s="11"/>
-      <c r="T34" s="11"/>
-      <c r="U34" s="11"/>
-      <c r="V34" s="11"/>
-      <c r="W34" s="11"/>
-      <c r="X34" s="11"/>
-      <c r="Y34" s="11"/>
+      <c r="A34" s="72"/>
+      <c r="B34" s="78"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="81"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="20"/>
+      <c r="S34" s="20"/>
+      <c r="T34" s="20"/>
+      <c r="U34" s="20"/>
+      <c r="V34" s="20"/>
+      <c r="W34" s="20"/>
+      <c r="X34" s="20"/>
+      <c r="Y34" s="20"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="LtYAETV0sF6s+k/w5V56PCUFAGy33oaKSDKyfqodzJpDYWSxXKLRIIJo/uX4zzAGqncW7fY3+y8vbOk5yj8jWQ==" saltValue="g2v0t8nvFiPWHfh+yOHjQQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="N2:N16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -3121,312 +3338,345 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327A2756-5D85-4831-B939-ADBAF297377F}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.5234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.20703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.20703125" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.21875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="21"/>
+    <col min="6" max="6" width="11" style="21" customWidth="1"/>
+    <col min="7" max="12" width="8.88671875" style="21"/>
+    <col min="13" max="13" width="17" style="21" customWidth="1"/>
+    <col min="14" max="14" width="33.6640625" style="21" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="49.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:14" ht="52.8">
+      <c r="A1" s="19"/>
+      <c r="B1" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="85" t="s">
         <v>3</v>
       </c>
       <c r="M1">
         <f>COUNTA(D2:D13)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="1" t="s">
+      <c r="N1" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="52">
+      <c r="B2" s="86">
         <v>166018</v>
       </c>
-      <c r="C2" s="52">
+      <c r="C2" s="86">
         <v>154290</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="4">
         <v>137349</v>
       </c>
-      <c r="E2" s="53">
+      <c r="E2" s="87">
         <f t="shared" ref="E2:F9" si="0">(C2-B2)/B2</f>
         <v>-7.0642942331554409E-2</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="5">
         <f t="shared" si="0"/>
         <v>-0.10979972778533929</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="1" t="s">
+      <c r="N2" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="56">
+      <c r="B3" s="88">
         <v>153234</v>
       </c>
-      <c r="C3" s="52">
+      <c r="C3" s="86">
         <v>139138</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="4">
         <v>126757</v>
       </c>
-      <c r="E3" s="53">
+      <c r="E3" s="87">
         <f t="shared" si="0"/>
         <v>-9.199002832269601E-2</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="5">
         <f t="shared" si="0"/>
         <v>-8.8983599016803458E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="1" t="s">
+      <c r="N3" s="23"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="52">
+      <c r="B4" s="86">
         <v>149129</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="86">
         <v>139609</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="4">
         <v>117550</v>
       </c>
-      <c r="E4" s="53">
+      <c r="E4" s="87">
         <f t="shared" si="0"/>
         <v>-6.3837348872452709E-2</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="5">
         <f t="shared" si="0"/>
         <v>-0.15800557270663065</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="1" t="s">
+      <c r="N4" s="23"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="52">
+      <c r="B5" s="86">
         <v>146506</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C5" s="86">
         <v>126227</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="4">
         <v>113477</v>
       </c>
-      <c r="E5" s="53">
+      <c r="E5" s="87">
         <f t="shared" si="0"/>
         <v>-0.13841753921341104</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="5">
         <f t="shared" si="0"/>
         <v>-0.10100850055851759</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="1" t="s">
+      <c r="N5" s="23"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="52">
+      <c r="B6" s="86">
         <v>122937</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="86">
         <v>128749</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="4">
         <v>108336</v>
       </c>
-      <c r="E6" s="53">
+      <c r="E6" s="87">
         <f t="shared" si="0"/>
         <v>4.7276247183516758E-2</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="5">
         <f t="shared" si="0"/>
         <v>-0.15854880426255738</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="1" t="s">
+      <c r="N6" s="23"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="52">
+      <c r="B7" s="86">
         <v>113710</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="86">
         <v>125671</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="4">
         <v>98523</v>
       </c>
-      <c r="E7" s="53">
+      <c r="E7" s="87">
         <f t="shared" si="0"/>
         <v>0.10518863776272976</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="5">
         <f t="shared" si="0"/>
         <v>-0.21602438112213637</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="1" t="s">
+      <c r="N7" s="23"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="52">
+      <c r="B8" s="86">
         <v>117122</v>
       </c>
-      <c r="C8" s="52">
+      <c r="C8" s="86">
         <v>147302</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="4">
         <v>103029</v>
       </c>
-      <c r="E8" s="53">
+      <c r="E8" s="87">
         <f t="shared" si="0"/>
         <v>0.25768002595584094</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="5">
         <f t="shared" si="0"/>
         <v>-0.30055939498445372</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="1" t="s">
+      <c r="N8" s="23"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="52">
+      <c r="B9" s="86">
         <v>126623</v>
       </c>
-      <c r="C9" s="52">
+      <c r="C9" s="86">
         <v>145461</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="4">
         <v>115694</v>
       </c>
-      <c r="E9" s="53">
+      <c r="E9" s="87">
         <f t="shared" si="0"/>
         <v>0.14877233993824188</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="5">
         <f t="shared" si="0"/>
         <v>-0.20463904414241618</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="1" t="s">
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="52">
+      <c r="B10" s="86">
         <v>122360</v>
       </c>
-      <c r="C10" s="52">
+      <c r="C10" s="86">
         <v>149470</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="53">
+      <c r="D10" s="4"/>
+      <c r="E10" s="87">
         <f>(C10-B10)/B10</f>
         <v>0.22155933311539719</v>
       </c>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="1" t="s">
+      <c r="F10" s="5"/>
+      <c r="N10" s="23"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="52">
+      <c r="B11" s="86">
         <v>132280</v>
       </c>
-      <c r="C11" s="52">
+      <c r="C11" s="86">
         <v>165507</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="53">
+      <c r="D11" s="4"/>
+      <c r="E11" s="87">
         <f>(C11-B11)/B11</f>
         <v>0.25118687632295134</v>
       </c>
-      <c r="F11" s="14"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="1" t="s">
+      <c r="F11" s="5"/>
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="52">
+      <c r="B12" s="86">
         <v>128303</v>
       </c>
-      <c r="C12" s="52">
+      <c r="C12" s="86">
         <v>162736</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="53">
+      <c r="D12" s="4"/>
+      <c r="E12" s="87">
         <f>(C12-B12)/B12</f>
         <v>0.2683725244148617</v>
       </c>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="1" t="s">
+      <c r="F12" s="5"/>
+      <c r="N12" s="23"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="52">
+      <c r="B13" s="86">
         <v>132120</v>
       </c>
-      <c r="C13" s="52">
+      <c r="C13" s="86">
         <v>165619</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="53">
+      <c r="D13" s="4"/>
+      <c r="E13" s="87">
         <f>(C13-B13)/B13</f>
         <v>0.25354980320920373</v>
       </c>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="23" t="s">
+      <c r="F13" s="5"/>
+      <c r="N13" s="23"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="11">
         <f>SUM(B2:B13)</f>
         <v>1610342</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="11">
         <f>SUM(C2:C13)</f>
         <v>1749779</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="11">
         <f>SUM(D2:D13)</f>
         <v>920715</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="13">
         <f>(C14-B14)/B14</f>
         <v>8.6588438977558801E-2</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="13">
         <f>AVERAGE(F2:F13)</f>
         <v>-0.16719612807235684</v>
       </c>
+      <c r="N14" s="23"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="N15" s="23"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="N16" s="23"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="HOLRtgJpW0u/R9b0hVJpboOeEEDkGbF0Kqf4wAZxseaf//yp+NnFVo4j4uJT/QnnPZJeeF1xlpoEuYs0ZttsWA==" saltValue="AAuuy3hONqvmSqQTNXV/iA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="N2:N16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -3434,407 +3684,436 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116C5861-0548-4071-B9F1-0FF3651A304B}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5234375" customWidth="1"/>
-    <col min="5" max="5" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5234375" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="21"/>
+    <col min="2" max="3" width="14.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" style="21" customWidth="1"/>
+    <col min="7" max="9" width="8.88671875" style="21"/>
+    <col min="10" max="10" width="9.109375" style="21" customWidth="1"/>
+    <col min="11" max="12" width="8.88671875" style="21"/>
+    <col min="13" max="13" width="15.88671875" style="21" customWidth="1"/>
+    <col min="14" max="14" width="32.44140625" style="21" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="36.9">
-      <c r="A1" s="1"/>
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:14" ht="39.6">
+      <c r="A1" s="19"/>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
       <c r="M1">
         <f>COUNTA(D2:D13)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="1" t="s">
+      <c r="N1" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="4">
         <v>40365</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="4">
         <v>41888</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="4">
         <v>46250</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="5">
         <f t="shared" ref="E2:F9" si="0">(C2-B2)/B2</f>
         <v>3.773070729592469E-2</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="6">
         <f t="shared" si="0"/>
         <v>0.10413483575248281</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="1" t="s">
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="N2" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="4">
         <v>37545</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="7">
         <v>50219</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="4">
         <v>33335</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="5">
         <f t="shared" si="0"/>
         <v>0.3375682514316154</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="6">
         <f t="shared" si="0"/>
         <v>-0.33620741153746592</v>
       </c>
-      <c r="G3" s="83" t="s">
+      <c r="G3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="1" t="s">
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="N3" s="23"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="4">
         <v>25781.81</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="7">
         <v>45023</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="14">
+      <c r="D4" s="4"/>
+      <c r="E4" s="5">
         <f t="shared" si="0"/>
         <v>0.74630873472421055</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="6">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="1" t="s">
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="N4" s="23"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="4">
         <v>25781.81</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="7">
         <v>25839</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="14">
+      <c r="D5" s="4"/>
+      <c r="E5" s="5">
         <f t="shared" si="0"/>
         <v>2.2182306052212272E-3</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="6">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="1" t="s">
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="N5" s="23"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="4">
         <v>13432.28</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="7">
         <v>12769</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="14">
+      <c r="D6" s="4"/>
+      <c r="E6" s="5">
         <f t="shared" si="0"/>
         <v>-4.9379554327336879E-2</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="6">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="1" t="s">
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="N6" s="23"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="4">
         <v>15430.56</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="7">
         <v>10444</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="14">
+      <c r="D7" s="4"/>
+      <c r="E7" s="5">
         <f t="shared" si="0"/>
         <v>-0.32316131106064844</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="6">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="1" t="s">
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="N7" s="23"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="4">
         <v>7210.53</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="4">
         <v>9191</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="14">
+      <c r="D8" s="4"/>
+      <c r="E8" s="5">
         <f t="shared" si="0"/>
         <v>0.27466358228868065</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="6">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="1" t="s">
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="N8" s="23"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="4">
         <v>7045.99</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="4">
         <v>11379</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="14">
+      <c r="D9" s="4"/>
+      <c r="E9" s="5">
         <f t="shared" si="0"/>
         <v>0.61496113392156393</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="6">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="18" t="s">
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="8">
         <v>23032</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="4">
         <v>11779</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="19">
+      <c r="D10" s="4"/>
+      <c r="E10" s="9">
         <f>(C10-B10)/B10</f>
         <v>-0.48858110455019105</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="18" t="s">
+      <c r="F10" s="6"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="N10" s="23"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="8">
         <v>36770</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="4">
         <v>23418</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="19">
+      <c r="D11" s="4"/>
+      <c r="E11" s="9">
         <f>(C11-B11)/B11</f>
         <v>-0.3631221104161001</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="18" t="s">
+      <c r="F11" s="6"/>
+      <c r="G11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="8">
         <v>40381</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="4">
         <v>34717</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="19">
+      <c r="D12" s="4"/>
+      <c r="E12" s="9">
         <f>(C12-B12)/B12</f>
         <v>-0.14026398553775291</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="1" t="s">
+      <c r="F12" s="6"/>
+      <c r="G12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="N12" s="23"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="10">
         <v>34355</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="4">
         <v>36455</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="14">
+      <c r="D13" s="4"/>
+      <c r="E13" s="5">
         <f>(C13-B13)/B13</f>
         <v>6.1126473584631059E-2</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="23" t="s">
+      <c r="F13" s="6"/>
+      <c r="G13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="N13" s="23"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="11">
         <f>SUM(B2:B13)</f>
         <v>307130.98</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="11">
         <f>SUM(C2:C13)</f>
         <v>313121</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="12">
         <f>SUM(D2:D13)</f>
         <v>79585</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="13">
         <f>(C14-B14)/B14</f>
         <v>1.9503144879751366E-2</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="14">
         <f>AVERAGE(F2:F13)</f>
         <v>-0.77900907197312286</v>
       </c>
-      <c r="G14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-    </row>
-    <row r="15" spans="1:13" ht="24.6">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34" t="s">
+      <c r="G14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="N14" s="23"/>
+    </row>
+    <row r="15" spans="1:14" ht="26.4">
+      <c r="A15" s="28"/>
+      <c r="B15" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="35" t="s">
+      <c r="D15" s="15"/>
+      <c r="E15" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="36"/>
-      <c r="G15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="33"/>
-      <c r="B16" s="40">
+      <c r="F15" s="17"/>
+      <c r="G15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="N15" s="23"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="28"/>
+      <c r="B16" s="18">
         <v>331445.11</v>
       </c>
-      <c r="C16" s="40">
+      <c r="C16" s="18">
         <v>272775.98</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="15">
+      <c r="D16" s="15"/>
+      <c r="E16" s="6">
         <f>(C16-B16)/C16</f>
         <v>-0.2150817311700246</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="N16" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <sheetProtection algorithmName="SHA-512" hashValue="szcWKy50EcSI7AzlOvmrgYkTpjEMkMI3My+EHw1R2YFiqpS8FQLKM/JNzLzV5Zgi1oK3eXmS2ug0HJ+GuGkpfA==" saltValue="LkFVj7kPGLLTrdsUBzaurg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="2">
     <mergeCell ref="G3:K3"/>
+    <mergeCell ref="N2:N16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Remove slide hiding, add annotations for when consumption is up
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Waste" sheetId="1" state="visible" r:id="rId2"/>
@@ -725,7 +725,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="60">
   <si>
     <t xml:space="preserve">Waste</t>
   </si>
@@ -784,6 +784,9 @@
     <t xml:space="preserve">Total</t>
   </si>
   <si>
+    <t xml:space="preserve">Nothing to report? Here’s a default fun fact:</t>
+  </si>
+  <si>
     <t xml:space="preserve">Water 2017 (M3)</t>
   </si>
   <si>
@@ -799,6 +802,9 @@
     <t xml:space="preserve">Percentage Difference Vs last year</t>
   </si>
   <si>
+    <t xml:space="preserve">Top Tip!</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cabot Circus uses state-of-the-art rainwater harvesting technology, which helps reduce water waste!</t>
   </si>
   <si>
@@ -853,6 +859,9 @@
     <t xml:space="preserve">Percentage Difference Vs Last Year</t>
   </si>
   <si>
+    <t xml:space="preserve">We’ve seen the light.</t>
+  </si>
+  <si>
     <t xml:space="preserve">In 2018, we replaced our car park's lights with LEDs. This will save around 1,500,000 kWh a year!</t>
   </si>
   <si>
@@ -880,16 +889,22 @@
     <t xml:space="preserve">Gas 2019 (kWh)</t>
   </si>
   <si>
+    <t xml:space="preserve">This month, we’re up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We always strive to be transparent with our customers. This month, we’re up for our gas usage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reporting on invoice consumption not meter reads.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015 Gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017 Gas</t>
+  </si>
+  <si>
     <t xml:space="preserve">Using a machine known as an anaerobic digester, we convert tons of food waste back into energy!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reporting on invoice consumption not meter reads.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015 Gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017 Gas</t>
   </si>
 </sst>
 </file>
@@ -906,7 +921,7 @@
     <numFmt numFmtId="170" formatCode="0.00%"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -931,13 +946,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -954,6 +969,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1120,7 +1143,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1146,15 +1169,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="81">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1163,15 +1182,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1179,15 +1198,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1195,15 +1214,15 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1219,55 +1238,59 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="5" borderId="2" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="5" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1275,15 +1298,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1291,35 +1310,31 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="7" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1331,172 +1346,167 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="5" fillId="10" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="10" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="3" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="4" fillId="10" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="11" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="5" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 14" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="nullCell" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1566,10 +1576,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q13" activeCellId="0" sqref="Q13"/>
+      <selection pane="topLeft" activeCell="S15" activeCellId="0" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1776,6 +1786,36 @@
       </c>
       <c r="N14" s="9"/>
     </row>
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N17" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N18" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="1">
@@ -1796,10 +1836,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1811,44 +1851,44 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="79.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16"/>
-      <c r="B1" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="18" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>23</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>24</v>
       </c>
       <c r="M1" s="1" t="n">
         <f aca="false">COUNTA(D2:D13)</f>
         <v>2</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="21" t="n">
+      <c r="B2" s="22" t="n">
         <v>6150</v>
       </c>
-      <c r="C2" s="22" t="n">
+      <c r="C2" s="23" t="n">
         <v>8273</v>
       </c>
-      <c r="D2" s="22" t="n">
+      <c r="D2" s="23" t="n">
         <v>8065</v>
       </c>
-      <c r="E2" s="23" t="n">
+      <c r="E2" s="24" t="n">
         <f aca="false">(C2-B2)/B2</f>
         <v>0.34520325203252</v>
       </c>
@@ -1857,23 +1897,23 @@
         <v>-0.0257904525728456</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="21" t="n">
+      <c r="B3" s="22" t="n">
         <v>6071</v>
       </c>
-      <c r="C3" s="22" t="n">
+      <c r="C3" s="23" t="n">
         <v>7349</v>
       </c>
-      <c r="D3" s="22" t="n">
+      <c r="D3" s="23" t="n">
         <v>6895</v>
       </c>
-      <c r="E3" s="23" t="n">
+      <c r="E3" s="24" t="n">
         <f aca="false">(C3-B3)/B3</f>
         <v>0.210508977104266</v>
       </c>
@@ -1884,17 +1924,17 @@
       <c r="N3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="21" t="n">
+      <c r="B4" s="22" t="n">
         <v>5579</v>
       </c>
-      <c r="C4" s="22" t="n">
+      <c r="C4" s="23" t="n">
         <v>5620</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23" t="n">
+      <c r="D4" s="23"/>
+      <c r="E4" s="24" t="n">
         <f aca="false">(C4-B4)/B4</f>
         <v>0.00734898727370497</v>
       </c>
@@ -1905,17 +1945,17 @@
       <c r="N4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="21" t="n">
+      <c r="B5" s="22" t="n">
         <v>5734</v>
       </c>
-      <c r="C5" s="22" t="n">
+      <c r="C5" s="23" t="n">
         <v>8615</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23" t="n">
+      <c r="D5" s="23"/>
+      <c r="E5" s="24" t="n">
         <f aca="false">(C5-B5)/B5</f>
         <v>0.502441576560865</v>
       </c>
@@ -1926,17 +1966,17 @@
       <c r="N5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="21" t="n">
+      <c r="B6" s="22" t="n">
         <v>6577</v>
       </c>
-      <c r="C6" s="24" t="n">
+      <c r="C6" s="25" t="n">
         <v>10387</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23" t="n">
+      <c r="D6" s="23"/>
+      <c r="E6" s="24" t="n">
         <f aca="false">(C6-B6)/B6</f>
         <v>0.579291470275201</v>
       </c>
@@ -1947,17 +1987,17 @@
       <c r="N6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="21" t="n">
+      <c r="B7" s="22" t="n">
         <v>7009</v>
       </c>
-      <c r="C7" s="24" t="n">
+      <c r="C7" s="25" t="n">
         <v>8235</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23" t="n">
+      <c r="D7" s="23"/>
+      <c r="E7" s="24" t="n">
         <f aca="false">(C7-B7)/B7</f>
         <v>0.174917962619489</v>
       </c>
@@ -1968,17 +2008,17 @@
       <c r="N7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="21" t="n">
+      <c r="B8" s="22" t="n">
         <v>6729</v>
       </c>
-      <c r="C8" s="22" t="n">
+      <c r="C8" s="23" t="n">
         <v>7634</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23" t="n">
+      <c r="D8" s="23"/>
+      <c r="E8" s="24" t="n">
         <f aca="false">(C8-B8)/B8</f>
         <v>0.134492495170159</v>
       </c>
@@ -1989,17 +2029,17 @@
       <c r="N8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="21" t="n">
+      <c r="B9" s="22" t="n">
         <v>8567</v>
       </c>
-      <c r="C9" s="22" t="n">
+      <c r="C9" s="23" t="n">
         <v>8694</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23" t="n">
+      <c r="D9" s="23"/>
+      <c r="E9" s="24" t="n">
         <f aca="false">(C9-B9)/B9</f>
         <v>0.0148243259017159</v>
       </c>
@@ -2010,17 +2050,17 @@
       <c r="N9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="21" t="n">
+      <c r="B10" s="22" t="n">
         <v>8328</v>
       </c>
-      <c r="C10" s="22" t="n">
+      <c r="C10" s="23" t="n">
         <v>7729</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23" t="n">
+      <c r="D10" s="23"/>
+      <c r="E10" s="24" t="n">
         <f aca="false">(C10-B10)/B10</f>
         <v>-0.071926032660903</v>
       </c>
@@ -2031,17 +2071,17 @@
       <c r="N10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="21" t="n">
+      <c r="B11" s="22" t="n">
         <v>8404</v>
       </c>
-      <c r="C11" s="22" t="n">
+      <c r="C11" s="23" t="n">
         <v>8881</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23" t="n">
+      <c r="D11" s="23"/>
+      <c r="E11" s="24" t="n">
         <f aca="false">(C11-B11)/B11</f>
         <v>0.0567586863398382</v>
       </c>
@@ -2049,17 +2089,17 @@
       <c r="N11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="21" t="n">
+      <c r="B12" s="22" t="n">
         <v>8556</v>
       </c>
-      <c r="C12" s="22" t="n">
+      <c r="C12" s="23" t="n">
         <v>8520</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23" t="n">
+      <c r="D12" s="23"/>
+      <c r="E12" s="24" t="n">
         <f aca="false">(C12-B12)/B12</f>
         <v>-0.00420757363253857</v>
       </c>
@@ -2067,17 +2107,17 @@
       <c r="N12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="25" t="n">
+      <c r="B13" s="26" t="n">
         <v>8881</v>
       </c>
-      <c r="C13" s="22" t="n">
+      <c r="C13" s="23" t="n">
         <v>6912</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="26" t="n">
+      <c r="D13" s="23"/>
+      <c r="E13" s="27" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>-0.22170926697444</v>
       </c>
@@ -2085,61 +2125,85 @@
       <c r="N13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="28" t="n">
+      <c r="B14" s="29" t="n">
         <v>77704</v>
       </c>
-      <c r="C14" s="29" t="n">
+      <c r="C14" s="30" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>96849</v>
       </c>
-      <c r="D14" s="29" t="n">
+      <c r="D14" s="30" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>14960</v>
       </c>
-      <c r="E14" s="30" t="n">
+      <c r="E14" s="31" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>0.24638371255019</v>
       </c>
-      <c r="F14" s="31" t="e">
+      <c r="F14" s="32" t="e">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="32"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="17"/>
       <c r="E15" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="32"/>
+        <v>29</v>
+      </c>
+      <c r="F15" s="17"/>
       <c r="N15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="33"/>
-      <c r="B16" s="34" t="n">
+      <c r="B16" s="23" t="n">
         <v>81734</v>
       </c>
-      <c r="C16" s="34" t="n">
+      <c r="C16" s="23" t="n">
         <v>77704</v>
       </c>
-      <c r="D16" s="32"/>
-      <c r="E16" s="35" t="n">
+      <c r="D16" s="17"/>
+      <c r="E16" s="34" t="n">
         <f aca="false">(C16-B16)/B16</f>
         <v>-0.0493062862456261</v>
       </c>
-      <c r="F16" s="36"/>
+      <c r="F16" s="35"/>
       <c r="N16" s="9"/>
     </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N17" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N18" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="1">
@@ -2176,26 +2240,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="38" t="s">
+      <c r="A1" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="C1" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="D1" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="E1" s="37" t="s">
         <v>34</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>36</v>
       </c>
       <c r="M1" s="1" t="n">
         <f aca="false">COUNTA(E2:E13)</f>
@@ -2204,20 +2268,20 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="41" t="n">
+      <c r="B2" s="40" t="n">
         <v>1217</v>
       </c>
-      <c r="C2" s="41" t="n">
+      <c r="C2" s="40" t="n">
         <v>224</v>
       </c>
       <c r="D2" s="8" t="n">
         <f aca="false">(C2-B2)/B2</f>
         <v>-0.815940838126541</v>
       </c>
-      <c r="E2" s="22" t="n">
+      <c r="E2" s="23" t="n">
         <v>1493</v>
       </c>
       <c r="F2" s="8" t="n">
@@ -2228,23 +2292,23 @@
         <f aca="false">(E2-B2)/B2</f>
         <v>0.226787181594084</v>
       </c>
-      <c r="N2" s="42"/>
+      <c r="N2" s="41"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="41" t="n">
+      <c r="B3" s="40" t="n">
         <v>1518.25</v>
       </c>
-      <c r="C3" s="41" t="n">
+      <c r="C3" s="40" t="n">
         <v>221</v>
       </c>
       <c r="D3" s="8" t="n">
         <f aca="false">(C3-B3)/B3</f>
         <v>-0.854437674954717</v>
       </c>
-      <c r="E3" s="22" t="n">
+      <c r="E3" s="23" t="n">
         <v>1326</v>
       </c>
       <c r="F3" s="8" t="n">
@@ -2255,23 +2319,23 @@
         <f aca="false">(E3-B3)/B3</f>
         <v>-0.126626049728306</v>
       </c>
-      <c r="N3" s="43"/>
+      <c r="N3" s="42"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="41" t="n">
+      <c r="B4" s="40" t="n">
         <v>1203.4</v>
       </c>
-      <c r="C4" s="41" t="n">
+      <c r="C4" s="40" t="n">
         <v>203</v>
       </c>
       <c r="D4" s="8" t="n">
         <f aca="false">(C4-B4)/B4</f>
         <v>-0.831311284693369</v>
       </c>
-      <c r="E4" s="22" t="n">
+      <c r="E4" s="23" t="n">
         <v>1014</v>
       </c>
       <c r="F4" s="8" t="n">
@@ -2282,23 +2346,23 @@
         <f aca="false">(E4-B4)/B4</f>
         <v>-0.15738740235998</v>
       </c>
-      <c r="N4" s="43"/>
+      <c r="N4" s="42"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="22" t="n">
+      <c r="B5" s="23" t="n">
         <v>1408</v>
       </c>
-      <c r="C5" s="22" t="n">
+      <c r="C5" s="23" t="n">
         <v>1516</v>
       </c>
       <c r="D5" s="8" t="n">
         <f aca="false">(C5-B5)/B5</f>
         <v>0.0767045454545455</v>
       </c>
-      <c r="E5" s="22" t="n">
+      <c r="E5" s="23" t="n">
         <v>2664</v>
       </c>
       <c r="F5" s="8" t="n">
@@ -2309,23 +2373,23 @@
         <f aca="false">(E5-B5)/B5</f>
         <v>0.892045454545455</v>
       </c>
-      <c r="N5" s="43"/>
+      <c r="N5" s="42"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="22" t="n">
+      <c r="B6" s="23" t="n">
         <v>1264</v>
       </c>
-      <c r="C6" s="22" t="n">
+      <c r="C6" s="23" t="n">
         <v>1739</v>
       </c>
       <c r="D6" s="8" t="n">
         <f aca="false">(C6-B6)/B6</f>
         <v>0.375791139240506</v>
       </c>
-      <c r="E6" s="24" t="n">
+      <c r="E6" s="25" t="n">
         <v>3212</v>
       </c>
       <c r="F6" s="8" t="n">
@@ -2336,26 +2400,26 @@
         <f aca="false">(E6-B6)/B6</f>
         <v>1.54113924050633</v>
       </c>
-      <c r="N6" s="43"/>
+      <c r="N6" s="42"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="22" t="n">
+      <c r="B7" s="23" t="n">
         <v>1139</v>
       </c>
-      <c r="C7" s="22" t="n">
+      <c r="C7" s="23" t="n">
         <v>1853</v>
       </c>
       <c r="D7" s="8" t="n">
         <f aca="false">(C7-B7)/B7</f>
         <v>0.626865671641791</v>
       </c>
-      <c r="E7" s="24" t="n">
+      <c r="E7" s="25" t="n">
         <v>2547</v>
       </c>
-      <c r="F7" s="44" t="n">
+      <c r="F7" s="43" t="n">
         <f aca="false">(E7-C7)/C7</f>
         <v>0.374527792768483</v>
       </c>
@@ -2363,184 +2427,184 @@
         <f aca="false">(E7-B7)/B7</f>
         <v>1.23617208077261</v>
       </c>
-      <c r="N7" s="43"/>
+      <c r="N7" s="42"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="22" t="n">
+      <c r="B8" s="23" t="n">
         <v>2496</v>
       </c>
-      <c r="C8" s="22" t="n">
+      <c r="C8" s="23" t="n">
         <v>2137</v>
       </c>
       <c r="D8" s="8" t="n">
         <f aca="false">(C8-B8)/B8</f>
         <v>-0.143830128205128</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="45"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="44"/>
       <c r="G8" s="8"/>
-      <c r="N8" s="43"/>
+      <c r="N8" s="42"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="22" t="n">
+      <c r="B9" s="23" t="n">
         <v>2298</v>
       </c>
-      <c r="C9" s="22" t="n">
+      <c r="C9" s="23" t="n">
         <v>2842</v>
       </c>
       <c r="D9" s="8" t="n">
         <f aca="false">(C9-B9)/B9</f>
         <v>0.236727589208007</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="45"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="44"/>
       <c r="G9" s="8"/>
-      <c r="N9" s="43"/>
+      <c r="N9" s="42"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="22" t="n">
+      <c r="B10" s="23" t="n">
         <v>2263</v>
       </c>
-      <c r="C10" s="22" t="n">
+      <c r="C10" s="23" t="n">
         <v>3066</v>
       </c>
       <c r="D10" s="8" t="n">
         <f aca="false">(C10-B10)/B10</f>
         <v>0.354838709677419</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="46"/>
-      <c r="N10" s="43"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="45"/>
+      <c r="N10" s="42"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="22" t="n">
+      <c r="B11" s="23" t="n">
         <v>2253</v>
       </c>
-      <c r="C11" s="22" t="n">
+      <c r="C11" s="23" t="n">
         <v>3142</v>
       </c>
       <c r="D11" s="8" t="n">
         <f aca="false">(C11-B11)/B11</f>
         <v>0.394584997780737</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="45"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="44"/>
       <c r="G11" s="8"/>
-      <c r="N11" s="43"/>
+      <c r="N11" s="42"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="22" t="n">
+      <c r="B12" s="23" t="n">
         <v>2922</v>
       </c>
-      <c r="C12" s="22" t="n">
+      <c r="C12" s="23" t="n">
         <v>3341</v>
       </c>
       <c r="D12" s="8" t="n">
         <f aca="false">(C12-B12)/B12</f>
         <v>0.143394934976044</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="47"/>
-      <c r="N12" s="43"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="46"/>
+      <c r="N12" s="42"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="24" t="n">
+      <c r="B13" s="25" t="n">
         <v>4402</v>
       </c>
-      <c r="C13" s="24" t="n">
+      <c r="C13" s="25" t="n">
         <v>3233</v>
       </c>
-      <c r="D13" s="48" t="n">
+      <c r="D13" s="47" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>-0.265561108587006</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="47"/>
-      <c r="N13" s="43"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="46"/>
+      <c r="N13" s="42"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="29" t="n">
+      <c r="B14" s="30" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>24383.65</v>
       </c>
-      <c r="C14" s="29" t="n">
+      <c r="C14" s="30" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>23517</v>
       </c>
-      <c r="D14" s="31" t="n">
+      <c r="D14" s="32" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>-0.0355422588496801</v>
       </c>
-      <c r="E14" s="29" t="n">
+      <c r="E14" s="30" t="n">
         <f aca="false">SUM(E2:E13)</f>
         <v>12256</v>
       </c>
-      <c r="F14" s="51" t="n">
+      <c r="F14" s="50" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>2.77317912006462</v>
       </c>
-      <c r="G14" s="51" t="n">
+      <c r="G14" s="50" t="n">
         <f aca="false">AVERAGE(G2:G13)</f>
         <v>0.602021750888365</v>
       </c>
-      <c r="N14" s="43"/>
+      <c r="N14" s="42"/>
     </row>
     <row r="15" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="52"/>
-      <c r="B15" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="53" t="s">
-        <v>36</v>
+      <c r="A15" s="51"/>
+      <c r="B15" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="52" t="s">
+        <v>38</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="54"/>
-      <c r="N15" s="43"/>
+        <v>29</v>
+      </c>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="53"/>
+      <c r="N15" s="42"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="52"/>
-      <c r="B16" s="55" t="n">
+      <c r="A16" s="51"/>
+      <c r="B16" s="54" t="n">
         <v>23383</v>
       </c>
-      <c r="C16" s="55" t="n">
+      <c r="C16" s="54" t="n">
         <v>23517</v>
       </c>
-      <c r="D16" s="56" t="n">
+      <c r="D16" s="55" t="n">
         <f aca="false">(C16-B16)/B16</f>
         <v>0.00573065902578797</v>
       </c>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="54"/>
-      <c r="N16" s="43"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="53"/>
+      <c r="N16" s="42"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
@@ -2560,10 +2624,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2581,352 +2645,376 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="79.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16"/>
-      <c r="B1" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="58" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="C1" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="D1" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="59"/>
+      <c r="E1" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="58"/>
       <c r="M1" s="1" t="n">
         <f aca="false">COUNTA(D2:D13)</f>
         <v>2</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="60" t="n">
+      <c r="B2" s="59" t="n">
         <v>381400</v>
       </c>
-      <c r="C2" s="22" t="n">
+      <c r="C2" s="23" t="n">
         <v>358709</v>
       </c>
-      <c r="D2" s="22" t="n">
+      <c r="D2" s="23" t="n">
         <v>292117</v>
       </c>
-      <c r="E2" s="23" t="n">
+      <c r="E2" s="24" t="n">
         <f aca="false">(C2-B2)/B2</f>
         <v>-0.0594939695857368</v>
       </c>
-      <c r="F2" s="23" t="n">
+      <c r="F2" s="24" t="n">
         <f aca="false">(D2-C2)/C2</f>
         <v>-0.185643516053403</v>
       </c>
-      <c r="G2" s="59"/>
-      <c r="N2" s="61" t="s">
-        <v>42</v>
+      <c r="G2" s="58"/>
+      <c r="N2" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="60" t="n">
+      <c r="B3" s="59" t="n">
         <v>338378</v>
       </c>
-      <c r="C3" s="22" t="n">
+      <c r="C3" s="23" t="n">
         <v>320011</v>
       </c>
-      <c r="D3" s="22" t="n">
+      <c r="D3" s="23" t="n">
         <v>257282</v>
       </c>
-      <c r="E3" s="23" t="n">
+      <c r="E3" s="24" t="n">
         <f aca="false">(C3-B3)/B3</f>
         <v>-0.0542795335394145</v>
       </c>
-      <c r="F3" s="23" t="n">
+      <c r="F3" s="24" t="n">
         <f aca="false">(D3-C3)/C3</f>
         <v>-0.19602138676483</v>
       </c>
-      <c r="G3" s="59"/>
-      <c r="N3" s="61"/>
+      <c r="G3" s="58"/>
+      <c r="N3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="60" t="n">
+      <c r="B4" s="59" t="n">
         <v>354957</v>
       </c>
-      <c r="C4" s="22" t="n">
+      <c r="C4" s="23" t="n">
         <v>323736</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23" t="n">
+      <c r="D4" s="23"/>
+      <c r="E4" s="24" t="n">
         <f aca="false">(C4-B4)/B4</f>
         <v>-0.0879571328358083</v>
       </c>
-      <c r="F4" s="23" t="n">
+      <c r="F4" s="24" t="n">
         <f aca="false">(D4-C4)/C4</f>
         <v>-1</v>
       </c>
-      <c r="G4" s="59"/>
-      <c r="N4" s="61"/>
+      <c r="G4" s="58"/>
+      <c r="N4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="60" t="n">
+      <c r="B5" s="59" t="n">
         <v>329975</v>
       </c>
-      <c r="C5" s="22" t="n">
+      <c r="C5" s="23" t="n">
         <v>307995</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23" t="n">
+      <c r="D5" s="23"/>
+      <c r="E5" s="24" t="n">
         <f aca="false">(C5-B5)/B5</f>
         <v>-0.066611106902038</v>
       </c>
-      <c r="F5" s="23" t="n">
+      <c r="F5" s="24" t="n">
         <f aca="false">(D5-C5)/C5</f>
         <v>-1</v>
       </c>
-      <c r="G5" s="59"/>
-      <c r="N5" s="61"/>
+      <c r="G5" s="58"/>
+      <c r="N5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="60" t="n">
+      <c r="B6" s="59" t="n">
         <v>333225</v>
       </c>
-      <c r="C6" s="22" t="n">
+      <c r="C6" s="23" t="n">
         <v>305855</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23" t="n">
+      <c r="D6" s="23"/>
+      <c r="E6" s="24" t="n">
         <f aca="false">(C6-B6)/B6</f>
         <v>-0.0821366944256883</v>
       </c>
-      <c r="F6" s="23" t="n">
+      <c r="F6" s="24" t="n">
         <f aca="false">(D6-C6)/C6</f>
         <v>-1</v>
       </c>
-      <c r="G6" s="59"/>
-      <c r="N6" s="61"/>
+      <c r="G6" s="58"/>
+      <c r="N6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="60" t="n">
+      <c r="B7" s="59" t="n">
         <v>319566</v>
       </c>
-      <c r="C7" s="22" t="n">
+      <c r="C7" s="23" t="n">
         <v>289224</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23" t="n">
+      <c r="D7" s="23"/>
+      <c r="E7" s="24" t="n">
         <f aca="false">(C7-B7)/B7</f>
         <v>-0.0949475225774957</v>
       </c>
-      <c r="F7" s="23" t="n">
+      <c r="F7" s="24" t="n">
         <f aca="false">(D7-C7)/C7</f>
         <v>-1</v>
       </c>
-      <c r="G7" s="59"/>
-      <c r="N7" s="61"/>
+      <c r="G7" s="58"/>
+      <c r="N7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="60" t="n">
+      <c r="B8" s="59" t="n">
         <v>345523</v>
       </c>
-      <c r="C8" s="22" t="n">
+      <c r="C8" s="23" t="n">
         <v>304267</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23" t="n">
+      <c r="D8" s="23"/>
+      <c r="E8" s="24" t="n">
         <f aca="false">(C8-B8)/B8</f>
         <v>-0.119401602787658</v>
       </c>
-      <c r="F8" s="23" t="n">
+      <c r="F8" s="24" t="n">
         <f aca="false">(D8-C8)/C8</f>
         <v>-1</v>
       </c>
-      <c r="G8" s="59"/>
-      <c r="N8" s="61"/>
+      <c r="G8" s="58"/>
+      <c r="N8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="60" t="n">
+      <c r="B9" s="59" t="n">
         <v>344469</v>
       </c>
-      <c r="C9" s="22" t="n">
+      <c r="C9" s="23" t="n">
         <v>314709</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23" t="n">
+      <c r="D9" s="23"/>
+      <c r="E9" s="24" t="n">
         <f aca="false">(C9-B9)/B9</f>
         <v>-0.0863938409552093</v>
       </c>
-      <c r="F9" s="23" t="n">
+      <c r="F9" s="24" t="n">
         <f aca="false">(D9-C9)/C9</f>
         <v>-1</v>
       </c>
-      <c r="G9" s="59"/>
-      <c r="N9" s="61"/>
+      <c r="G9" s="58"/>
+      <c r="N9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="22" t="n">
+      <c r="B10" s="23" t="n">
         <v>342330</v>
       </c>
-      <c r="C10" s="22" t="n">
+      <c r="C10" s="23" t="n">
         <v>300248</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23" t="n">
+      <c r="D10" s="23"/>
+      <c r="E10" s="24" t="n">
         <f aca="false">(C10-B10)/B10</f>
         <v>-0.122928168726083</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="59"/>
-      <c r="N10" s="61"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="58"/>
+      <c r="N10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="22" t="n">
+      <c r="B11" s="23" t="n">
         <v>367756</v>
       </c>
-      <c r="C11" s="22" t="n">
+      <c r="C11" s="23" t="n">
         <v>303597</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23" t="n">
+      <c r="D11" s="23"/>
+      <c r="E11" s="24" t="n">
         <f aca="false">(C11-B11)/B11</f>
         <v>-0.17446078378055</v>
       </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="59"/>
-      <c r="N11" s="61"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="58"/>
+      <c r="N11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="22" t="n">
+      <c r="B12" s="23" t="n">
         <v>392032</v>
       </c>
-      <c r="C12" s="22" t="n">
+      <c r="C12" s="23" t="n">
         <v>300258</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23" t="n">
+      <c r="D12" s="23"/>
+      <c r="E12" s="24" t="n">
         <f aca="false">(C12-B12)/B12</f>
         <v>-0.234098236878622</v>
       </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="59"/>
-      <c r="N12" s="61"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="58"/>
+      <c r="N12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="62" t="n">
+      <c r="B13" s="60" t="n">
         <v>415125</v>
       </c>
-      <c r="C13" s="22" t="n">
+      <c r="C13" s="23" t="n">
         <v>316760</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23" t="n">
+      <c r="D13" s="23"/>
+      <c r="E13" s="24" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>-0.236952725082806</v>
       </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="59"/>
-      <c r="N13" s="61"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="58"/>
+      <c r="N13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="63" t="n">
+      <c r="B14" s="61" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>4264736</v>
       </c>
-      <c r="C14" s="63" t="n">
+      <c r="C14" s="61" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>3745369</v>
       </c>
-      <c r="D14" s="63" t="n">
+      <c r="D14" s="61" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>549399</v>
       </c>
-      <c r="E14" s="30" t="n">
+      <c r="E14" s="31" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>-0.121781746865457</v>
       </c>
-      <c r="F14" s="30" t="n">
+      <c r="F14" s="31" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>-0.797708112852279</v>
       </c>
-      <c r="G14" s="59"/>
-      <c r="N14" s="61"/>
+      <c r="G14" s="58"/>
+      <c r="N14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="64"/>
-      <c r="B15" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="66"/>
-      <c r="G15" s="59"/>
-      <c r="M15" s="67"/>
-      <c r="N15" s="61"/>
+      <c r="A15" s="62"/>
+      <c r="B15" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="63"/>
+      <c r="E15" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="64"/>
+      <c r="G15" s="58"/>
+      <c r="M15" s="65"/>
+      <c r="N15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="64"/>
-      <c r="B16" s="22" t="n">
+      <c r="A16" s="62"/>
+      <c r="B16" s="23" t="n">
         <v>4382326</v>
       </c>
-      <c r="C16" s="22" t="n">
+      <c r="C16" s="23" t="n">
         <f aca="false">C14</f>
         <v>3745369</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23" t="n">
+      <c r="D16" s="23"/>
+      <c r="E16" s="24" t="n">
         <f aca="false">(C16-B16)/C16</f>
         <v>-0.170065219208041</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="59"/>
-      <c r="M16" s="68"/>
-      <c r="N16" s="61"/>
-    </row>
+      <c r="F16" s="24"/>
+      <c r="G16" s="58"/>
+      <c r="M16" s="66"/>
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N17" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N18" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="1">
@@ -2950,7 +3038,7 @@
   </sheetPr>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -2968,21 +3056,21 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16"/>
-      <c r="B1" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="70" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="70" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="70" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="68" t="s">
         <v>33</v>
+      </c>
+      <c r="F1" s="68" t="s">
+        <v>35</v>
       </c>
       <c r="M1" s="1" t="n">
         <f aca="false">COUNTA(D2:D13)</f>
@@ -2991,286 +3079,286 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="71" t="n">
+      <c r="B2" s="69" t="n">
         <v>166018</v>
       </c>
-      <c r="C2" s="71" t="n">
+      <c r="C2" s="69" t="n">
         <v>154290</v>
       </c>
-      <c r="D2" s="22" t="n">
+      <c r="D2" s="23" t="n">
         <v>137349</v>
       </c>
-      <c r="E2" s="72" t="n">
+      <c r="E2" s="70" t="n">
         <f aca="false">(C2-B2)/B2</f>
         <v>-0.0706429423315544</v>
       </c>
-      <c r="F2" s="23" t="n">
+      <c r="F2" s="24" t="n">
         <f aca="false">(D2-C2)/C2</f>
         <v>-0.109799727785339</v>
       </c>
-      <c r="N2" s="42"/>
+      <c r="N2" s="41"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="73" t="n">
+      <c r="B3" s="71" t="n">
         <v>153234</v>
       </c>
-      <c r="C3" s="71" t="n">
+      <c r="C3" s="69" t="n">
         <v>139138</v>
       </c>
-      <c r="D3" s="22" t="n">
+      <c r="D3" s="23" t="n">
         <v>126757</v>
       </c>
-      <c r="E3" s="72" t="n">
+      <c r="E3" s="70" t="n">
         <f aca="false">(C3-B3)/B3</f>
         <v>-0.091990028322696</v>
       </c>
-      <c r="F3" s="23" t="n">
+      <c r="F3" s="24" t="n">
         <f aca="false">(D3-C3)/C3</f>
         <v>-0.0889835990168035</v>
       </c>
-      <c r="N3" s="43"/>
+      <c r="N3" s="42"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="71" t="n">
+      <c r="B4" s="69" t="n">
         <v>149129</v>
       </c>
-      <c r="C4" s="71" t="n">
+      <c r="C4" s="69" t="n">
         <v>139609</v>
       </c>
-      <c r="D4" s="22" t="n">
+      <c r="D4" s="23" t="n">
         <v>117550</v>
       </c>
-      <c r="E4" s="72" t="n">
+      <c r="E4" s="70" t="n">
         <f aca="false">(C4-B4)/B4</f>
         <v>-0.0638373488724527</v>
       </c>
-      <c r="F4" s="23" t="n">
+      <c r="F4" s="24" t="n">
         <f aca="false">(D4-C4)/C4</f>
         <v>-0.158005572706631</v>
       </c>
-      <c r="N4" s="43"/>
+      <c r="N4" s="42"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="71" t="n">
+      <c r="B5" s="69" t="n">
         <v>146506</v>
       </c>
-      <c r="C5" s="71" t="n">
+      <c r="C5" s="69" t="n">
         <v>126227</v>
       </c>
-      <c r="D5" s="22" t="n">
+      <c r="D5" s="23" t="n">
         <v>113477</v>
       </c>
-      <c r="E5" s="72" t="n">
+      <c r="E5" s="70" t="n">
         <f aca="false">(C5-B5)/B5</f>
         <v>-0.138417539213411</v>
       </c>
-      <c r="F5" s="23" t="n">
+      <c r="F5" s="24" t="n">
         <f aca="false">(D5-C5)/C5</f>
         <v>-0.101008500558518</v>
       </c>
-      <c r="N5" s="43"/>
+      <c r="N5" s="42"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="71" t="n">
+      <c r="B6" s="69" t="n">
         <v>122937</v>
       </c>
-      <c r="C6" s="71" t="n">
+      <c r="C6" s="69" t="n">
         <v>128749</v>
       </c>
-      <c r="D6" s="22" t="n">
+      <c r="D6" s="23" t="n">
         <v>108336</v>
       </c>
-      <c r="E6" s="72" t="n">
+      <c r="E6" s="70" t="n">
         <f aca="false">(C6-B6)/B6</f>
         <v>0.0472762471835168</v>
       </c>
-      <c r="F6" s="23" t="n">
+      <c r="F6" s="24" t="n">
         <f aca="false">(D6-C6)/C6</f>
         <v>-0.158548804262557</v>
       </c>
-      <c r="N6" s="43"/>
+      <c r="N6" s="42"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="71" t="n">
+      <c r="B7" s="69" t="n">
         <v>113710</v>
       </c>
-      <c r="C7" s="71" t="n">
+      <c r="C7" s="69" t="n">
         <v>125671</v>
       </c>
-      <c r="D7" s="22" t="n">
+      <c r="D7" s="23" t="n">
         <v>98523</v>
       </c>
-      <c r="E7" s="72" t="n">
+      <c r="E7" s="70" t="n">
         <f aca="false">(C7-B7)/B7</f>
         <v>0.10518863776273</v>
       </c>
-      <c r="F7" s="23" t="n">
+      <c r="F7" s="24" t="n">
         <f aca="false">(D7-C7)/C7</f>
         <v>-0.216024381122136</v>
       </c>
-      <c r="N7" s="43"/>
+      <c r="N7" s="42"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="71" t="n">
+      <c r="B8" s="69" t="n">
         <v>117122</v>
       </c>
-      <c r="C8" s="71" t="n">
+      <c r="C8" s="69" t="n">
         <v>147302</v>
       </c>
-      <c r="D8" s="22" t="n">
+      <c r="D8" s="23" t="n">
         <v>103029</v>
       </c>
-      <c r="E8" s="72" t="n">
+      <c r="E8" s="70" t="n">
         <f aca="false">(C8-B8)/B8</f>
         <v>0.257680025955841</v>
       </c>
-      <c r="F8" s="23" t="n">
+      <c r="F8" s="24" t="n">
         <f aca="false">(D8-C8)/C8</f>
         <v>-0.300559394984454</v>
       </c>
-      <c r="N8" s="43"/>
+      <c r="N8" s="42"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="71" t="n">
+      <c r="B9" s="69" t="n">
         <v>126623</v>
       </c>
-      <c r="C9" s="71" t="n">
+      <c r="C9" s="69" t="n">
         <v>145461</v>
       </c>
-      <c r="D9" s="22" t="n">
+      <c r="D9" s="23" t="n">
         <v>115694</v>
       </c>
-      <c r="E9" s="72" t="n">
+      <c r="E9" s="70" t="n">
         <f aca="false">(C9-B9)/B9</f>
         <v>0.148772339938242</v>
       </c>
-      <c r="F9" s="23" t="n">
+      <c r="F9" s="24" t="n">
         <f aca="false">(D9-C9)/C9</f>
         <v>-0.204639044142416</v>
       </c>
-      <c r="N9" s="43"/>
+      <c r="N9" s="42"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="71" t="n">
+      <c r="B10" s="69" t="n">
         <v>122360</v>
       </c>
-      <c r="C10" s="71" t="n">
+      <c r="C10" s="69" t="n">
         <v>149470</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="72" t="n">
+      <c r="D10" s="23"/>
+      <c r="E10" s="70" t="n">
         <f aca="false">(C10-B10)/B10</f>
         <v>0.221559333115397</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="N10" s="43"/>
+      <c r="F10" s="24"/>
+      <c r="N10" s="42"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="71" t="n">
+      <c r="B11" s="69" t="n">
         <v>132280</v>
       </c>
-      <c r="C11" s="71" t="n">
+      <c r="C11" s="69" t="n">
         <v>165507</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="72" t="n">
+      <c r="D11" s="23"/>
+      <c r="E11" s="70" t="n">
         <f aca="false">(C11-B11)/B11</f>
         <v>0.251186876322951</v>
       </c>
-      <c r="F11" s="23"/>
-      <c r="N11" s="43"/>
+      <c r="F11" s="24"/>
+      <c r="N11" s="42"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="71" t="n">
+      <c r="B12" s="69" t="n">
         <v>128303</v>
       </c>
-      <c r="C12" s="71" t="n">
+      <c r="C12" s="69" t="n">
         <v>162736</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="72" t="n">
+      <c r="D12" s="23"/>
+      <c r="E12" s="70" t="n">
         <f aca="false">(C12-B12)/B12</f>
         <v>0.268372524414862</v>
       </c>
-      <c r="F12" s="23"/>
-      <c r="N12" s="43"/>
+      <c r="F12" s="24"/>
+      <c r="N12" s="42"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="71" t="n">
+      <c r="B13" s="69" t="n">
         <v>132120</v>
       </c>
-      <c r="C13" s="71" t="n">
+      <c r="C13" s="69" t="n">
         <v>165619</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="72" t="n">
+      <c r="D13" s="23"/>
+      <c r="E13" s="70" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>0.253549803209204</v>
       </c>
-      <c r="F13" s="23"/>
-      <c r="N13" s="43"/>
+      <c r="F13" s="24"/>
+      <c r="N13" s="42"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="63" t="n">
+      <c r="B14" s="61" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>1610342</v>
       </c>
-      <c r="C14" s="63" t="n">
+      <c r="C14" s="61" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>1749779</v>
       </c>
-      <c r="D14" s="63" t="n">
+      <c r="D14" s="61" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>920715</v>
       </c>
-      <c r="E14" s="30" t="n">
+      <c r="E14" s="31" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>0.0865884389775588</v>
       </c>
-      <c r="F14" s="30" t="n">
+      <c r="F14" s="31" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>-0.167196128072357</v>
       </c>
-      <c r="N14" s="43"/>
+      <c r="N14" s="42"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3292,21 +3380,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="32.44"/>
@@ -3314,49 +3402,49 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16"/>
-      <c r="B1" s="74" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="74" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="75" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="76" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="75" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
       <c r="M1" s="1" t="n">
         <f aca="false">COUNTA(D2:D13)</f>
         <v>2</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="22" t="n">
+      <c r="B2" s="23" t="n">
         <v>40365</v>
       </c>
-      <c r="C2" s="22" t="n">
+      <c r="C2" s="23" t="n">
         <v>41888</v>
       </c>
-      <c r="D2" s="22" t="n">
+      <c r="D2" s="23" t="n">
         <v>46250</v>
       </c>
-      <c r="E2" s="23" t="n">
+      <c r="E2" s="24" t="n">
         <f aca="false">(C2-B2)/B2</f>
         <v>0.0377307072959247</v>
       </c>
@@ -3364,29 +3452,29 @@
         <f aca="false">(D2-C2)/C2</f>
         <v>0.104134835752483</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
       <c r="N2" s="9" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="22" t="n">
+      <c r="B3" s="23" t="n">
         <v>37545</v>
       </c>
-      <c r="C3" s="41" t="n">
+      <c r="C3" s="40" t="n">
         <v>50219</v>
       </c>
-      <c r="D3" s="22" t="n">
+      <c r="D3" s="23" t="n">
         <v>33335</v>
       </c>
-      <c r="E3" s="23" t="n">
+      <c r="E3" s="24" t="n">
         <f aca="false">(C3-B3)/B3</f>
         <v>0.337568251431615</v>
       </c>
@@ -3394,27 +3482,27 @@
         <f aca="false">(D3-C3)/C3</f>
         <v>-0.336207411537466</v>
       </c>
-      <c r="G3" s="77" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
+      <c r="G3" s="75" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
       <c r="N3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="22" t="n">
+      <c r="B4" s="23" t="n">
         <v>25781.81</v>
       </c>
-      <c r="C4" s="41" t="n">
+      <c r="C4" s="40" t="n">
         <v>45023</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23" t="n">
+      <c r="D4" s="23"/>
+      <c r="E4" s="24" t="n">
         <f aca="false">(C4-B4)/B4</f>
         <v>0.746308734724211</v>
       </c>
@@ -3422,25 +3510,25 @@
         <f aca="false">(D4-C4)/C4</f>
         <v>-1</v>
       </c>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
       <c r="N4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="22" t="n">
+      <c r="B5" s="23" t="n">
         <v>25781.81</v>
       </c>
-      <c r="C5" s="41" t="n">
+      <c r="C5" s="40" t="n">
         <v>25839</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23" t="n">
+      <c r="D5" s="23"/>
+      <c r="E5" s="24" t="n">
         <f aca="false">(C5-B5)/B5</f>
         <v>0.00221823060522123</v>
       </c>
@@ -3448,25 +3536,25 @@
         <f aca="false">(D5-C5)/C5</f>
         <v>-1</v>
       </c>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
       <c r="N5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="22" t="n">
+      <c r="B6" s="23" t="n">
         <v>13432.28</v>
       </c>
-      <c r="C6" s="41" t="n">
+      <c r="C6" s="40" t="n">
         <v>12769</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23" t="n">
+      <c r="D6" s="23"/>
+      <c r="E6" s="24" t="n">
         <f aca="false">(C6-B6)/B6</f>
         <v>-0.0493795543273369</v>
       </c>
@@ -3474,25 +3562,25 @@
         <f aca="false">(D6-C6)/C6</f>
         <v>-1</v>
       </c>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
       <c r="N6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="22" t="n">
+      <c r="B7" s="23" t="n">
         <v>15430.56</v>
       </c>
-      <c r="C7" s="41" t="n">
+      <c r="C7" s="40" t="n">
         <v>10444</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23" t="n">
+      <c r="D7" s="23"/>
+      <c r="E7" s="24" t="n">
         <f aca="false">(C7-B7)/B7</f>
         <v>-0.323161311060648</v>
       </c>
@@ -3500,25 +3588,25 @@
         <f aca="false">(D7-C7)/C7</f>
         <v>-1</v>
       </c>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
       <c r="N7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="22" t="n">
+      <c r="B8" s="23" t="n">
         <v>7210.53</v>
       </c>
-      <c r="C8" s="22" t="n">
+      <c r="C8" s="23" t="n">
         <v>9191</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23" t="n">
+      <c r="D8" s="23"/>
+      <c r="E8" s="24" t="n">
         <f aca="false">(C8-B8)/B8</f>
         <v>0.274663582288681</v>
       </c>
@@ -3526,25 +3614,25 @@
         <f aca="false">(D8-C8)/C8</f>
         <v>-1</v>
       </c>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
       <c r="N8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="22" t="n">
+      <c r="B9" s="23" t="n">
         <v>7045.99</v>
       </c>
-      <c r="C9" s="22" t="n">
+      <c r="C9" s="23" t="n">
         <v>11379</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23" t="n">
+      <c r="D9" s="23"/>
+      <c r="E9" s="24" t="n">
         <f aca="false">(C9-B9)/B9</f>
         <v>0.614961133921564</v>
       </c>
@@ -3552,171 +3640,195 @@
         <f aca="false">(D9-C9)/C9</f>
         <v>-1</v>
       </c>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
       <c r="N9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="24" t="n">
+      <c r="B10" s="25" t="n">
         <v>23032</v>
       </c>
-      <c r="C10" s="22" t="n">
+      <c r="C10" s="23" t="n">
         <v>11779</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="26" t="n">
+      <c r="D10" s="23"/>
+      <c r="E10" s="27" t="n">
         <f aca="false">(C10-B10)/B10</f>
         <v>-0.488581104550191</v>
       </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
       <c r="N10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="24" t="n">
+      <c r="B11" s="25" t="n">
         <v>36770</v>
       </c>
-      <c r="C11" s="22" t="n">
+      <c r="C11" s="23" t="n">
         <v>23418</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="26" t="n">
+      <c r="D11" s="23"/>
+      <c r="E11" s="27" t="n">
         <f aca="false">(C11-B11)/B11</f>
         <v>-0.3631221104161</v>
       </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
+      <c r="G11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
       <c r="N11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="69" t="s">
+      <c r="A12" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="24" t="n">
+      <c r="B12" s="25" t="n">
         <v>40381</v>
       </c>
-      <c r="C12" s="22" t="n">
+      <c r="C12" s="23" t="n">
         <v>34717</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="26" t="n">
+      <c r="D12" s="23"/>
+      <c r="E12" s="27" t="n">
         <f aca="false">(C12-B12)/B12</f>
         <v>-0.140263985537753</v>
       </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
+      <c r="G12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
       <c r="N12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="78" t="n">
+      <c r="B13" s="76" t="n">
         <v>34355</v>
       </c>
-      <c r="C13" s="22" t="n">
+      <c r="C13" s="23" t="n">
         <v>36455</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23" t="n">
+      <c r="D13" s="23"/>
+      <c r="E13" s="24" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>0.0611264735846311</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
+      <c r="G13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
       <c r="N13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="63" t="n">
+      <c r="B14" s="61" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>307130.98</v>
       </c>
-      <c r="C14" s="63" t="n">
+      <c r="C14" s="61" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>313121</v>
       </c>
-      <c r="D14" s="29" t="n">
+      <c r="D14" s="30" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>79585</v>
       </c>
-      <c r="E14" s="30" t="n">
+      <c r="E14" s="31" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>0.0195031448797514</v>
       </c>
-      <c r="F14" s="31" t="n">
+      <c r="F14" s="32" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>-0.779009071973123</v>
       </c>
-      <c r="G14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
+      <c r="G14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
       <c r="N14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="79"/>
-      <c r="B15" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="80" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="80"/>
-      <c r="E15" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="81"/>
-      <c r="G15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="78" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="78"/>
+      <c r="E15" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="79"/>
+      <c r="G15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
       <c r="N15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="79"/>
-      <c r="B16" s="82" t="n">
+      <c r="A16" s="77"/>
+      <c r="B16" s="80" t="n">
         <v>331445.11</v>
       </c>
-      <c r="C16" s="82" t="n">
+      <c r="C16" s="80" t="n">
         <v>272775.98</v>
       </c>
-      <c r="D16" s="80"/>
+      <c r="D16" s="78"/>
       <c r="E16" s="8" t="n">
         <f aca="false">(C16-B16)/C16</f>
         <v>-0.215081731170025</v>
       </c>
-      <c r="F16" s="81"/>
-      <c r="G16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
       <c r="N16" s="9"/>
     </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N17" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N18" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Write suggestions for comments in the spreadsheet
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -725,7 +725,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="65">
   <si>
     <t xml:space="preserve">Waste</t>
   </si>
@@ -739,12 +739,18 @@
     <t xml:space="preserve">Percentage Recycled</t>
   </si>
   <si>
+    <t xml:space="preserve">Title: </t>
+  </si>
+  <si>
     <t xml:space="preserve">Did you know?</t>
   </si>
   <si>
     <t xml:space="preserve">Jan</t>
   </si>
   <si>
+    <t xml:space="preserve">Comment: </t>
+  </si>
+  <si>
     <t xml:space="preserve">Every week, we donate leftover clothes hangers to you, our customers! Find them by the Customer Service Desk.</t>
   </si>
   <si>
@@ -784,7 +790,7 @@
     <t xml:space="preserve">Total</t>
   </si>
   <si>
-    <t xml:space="preserve">Nothing to report? Here’s a default fun fact:</t>
+    <t xml:space="preserve">Nothing to report? Try using this comment for the waste slide:</t>
   </si>
   <si>
     <t xml:space="preserve">Water 2017 (M3)</t>
@@ -802,21 +808,24 @@
     <t xml:space="preserve">Percentage Difference Vs last year</t>
   </si>
   <si>
-    <t xml:space="preserve">Top Tip!</t>
+    <t xml:space="preserve">Top tip!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015 Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017 Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage Difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nothing to report? Try using this comment for the water slide:</t>
   </si>
   <si>
     <t xml:space="preserve">Cabot Circus uses state-of-the-art rainwater harvesting technology, which helps reduce water waste!</t>
   </si>
   <si>
-    <t xml:space="preserve">2015 Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017 Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage Difference</t>
-  </si>
-  <si>
     <t xml:space="preserve">Landlord Water only</t>
   </si>
   <si>
@@ -871,6 +880,9 @@
     <t xml:space="preserve">2017 Elec</t>
   </si>
   <si>
+    <t xml:space="preserve">Nothing to report? Try using this comment for the electricity slide:</t>
+  </si>
+  <si>
     <t xml:space="preserve">CP Elec 2016 (kWh)</t>
   </si>
   <si>
@@ -902,6 +914,9 @@
   </si>
   <si>
     <t xml:space="preserve">2017 Gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nothing to report? Try using this comment for the gas slide:</t>
   </si>
   <si>
     <t xml:space="preserve">Using a machine known as an anaerobic digester, we convert tons of food waste back into energy!</t>
@@ -921,7 +936,7 @@
     <numFmt numFmtId="170" formatCode="0.00%"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -958,6 +973,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -969,14 +992,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1036,6 +1051,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1106,7 +1127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1119,6 +1140,13 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -1173,7 +1201,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="84">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1194,7 +1222,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1210,7 +1242,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1226,19 +1258,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="167" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1278,7 +1314,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1294,7 +1330,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1302,7 +1338,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1318,6 +1354,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -1334,6 +1374,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -1347,7 +1391,7 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1370,7 +1414,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1414,7 +1458,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1434,14 +1478,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -1454,7 +1490,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1474,11 +1510,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1576,10 +1616,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S15" activeCellId="0" sqref="S15"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1593,7 +1633,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="8.89"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="30.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1606,201 +1646,231 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="1" t="n">
-        <f aca="false">COUNTA(C2:C13)</f>
-        <v>2</v>
-      </c>
-      <c r="N1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="N1" s="6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="7" t="n">
+      <c r="A2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="8" t="n">
         <v>136.2</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="8" t="n">
         <v>122.19</v>
       </c>
-      <c r="D2" s="8" t="n">
+      <c r="D2" s="9" t="n">
         <f aca="false">C2/B2</f>
         <v>0.897136563876652</v>
       </c>
-      <c r="N2" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="N2" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="n">
         <v>138.2</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="8" t="n">
         <v>124.62</v>
       </c>
-      <c r="D3" s="8" t="n">
+      <c r="D3" s="9" t="n">
         <f aca="false">C3/B3</f>
         <v>0.901736613603473</v>
       </c>
-      <c r="N3" s="9"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8" t="e">
+      <c r="M3" s="5"/>
+      <c r="N3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9" t="e">
         <f aca="false">C4/B4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N4" s="9"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8" t="e">
+      <c r="M4" s="5"/>
+      <c r="N4" s="10"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9" t="e">
         <f aca="false">C5/B5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N5" s="9"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8" t="e">
+      <c r="M5" s="5"/>
+      <c r="N5" s="10"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9" t="e">
         <f aca="false">C6/B6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N6" s="9"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="8" t="e">
+      <c r="M6" s="5"/>
+      <c r="N6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="9" t="e">
         <f aca="false">C7/B7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N7" s="9"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="8" t="e">
+      <c r="M7" s="5"/>
+      <c r="N7" s="10"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="9" t="e">
         <f aca="false">C8/B8</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="8" t="e">
+      <c r="M8" s="5"/>
+      <c r="N8" s="10"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="9" t="e">
         <f aca="false">C9/B9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N9" s="9"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="8" t="e">
+      <c r="M9" s="5"/>
+      <c r="N9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="9" t="e">
         <f aca="false">C10/B10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N10" s="9"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="8" t="e">
+      <c r="M10" s="5"/>
+      <c r="N10" s="10"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="9" t="e">
         <f aca="false">C11/B11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N11" s="9"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="8" t="e">
+      <c r="M11" s="5"/>
+      <c r="N11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="9" t="e">
         <f aca="false">C12/B12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N12" s="9"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="8" t="e">
+      <c r="M12" s="5"/>
+      <c r="N12" s="10"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="9" t="e">
         <f aca="false">C13/B13</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N13" s="9"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="14" t="n">
+      <c r="M13" s="5"/>
+      <c r="N13" s="10"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="15" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>274.4</v>
       </c>
-      <c r="C14" s="14" t="n">
+      <c r="C14" s="15" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>246.81</v>
       </c>
-      <c r="D14" s="15" t="e">
+      <c r="D14" s="16" t="e">
         <f aca="false">AVERAGE(D2:D13)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N14" s="9"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N15" s="9"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N16" s="9"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="10"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M15" s="5"/>
+      <c r="N15" s="10"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M16" s="5"/>
+      <c r="N16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N17" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N18" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="M17" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M18" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="18"/>
+      <c r="T18" s="18"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1818,8 +1888,11 @@
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
-  <mergeCells count="1">
+  <mergeCells count="4">
+    <mergeCell ref="M2:M16"/>
     <mergeCell ref="N2:N16"/>
+    <mergeCell ref="M17:T17"/>
+    <mergeCell ref="M18:T18"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1836,10 +1909,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
+      <selection pane="topLeft" activeCell="R16" activeCellId="0" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1850,345 +1923,373 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="8.89"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="79.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17"/>
-      <c r="B1" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="19" t="s">
+    <row r="1" customFormat="false" ht="50.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="19"/>
+      <c r="B1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="1" t="n">
-        <f aca="false">COUNTA(D2:D13)</f>
-        <v>2</v>
-      </c>
-      <c r="N1" s="5" t="s">
+      <c r="E1" s="22" t="s">
         <v>25</v>
       </c>
+      <c r="F1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="22" t="n">
+      <c r="A2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="24" t="n">
         <v>6150</v>
       </c>
-      <c r="C2" s="23" t="n">
+      <c r="C2" s="25" t="n">
         <v>8273</v>
       </c>
-      <c r="D2" s="23" t="n">
+      <c r="D2" s="25" t="n">
         <v>8065</v>
       </c>
-      <c r="E2" s="24" t="n">
+      <c r="E2" s="26" t="n">
         <f aca="false">(C2-B2)/B2</f>
         <v>0.34520325203252</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="9" t="n">
         <f aca="false">(D2-C2)/D2</f>
         <v>-0.0257904525728456</v>
       </c>
-      <c r="N2" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
+      <c r="M2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="22" t="n">
+      <c r="N2" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="24" t="n">
         <v>6071</v>
       </c>
-      <c r="C3" s="23" t="n">
+      <c r="C3" s="25" t="n">
         <v>7349</v>
       </c>
-      <c r="D3" s="23" t="n">
+      <c r="D3" s="25" t="n">
         <v>6895</v>
       </c>
-      <c r="E3" s="24" t="n">
+      <c r="E3" s="26" t="n">
         <f aca="false">(C3-B3)/B3</f>
         <v>0.210508977104266</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="9" t="n">
         <f aca="false">(D3-C3)/D3</f>
         <v>-0.0658448150833938</v>
       </c>
-      <c r="N3" s="9"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="22" t="n">
+      <c r="M3" s="5"/>
+      <c r="N3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="24" t="n">
         <v>5579</v>
       </c>
-      <c r="C4" s="23" t="n">
+      <c r="C4" s="25" t="n">
         <v>5620</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24" t="n">
+      <c r="D4" s="25"/>
+      <c r="E4" s="26" t="n">
         <f aca="false">(C4-B4)/B4</f>
         <v>0.00734898727370497</v>
       </c>
-      <c r="F4" s="8" t="e">
+      <c r="F4" s="9" t="e">
         <f aca="false">(D4-C4)/D4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N4" s="9"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="22" t="n">
+      <c r="M4" s="5"/>
+      <c r="N4" s="10"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="24" t="n">
         <v>5734</v>
       </c>
-      <c r="C5" s="23" t="n">
+      <c r="C5" s="25" t="n">
         <v>8615</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24" t="n">
+      <c r="D5" s="25"/>
+      <c r="E5" s="26" t="n">
         <f aca="false">(C5-B5)/B5</f>
         <v>0.502441576560865</v>
       </c>
-      <c r="F5" s="8" t="e">
+      <c r="F5" s="9" t="e">
         <f aca="false">(D5-C5)/D5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N5" s="9"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="22" t="n">
+      <c r="M5" s="5"/>
+      <c r="N5" s="10"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="24" t="n">
         <v>6577</v>
       </c>
-      <c r="C6" s="25" t="n">
+      <c r="C6" s="27" t="n">
         <v>10387</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24" t="n">
+      <c r="D6" s="25"/>
+      <c r="E6" s="26" t="n">
         <f aca="false">(C6-B6)/B6</f>
         <v>0.579291470275201</v>
       </c>
-      <c r="F6" s="8" t="e">
+      <c r="F6" s="9" t="e">
         <f aca="false">(D6-C6)/D6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N6" s="9"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="22" t="n">
+      <c r="M6" s="5"/>
+      <c r="N6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="24" t="n">
         <v>7009</v>
       </c>
-      <c r="C7" s="25" t="n">
+      <c r="C7" s="27" t="n">
         <v>8235</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24" t="n">
+      <c r="D7" s="25"/>
+      <c r="E7" s="26" t="n">
         <f aca="false">(C7-B7)/B7</f>
         <v>0.174917962619489</v>
       </c>
-      <c r="F7" s="8" t="e">
+      <c r="F7" s="9" t="e">
         <f aca="false">(D7-C7)/D7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N7" s="9"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="22" t="n">
+      <c r="M7" s="5"/>
+      <c r="N7" s="10"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="24" t="n">
         <v>6729</v>
       </c>
-      <c r="C8" s="23" t="n">
+      <c r="C8" s="25" t="n">
         <v>7634</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24" t="n">
+      <c r="D8" s="25"/>
+      <c r="E8" s="26" t="n">
         <f aca="false">(C8-B8)/B8</f>
         <v>0.134492495170159</v>
       </c>
-      <c r="F8" s="8" t="e">
+      <c r="F8" s="9" t="e">
         <f aca="false">(D8-C8)/D8</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="22" t="n">
+      <c r="M8" s="5"/>
+      <c r="N8" s="10"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="24" t="n">
         <v>8567</v>
       </c>
-      <c r="C9" s="23" t="n">
+      <c r="C9" s="25" t="n">
         <v>8694</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24" t="n">
+      <c r="D9" s="25"/>
+      <c r="E9" s="26" t="n">
         <f aca="false">(C9-B9)/B9</f>
         <v>0.0148243259017159</v>
       </c>
-      <c r="F9" s="8" t="e">
+      <c r="F9" s="9" t="e">
         <f aca="false">(D9-C9)/D9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N9" s="9"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="22" t="n">
+      <c r="M9" s="5"/>
+      <c r="N9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="24" t="n">
         <v>8328</v>
       </c>
-      <c r="C10" s="23" t="n">
+      <c r="C10" s="25" t="n">
         <v>7729</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24" t="n">
+      <c r="D10" s="25"/>
+      <c r="E10" s="26" t="n">
         <f aca="false">(C10-B10)/B10</f>
         <v>-0.071926032660903</v>
       </c>
-      <c r="F10" s="8" t="e">
+      <c r="F10" s="9" t="e">
         <f aca="false">(D10-C10)/D10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N10" s="9"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="22" t="n">
+      <c r="M10" s="5"/>
+      <c r="N10" s="10"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="24" t="n">
         <v>8404</v>
       </c>
-      <c r="C11" s="23" t="n">
+      <c r="C11" s="25" t="n">
         <v>8881</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24" t="n">
+      <c r="D11" s="25"/>
+      <c r="E11" s="26" t="n">
         <f aca="false">(C11-B11)/B11</f>
         <v>0.0567586863398382</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="N11" s="9"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="22" t="n">
+      <c r="F11" s="9"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="24" t="n">
         <v>8556</v>
       </c>
-      <c r="C12" s="23" t="n">
+      <c r="C12" s="25" t="n">
         <v>8520</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24" t="n">
+      <c r="D12" s="25"/>
+      <c r="E12" s="26" t="n">
         <f aca="false">(C12-B12)/B12</f>
         <v>-0.00420757363253857</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="N12" s="9"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="26" t="n">
+      <c r="F12" s="9"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="10"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="28" t="n">
         <v>8881</v>
       </c>
-      <c r="C13" s="23" t="n">
+      <c r="C13" s="25" t="n">
         <v>6912</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="27" t="n">
+      <c r="D13" s="25"/>
+      <c r="E13" s="29" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>-0.22170926697444</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="N13" s="9"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="29" t="n">
+      <c r="F13" s="9"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="10"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="31" t="n">
         <v>77704</v>
       </c>
-      <c r="C14" s="30" t="n">
+      <c r="C14" s="32" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>96849</v>
       </c>
-      <c r="D14" s="30" t="n">
+      <c r="D14" s="32" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>14960</v>
       </c>
-      <c r="E14" s="31" t="n">
+      <c r="E14" s="33" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>0.24638371255019</v>
       </c>
-      <c r="F14" s="32" t="e">
+      <c r="F14" s="34" t="e">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N14" s="9"/>
-    </row>
-    <row r="15" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="17" t="s">
+      <c r="M14" s="5"/>
+      <c r="N14" s="10"/>
+    </row>
+    <row r="15" customFormat="false" ht="43.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="33" t="s">
+      <c r="C15" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="N15" s="9"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="33"/>
-      <c r="B16" s="23" t="n">
+      <c r="D15" s="19"/>
+      <c r="E15" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="19"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="10"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="35"/>
+      <c r="B16" s="25" t="n">
         <v>81734</v>
       </c>
-      <c r="C16" s="23" t="n">
+      <c r="C16" s="25" t="n">
         <v>77704</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="34" t="n">
+      <c r="D16" s="19"/>
+      <c r="E16" s="36" t="n">
         <f aca="false">(C16-B16)/B16</f>
         <v>-0.0493062862456261</v>
       </c>
-      <c r="F16" s="35"/>
-      <c r="N16" s="9"/>
+      <c r="F16" s="37"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N17" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N18" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="M17" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M18" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="38"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2206,8 +2307,11 @@
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
-  <mergeCells count="1">
+  <mergeCells count="4">
+    <mergeCell ref="M2:M16"/>
     <mergeCell ref="N2:N16"/>
+    <mergeCell ref="M17:S17"/>
+    <mergeCell ref="M18:S18"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2228,7 +2332,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2240,371 +2344,367 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="B1" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="D1" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="1" t="n">
-        <f aca="false">COUNTA(E2:E13)</f>
+      <c r="E1" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="43"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="5"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="40" t="n">
+      <c r="B2" s="44" t="n">
         <v>1217</v>
       </c>
-      <c r="C2" s="40" t="n">
+      <c r="C2" s="44" t="n">
         <v>224</v>
       </c>
-      <c r="D2" s="8" t="n">
+      <c r="D2" s="9" t="n">
         <f aca="false">(C2-B2)/B2</f>
         <v>-0.815940838126541</v>
       </c>
-      <c r="E2" s="23" t="n">
+      <c r="E2" s="25" t="n">
         <v>1493</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="9" t="n">
         <f aca="false">(E2-C2)/C2</f>
         <v>5.66517857142857</v>
       </c>
-      <c r="G2" s="8" t="n">
+      <c r="G2" s="9" t="n">
         <f aca="false">(E2-B2)/B2</f>
         <v>0.226787181594084</v>
       </c>
-      <c r="N2" s="41"/>
+      <c r="N2" s="45"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="40" t="n">
+      <c r="A3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="44" t="n">
         <v>1518.25</v>
       </c>
-      <c r="C3" s="40" t="n">
+      <c r="C3" s="44" t="n">
         <v>221</v>
       </c>
-      <c r="D3" s="8" t="n">
+      <c r="D3" s="9" t="n">
         <f aca="false">(C3-B3)/B3</f>
         <v>-0.854437674954717</v>
       </c>
-      <c r="E3" s="23" t="n">
+      <c r="E3" s="25" t="n">
         <v>1326</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="9" t="n">
         <f aca="false">(E3-C3)/C3</f>
         <v>5</v>
       </c>
-      <c r="G3" s="8" t="n">
+      <c r="G3" s="9" t="n">
         <f aca="false">(E3-B3)/B3</f>
         <v>-0.126626049728306</v>
       </c>
-      <c r="N3" s="42"/>
+      <c r="N3" s="46"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="40" t="n">
+      <c r="A4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="44" t="n">
         <v>1203.4</v>
       </c>
-      <c r="C4" s="40" t="n">
+      <c r="C4" s="44" t="n">
         <v>203</v>
       </c>
-      <c r="D4" s="8" t="n">
+      <c r="D4" s="9" t="n">
         <f aca="false">(C4-B4)/B4</f>
         <v>-0.831311284693369</v>
       </c>
-      <c r="E4" s="23" t="n">
+      <c r="E4" s="25" t="n">
         <v>1014</v>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="9" t="n">
         <f aca="false">(E4-C4)/C4</f>
         <v>3.99507389162562</v>
       </c>
-      <c r="G4" s="8" t="n">
+      <c r="G4" s="9" t="n">
         <f aca="false">(E4-B4)/B4</f>
         <v>-0.15738740235998</v>
       </c>
-      <c r="N4" s="42"/>
+      <c r="N4" s="46"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="23" t="n">
+      <c r="A5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="25" t="n">
         <v>1408</v>
       </c>
-      <c r="C5" s="23" t="n">
+      <c r="C5" s="25" t="n">
         <v>1516</v>
       </c>
-      <c r="D5" s="8" t="n">
+      <c r="D5" s="9" t="n">
         <f aca="false">(C5-B5)/B5</f>
         <v>0.0767045454545455</v>
       </c>
-      <c r="E5" s="23" t="n">
+      <c r="E5" s="25" t="n">
         <v>2664</v>
       </c>
-      <c r="F5" s="8" t="n">
+      <c r="F5" s="9" t="n">
         <f aca="false">(E5-C5)/C5</f>
         <v>0.757255936675462</v>
       </c>
-      <c r="G5" s="8" t="n">
+      <c r="G5" s="9" t="n">
         <f aca="false">(E5-B5)/B5</f>
         <v>0.892045454545455</v>
       </c>
-      <c r="N5" s="42"/>
+      <c r="N5" s="46"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="23" t="n">
+      <c r="A6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="25" t="n">
         <v>1264</v>
       </c>
-      <c r="C6" s="23" t="n">
+      <c r="C6" s="25" t="n">
         <v>1739</v>
       </c>
-      <c r="D6" s="8" t="n">
+      <c r="D6" s="9" t="n">
         <f aca="false">(C6-B6)/B6</f>
         <v>0.375791139240506</v>
       </c>
-      <c r="E6" s="25" t="n">
+      <c r="E6" s="27" t="n">
         <v>3212</v>
       </c>
-      <c r="F6" s="8" t="n">
+      <c r="F6" s="9" t="n">
         <f aca="false">(E6-C6)/C6</f>
         <v>0.847038527889592</v>
       </c>
-      <c r="G6" s="8" t="n">
+      <c r="G6" s="9" t="n">
         <f aca="false">(E6-B6)/B6</f>
         <v>1.54113924050633</v>
       </c>
-      <c r="N6" s="42"/>
+      <c r="N6" s="46"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="23" t="n">
+      <c r="A7" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="25" t="n">
         <v>1139</v>
       </c>
-      <c r="C7" s="23" t="n">
+      <c r="C7" s="25" t="n">
         <v>1853</v>
       </c>
-      <c r="D7" s="8" t="n">
+      <c r="D7" s="9" t="n">
         <f aca="false">(C7-B7)/B7</f>
         <v>0.626865671641791</v>
       </c>
-      <c r="E7" s="25" t="n">
+      <c r="E7" s="27" t="n">
         <v>2547</v>
       </c>
-      <c r="F7" s="43" t="n">
+      <c r="F7" s="47" t="n">
         <f aca="false">(E7-C7)/C7</f>
         <v>0.374527792768483</v>
       </c>
-      <c r="G7" s="8" t="n">
+      <c r="G7" s="9" t="n">
         <f aca="false">(E7-B7)/B7</f>
         <v>1.23617208077261</v>
       </c>
-      <c r="N7" s="42"/>
+      <c r="N7" s="46"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="23" t="n">
+      <c r="A8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="25" t="n">
         <v>2496</v>
       </c>
-      <c r="C8" s="23" t="n">
+      <c r="C8" s="25" t="n">
         <v>2137</v>
       </c>
-      <c r="D8" s="8" t="n">
+      <c r="D8" s="9" t="n">
         <f aca="false">(C8-B8)/B8</f>
         <v>-0.143830128205128</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="8"/>
-      <c r="N8" s="42"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="9"/>
+      <c r="N8" s="46"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="23" t="n">
+      <c r="A9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="25" t="n">
         <v>2298</v>
       </c>
-      <c r="C9" s="23" t="n">
+      <c r="C9" s="25" t="n">
         <v>2842</v>
       </c>
-      <c r="D9" s="8" t="n">
+      <c r="D9" s="9" t="n">
         <f aca="false">(C9-B9)/B9</f>
         <v>0.236727589208007</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="8"/>
-      <c r="N9" s="42"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="9"/>
+      <c r="N9" s="46"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="23" t="n">
+      <c r="A10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="25" t="n">
         <v>2263</v>
       </c>
-      <c r="C10" s="23" t="n">
+      <c r="C10" s="25" t="n">
         <v>3066</v>
       </c>
-      <c r="D10" s="8" t="n">
+      <c r="D10" s="9" t="n">
         <f aca="false">(C10-B10)/B10</f>
         <v>0.354838709677419</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="45"/>
-      <c r="N10" s="42"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="49"/>
+      <c r="N10" s="46"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="23" t="n">
+      <c r="A11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="25" t="n">
         <v>2253</v>
       </c>
-      <c r="C11" s="23" t="n">
+      <c r="C11" s="25" t="n">
         <v>3142</v>
       </c>
-      <c r="D11" s="8" t="n">
+      <c r="D11" s="9" t="n">
         <f aca="false">(C11-B11)/B11</f>
         <v>0.394584997780737</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="8"/>
-      <c r="N11" s="42"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="9"/>
+      <c r="N11" s="46"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="23" t="n">
+      <c r="A12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="25" t="n">
         <v>2922</v>
       </c>
-      <c r="C12" s="23" t="n">
+      <c r="C12" s="25" t="n">
         <v>3341</v>
       </c>
-      <c r="D12" s="8" t="n">
+      <c r="D12" s="9" t="n">
         <f aca="false">(C12-B12)/B12</f>
         <v>0.143394934976044</v>
       </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="46"/>
-      <c r="N12" s="42"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="50"/>
+      <c r="N12" s="46"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="25" t="n">
+      <c r="A13" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="27" t="n">
         <v>4402</v>
       </c>
-      <c r="C13" s="25" t="n">
+      <c r="C13" s="27" t="n">
         <v>3233</v>
       </c>
-      <c r="D13" s="47" t="n">
+      <c r="D13" s="51" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>-0.265561108587006</v>
       </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="46"/>
-      <c r="N13" s="42"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="50"/>
+      <c r="N13" s="46"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="30" t="n">
+      <c r="A14" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="32" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>24383.65</v>
       </c>
-      <c r="C14" s="30" t="n">
+      <c r="C14" s="32" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>23517</v>
       </c>
-      <c r="D14" s="32" t="n">
+      <c r="D14" s="34" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>-0.0355422588496801</v>
       </c>
-      <c r="E14" s="30" t="n">
+      <c r="E14" s="32" t="n">
         <f aca="false">SUM(E2:E13)</f>
         <v>12256</v>
       </c>
-      <c r="F14" s="50" t="n">
+      <c r="F14" s="54" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>2.77317912006462</v>
       </c>
-      <c r="G14" s="50" t="n">
+      <c r="G14" s="54" t="n">
         <f aca="false">AVERAGE(G2:G13)</f>
         <v>0.602021750888365</v>
       </c>
-      <c r="N14" s="42"/>
+      <c r="N14" s="46"/>
     </row>
     <row r="15" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="51"/>
-      <c r="B15" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="53"/>
-      <c r="N15" s="42"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="57"/>
+      <c r="N15" s="46"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="51"/>
-      <c r="B16" s="54" t="n">
+      <c r="A16" s="55"/>
+      <c r="B16" s="58" t="n">
         <v>23383</v>
       </c>
-      <c r="C16" s="54" t="n">
+      <c r="C16" s="58" t="n">
         <v>23517</v>
       </c>
-      <c r="D16" s="55" t="n">
+      <c r="D16" s="59" t="n">
         <f aca="false">(C16-B16)/B16</f>
         <v>0.00573065902578797</v>
       </c>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="53"/>
-      <c r="N16" s="42"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="57"/>
+      <c r="N16" s="46"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
@@ -2624,10 +2724,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2644,368 +2744,392 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="8.89"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="79.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17"/>
-      <c r="B1" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="57" t="s">
+    <row r="1" customFormat="false" ht="50.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="19"/>
+      <c r="B1" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="C1" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="58"/>
-      <c r="M1" s="1" t="n">
-        <f aca="false">COUNTA(D2:D13)</f>
-        <v>2</v>
-      </c>
-      <c r="N1" s="5" t="s">
+      <c r="D1" s="61" t="s">
         <v>44</v>
       </c>
+      <c r="E1" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="62"/>
+      <c r="M1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="59" t="n">
+      <c r="A2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="63" t="n">
         <v>381400</v>
       </c>
-      <c r="C2" s="23" t="n">
+      <c r="C2" s="25" t="n">
         <v>358709</v>
       </c>
-      <c r="D2" s="23" t="n">
+      <c r="D2" s="25" t="n">
         <v>292117</v>
       </c>
-      <c r="E2" s="24" t="n">
+      <c r="E2" s="26" t="n">
         <f aca="false">(C2-B2)/B2</f>
         <v>-0.0594939695857368</v>
       </c>
-      <c r="F2" s="24" t="n">
+      <c r="F2" s="26" t="n">
         <f aca="false">(D2-C2)/C2</f>
         <v>-0.185643516053403</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="N2" s="9" t="s">
-        <v>45</v>
+      <c r="G2" s="62"/>
+      <c r="M2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="59" t="n">
+      <c r="A3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="63" t="n">
         <v>338378</v>
       </c>
-      <c r="C3" s="23" t="n">
+      <c r="C3" s="25" t="n">
         <v>320011</v>
       </c>
-      <c r="D3" s="23" t="n">
+      <c r="D3" s="25" t="n">
         <v>257282</v>
       </c>
-      <c r="E3" s="24" t="n">
+      <c r="E3" s="26" t="n">
         <f aca="false">(C3-B3)/B3</f>
         <v>-0.0542795335394145</v>
       </c>
-      <c r="F3" s="24" t="n">
+      <c r="F3" s="26" t="n">
         <f aca="false">(D3-C3)/C3</f>
         <v>-0.19602138676483</v>
       </c>
-      <c r="G3" s="58"/>
-      <c r="N3" s="9"/>
+      <c r="G3" s="62"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="59" t="n">
+      <c r="A4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="63" t="n">
         <v>354957</v>
       </c>
-      <c r="C4" s="23" t="n">
+      <c r="C4" s="25" t="n">
         <v>323736</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24" t="n">
+      <c r="D4" s="25"/>
+      <c r="E4" s="26" t="n">
         <f aca="false">(C4-B4)/B4</f>
         <v>-0.0879571328358083</v>
       </c>
-      <c r="F4" s="24" t="n">
+      <c r="F4" s="26" t="n">
         <f aca="false">(D4-C4)/C4</f>
         <v>-1</v>
       </c>
-      <c r="G4" s="58"/>
-      <c r="N4" s="9"/>
+      <c r="G4" s="62"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="59" t="n">
+      <c r="A5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="63" t="n">
         <v>329975</v>
       </c>
-      <c r="C5" s="23" t="n">
+      <c r="C5" s="25" t="n">
         <v>307995</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24" t="n">
+      <c r="D5" s="25"/>
+      <c r="E5" s="26" t="n">
         <f aca="false">(C5-B5)/B5</f>
         <v>-0.066611106902038</v>
       </c>
-      <c r="F5" s="24" t="n">
+      <c r="F5" s="26" t="n">
         <f aca="false">(D5-C5)/C5</f>
         <v>-1</v>
       </c>
-      <c r="G5" s="58"/>
-      <c r="N5" s="9"/>
+      <c r="G5" s="62"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="59" t="n">
+      <c r="A6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="63" t="n">
         <v>333225</v>
       </c>
-      <c r="C6" s="23" t="n">
+      <c r="C6" s="25" t="n">
         <v>305855</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24" t="n">
+      <c r="D6" s="25"/>
+      <c r="E6" s="26" t="n">
         <f aca="false">(C6-B6)/B6</f>
         <v>-0.0821366944256883</v>
       </c>
-      <c r="F6" s="24" t="n">
+      <c r="F6" s="26" t="n">
         <f aca="false">(D6-C6)/C6</f>
         <v>-1</v>
       </c>
-      <c r="G6" s="58"/>
-      <c r="N6" s="9"/>
+      <c r="G6" s="62"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="59" t="n">
+      <c r="A7" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="63" t="n">
         <v>319566</v>
       </c>
-      <c r="C7" s="23" t="n">
+      <c r="C7" s="25" t="n">
         <v>289224</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24" t="n">
+      <c r="D7" s="25"/>
+      <c r="E7" s="26" t="n">
         <f aca="false">(C7-B7)/B7</f>
         <v>-0.0949475225774957</v>
       </c>
-      <c r="F7" s="24" t="n">
+      <c r="F7" s="26" t="n">
         <f aca="false">(D7-C7)/C7</f>
         <v>-1</v>
       </c>
-      <c r="G7" s="58"/>
-      <c r="N7" s="9"/>
+      <c r="G7" s="62"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="59" t="n">
+      <c r="A8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="63" t="n">
         <v>345523</v>
       </c>
-      <c r="C8" s="23" t="n">
+      <c r="C8" s="25" t="n">
         <v>304267</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24" t="n">
+      <c r="D8" s="25"/>
+      <c r="E8" s="26" t="n">
         <f aca="false">(C8-B8)/B8</f>
         <v>-0.119401602787658</v>
       </c>
-      <c r="F8" s="24" t="n">
+      <c r="F8" s="26" t="n">
         <f aca="false">(D8-C8)/C8</f>
         <v>-1</v>
       </c>
-      <c r="G8" s="58"/>
-      <c r="N8" s="9"/>
+      <c r="G8" s="62"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="59" t="n">
+      <c r="A9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="63" t="n">
         <v>344469</v>
       </c>
-      <c r="C9" s="23" t="n">
+      <c r="C9" s="25" t="n">
         <v>314709</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24" t="n">
+      <c r="D9" s="25"/>
+      <c r="E9" s="26" t="n">
         <f aca="false">(C9-B9)/B9</f>
         <v>-0.0863938409552093</v>
       </c>
-      <c r="F9" s="24" t="n">
+      <c r="F9" s="26" t="n">
         <f aca="false">(D9-C9)/C9</f>
         <v>-1</v>
       </c>
-      <c r="G9" s="58"/>
-      <c r="N9" s="9"/>
+      <c r="G9" s="62"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="23" t="n">
+      <c r="A10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="25" t="n">
         <v>342330</v>
       </c>
-      <c r="C10" s="23" t="n">
+      <c r="C10" s="25" t="n">
         <v>300248</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24" t="n">
+      <c r="D10" s="25"/>
+      <c r="E10" s="26" t="n">
         <f aca="false">(C10-B10)/B10</f>
         <v>-0.122928168726083</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="58"/>
-      <c r="N10" s="9"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="62"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="23" t="n">
+      <c r="A11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="25" t="n">
         <v>367756</v>
       </c>
-      <c r="C11" s="23" t="n">
+      <c r="C11" s="25" t="n">
         <v>303597</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24" t="n">
+      <c r="D11" s="25"/>
+      <c r="E11" s="26" t="n">
         <f aca="false">(C11-B11)/B11</f>
         <v>-0.17446078378055</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="58"/>
-      <c r="N11" s="9"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="62"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="23" t="n">
+      <c r="A12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="25" t="n">
         <v>392032</v>
       </c>
-      <c r="C12" s="23" t="n">
+      <c r="C12" s="25" t="n">
         <v>300258</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24" t="n">
+      <c r="D12" s="25"/>
+      <c r="E12" s="26" t="n">
         <f aca="false">(C12-B12)/B12</f>
         <v>-0.234098236878622</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="58"/>
-      <c r="N12" s="9"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="62"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="60" t="n">
+      <c r="A13" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="64" t="n">
         <v>415125</v>
       </c>
-      <c r="C13" s="23" t="n">
+      <c r="C13" s="25" t="n">
         <v>316760</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24" t="n">
+      <c r="D13" s="25"/>
+      <c r="E13" s="26" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>-0.236952725082806</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="58"/>
-      <c r="N13" s="9"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="62"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="61" t="n">
+      <c r="A14" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="65" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>4264736</v>
       </c>
-      <c r="C14" s="61" t="n">
+      <c r="C14" s="65" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>3745369</v>
       </c>
-      <c r="D14" s="61" t="n">
+      <c r="D14" s="65" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>549399</v>
       </c>
-      <c r="E14" s="31" t="n">
+      <c r="E14" s="33" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>-0.121781746865457</v>
       </c>
-      <c r="F14" s="31" t="n">
+      <c r="F14" s="33" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>-0.797708112852279</v>
       </c>
-      <c r="G14" s="58"/>
-      <c r="N14" s="9"/>
-    </row>
-    <row r="15" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="62"/>
-      <c r="B15" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="63"/>
-      <c r="E15" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="64"/>
-      <c r="G15" s="58"/>
-      <c r="M15" s="65"/>
-      <c r="N15" s="9"/>
+      <c r="G14" s="62"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="10"/>
+    </row>
+    <row r="15" customFormat="false" ht="30.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="66"/>
+      <c r="B15" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="67"/>
+      <c r="E15" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="68"/>
+      <c r="G15" s="62"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="62"/>
-      <c r="B16" s="23" t="n">
+      <c r="A16" s="66"/>
+      <c r="B16" s="25" t="n">
         <v>4382326</v>
       </c>
-      <c r="C16" s="23" t="n">
+      <c r="C16" s="25" t="n">
         <f aca="false">C14</f>
         <v>3745369</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="24" t="n">
+      <c r="D16" s="25"/>
+      <c r="E16" s="26" t="n">
         <f aca="false">(C16-B16)/C16</f>
         <v>-0.170065219208041</v>
       </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="58"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="9"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="62"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N17" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N18" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="M17" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M18" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3015,10 +3139,19 @@
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
-  <mergeCells count="1">
+  <mergeCells count="4">
+    <mergeCell ref="M2:M16"/>
     <mergeCell ref="N2:N16"/>
+    <mergeCell ref="M17:R17"/>
+    <mergeCell ref="M18:R18"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3039,7 +3172,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3056,309 +3189,305 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17"/>
-      <c r="B1" s="67" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="67" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="68" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="1" t="n">
-        <f aca="false">COUNTA(D2:D13)</f>
-        <v>8</v>
-      </c>
-      <c r="N1" s="5"/>
+      <c r="A1" s="19"/>
+      <c r="B1" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="70" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="43"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="69" t="n">
+      <c r="A2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="71" t="n">
         <v>166018</v>
       </c>
-      <c r="C2" s="69" t="n">
+      <c r="C2" s="71" t="n">
         <v>154290</v>
       </c>
-      <c r="D2" s="23" t="n">
+      <c r="D2" s="25" t="n">
         <v>137349</v>
       </c>
-      <c r="E2" s="70" t="n">
+      <c r="E2" s="72" t="n">
         <f aca="false">(C2-B2)/B2</f>
         <v>-0.0706429423315544</v>
       </c>
-      <c r="F2" s="24" t="n">
+      <c r="F2" s="26" t="n">
         <f aca="false">(D2-C2)/C2</f>
         <v>-0.109799727785339</v>
       </c>
-      <c r="N2" s="41"/>
+      <c r="N2" s="45"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="71" t="n">
+      <c r="A3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="73" t="n">
         <v>153234</v>
       </c>
-      <c r="C3" s="69" t="n">
+      <c r="C3" s="71" t="n">
         <v>139138</v>
       </c>
-      <c r="D3" s="23" t="n">
+      <c r="D3" s="25" t="n">
         <v>126757</v>
       </c>
-      <c r="E3" s="70" t="n">
+      <c r="E3" s="72" t="n">
         <f aca="false">(C3-B3)/B3</f>
         <v>-0.091990028322696</v>
       </c>
-      <c r="F3" s="24" t="n">
+      <c r="F3" s="26" t="n">
         <f aca="false">(D3-C3)/C3</f>
         <v>-0.0889835990168035</v>
       </c>
-      <c r="N3" s="42"/>
+      <c r="N3" s="46"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="69" t="n">
+      <c r="A4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="71" t="n">
         <v>149129</v>
       </c>
-      <c r="C4" s="69" t="n">
+      <c r="C4" s="71" t="n">
         <v>139609</v>
       </c>
-      <c r="D4" s="23" t="n">
+      <c r="D4" s="25" t="n">
         <v>117550</v>
       </c>
-      <c r="E4" s="70" t="n">
+      <c r="E4" s="72" t="n">
         <f aca="false">(C4-B4)/B4</f>
         <v>-0.0638373488724527</v>
       </c>
-      <c r="F4" s="24" t="n">
+      <c r="F4" s="26" t="n">
         <f aca="false">(D4-C4)/C4</f>
         <v>-0.158005572706631</v>
       </c>
-      <c r="N4" s="42"/>
+      <c r="N4" s="46"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="69" t="n">
+      <c r="A5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="71" t="n">
         <v>146506</v>
       </c>
-      <c r="C5" s="69" t="n">
+      <c r="C5" s="71" t="n">
         <v>126227</v>
       </c>
-      <c r="D5" s="23" t="n">
+      <c r="D5" s="25" t="n">
         <v>113477</v>
       </c>
-      <c r="E5" s="70" t="n">
+      <c r="E5" s="72" t="n">
         <f aca="false">(C5-B5)/B5</f>
         <v>-0.138417539213411</v>
       </c>
-      <c r="F5" s="24" t="n">
+      <c r="F5" s="26" t="n">
         <f aca="false">(D5-C5)/C5</f>
         <v>-0.101008500558518</v>
       </c>
-      <c r="N5" s="42"/>
+      <c r="N5" s="46"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="69" t="n">
+      <c r="A6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="71" t="n">
         <v>122937</v>
       </c>
-      <c r="C6" s="69" t="n">
+      <c r="C6" s="71" t="n">
         <v>128749</v>
       </c>
-      <c r="D6" s="23" t="n">
+      <c r="D6" s="25" t="n">
         <v>108336</v>
       </c>
-      <c r="E6" s="70" t="n">
+      <c r="E6" s="72" t="n">
         <f aca="false">(C6-B6)/B6</f>
         <v>0.0472762471835168</v>
       </c>
-      <c r="F6" s="24" t="n">
+      <c r="F6" s="26" t="n">
         <f aca="false">(D6-C6)/C6</f>
         <v>-0.158548804262557</v>
       </c>
-      <c r="N6" s="42"/>
+      <c r="N6" s="46"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="69" t="n">
+      <c r="A7" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="71" t="n">
         <v>113710</v>
       </c>
-      <c r="C7" s="69" t="n">
+      <c r="C7" s="71" t="n">
         <v>125671</v>
       </c>
-      <c r="D7" s="23" t="n">
+      <c r="D7" s="25" t="n">
         <v>98523</v>
       </c>
-      <c r="E7" s="70" t="n">
+      <c r="E7" s="72" t="n">
         <f aca="false">(C7-B7)/B7</f>
         <v>0.10518863776273</v>
       </c>
-      <c r="F7" s="24" t="n">
+      <c r="F7" s="26" t="n">
         <f aca="false">(D7-C7)/C7</f>
         <v>-0.216024381122136</v>
       </c>
-      <c r="N7" s="42"/>
+      <c r="N7" s="46"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="69" t="n">
+      <c r="A8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="71" t="n">
         <v>117122</v>
       </c>
-      <c r="C8" s="69" t="n">
+      <c r="C8" s="71" t="n">
         <v>147302</v>
       </c>
-      <c r="D8" s="23" t="n">
+      <c r="D8" s="25" t="n">
         <v>103029</v>
       </c>
-      <c r="E8" s="70" t="n">
+      <c r="E8" s="72" t="n">
         <f aca="false">(C8-B8)/B8</f>
         <v>0.257680025955841</v>
       </c>
-      <c r="F8" s="24" t="n">
+      <c r="F8" s="26" t="n">
         <f aca="false">(D8-C8)/C8</f>
         <v>-0.300559394984454</v>
       </c>
-      <c r="N8" s="42"/>
+      <c r="N8" s="46"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="69" t="n">
+      <c r="A9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="71" t="n">
         <v>126623</v>
       </c>
-      <c r="C9" s="69" t="n">
+      <c r="C9" s="71" t="n">
         <v>145461</v>
       </c>
-      <c r="D9" s="23" t="n">
+      <c r="D9" s="25" t="n">
         <v>115694</v>
       </c>
-      <c r="E9" s="70" t="n">
+      <c r="E9" s="72" t="n">
         <f aca="false">(C9-B9)/B9</f>
         <v>0.148772339938242</v>
       </c>
-      <c r="F9" s="24" t="n">
+      <c r="F9" s="26" t="n">
         <f aca="false">(D9-C9)/C9</f>
         <v>-0.204639044142416</v>
       </c>
-      <c r="N9" s="42"/>
+      <c r="N9" s="46"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="69" t="n">
+      <c r="A10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="71" t="n">
         <v>122360</v>
       </c>
-      <c r="C10" s="69" t="n">
+      <c r="C10" s="71" t="n">
         <v>149470</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="70" t="n">
+      <c r="D10" s="25"/>
+      <c r="E10" s="72" t="n">
         <f aca="false">(C10-B10)/B10</f>
         <v>0.221559333115397</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="N10" s="42"/>
+      <c r="F10" s="26"/>
+      <c r="N10" s="46"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="69" t="n">
+      <c r="A11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="71" t="n">
         <v>132280</v>
       </c>
-      <c r="C11" s="69" t="n">
+      <c r="C11" s="71" t="n">
         <v>165507</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="70" t="n">
+      <c r="D11" s="25"/>
+      <c r="E11" s="72" t="n">
         <f aca="false">(C11-B11)/B11</f>
         <v>0.251186876322951</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="N11" s="42"/>
+      <c r="F11" s="26"/>
+      <c r="N11" s="46"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="69" t="n">
+      <c r="A12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="71" t="n">
         <v>128303</v>
       </c>
-      <c r="C12" s="69" t="n">
+      <c r="C12" s="71" t="n">
         <v>162736</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="70" t="n">
+      <c r="D12" s="25"/>
+      <c r="E12" s="72" t="n">
         <f aca="false">(C12-B12)/B12</f>
         <v>0.268372524414862</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="N12" s="42"/>
+      <c r="F12" s="26"/>
+      <c r="N12" s="46"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="69" t="n">
+      <c r="A13" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="71" t="n">
         <v>132120</v>
       </c>
-      <c r="C13" s="69" t="n">
+      <c r="C13" s="71" t="n">
         <v>165619</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="70" t="n">
+      <c r="D13" s="25"/>
+      <c r="E13" s="72" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>0.253549803209204</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="N13" s="42"/>
+      <c r="F13" s="26"/>
+      <c r="N13" s="46"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="61" t="n">
+      <c r="A14" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="65" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>1610342</v>
       </c>
-      <c r="C14" s="61" t="n">
+      <c r="C14" s="65" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>1749779</v>
       </c>
-      <c r="D14" s="61" t="n">
+      <c r="D14" s="65" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>920715</v>
       </c>
-      <c r="E14" s="31" t="n">
+      <c r="E14" s="33" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>0.0865884389775588</v>
       </c>
-      <c r="F14" s="31" t="n">
+      <c r="F14" s="33" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>-0.167196128072357</v>
       </c>
-      <c r="N14" s="42"/>
+      <c r="N14" s="46"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3380,10 +3509,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4"/>
+      <selection pane="topLeft" activeCell="Q15" activeCellId="0" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3394,426 +3523,452 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="32.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="8.89"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17"/>
-      <c r="B1" s="72" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" s="73" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" s="74" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="73" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="M1" s="1" t="n">
-        <f aca="false">COUNTA(D2:D13)</f>
-        <v>2</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>54</v>
+    <row r="1" customFormat="false" ht="30.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="19"/>
+      <c r="B1" s="74" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="M1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="23" t="n">
+      <c r="A2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="25" t="n">
         <v>40365</v>
       </c>
-      <c r="C2" s="23" t="n">
+      <c r="C2" s="25" t="n">
         <v>41888</v>
       </c>
-      <c r="D2" s="23" t="n">
+      <c r="D2" s="25" t="n">
         <v>46250</v>
       </c>
-      <c r="E2" s="24" t="n">
+      <c r="E2" s="26" t="n">
         <f aca="false">(C2-B2)/B2</f>
         <v>0.0377307072959247</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="9" t="n">
         <f aca="false">(D2-C2)/C2</f>
         <v>0.104134835752483</v>
       </c>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="N2" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="M2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="23" t="n">
+      <c r="N2" s="77" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="25" t="n">
         <v>37545</v>
       </c>
-      <c r="C3" s="40" t="n">
+      <c r="C3" s="44" t="n">
         <v>50219</v>
       </c>
-      <c r="D3" s="23" t="n">
+      <c r="D3" s="25" t="n">
         <v>33335</v>
       </c>
-      <c r="E3" s="24" t="n">
+      <c r="E3" s="26" t="n">
         <f aca="false">(C3-B3)/B3</f>
         <v>0.337568251431615</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="9" t="n">
         <f aca="false">(D3-C3)/C3</f>
         <v>-0.336207411537466</v>
       </c>
-      <c r="G3" s="75" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="N3" s="9"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="23" t="n">
+      <c r="G3" s="78" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="77"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="25" t="n">
         <v>25781.81</v>
       </c>
-      <c r="C4" s="40" t="n">
+      <c r="C4" s="44" t="n">
         <v>45023</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24" t="n">
+      <c r="D4" s="25"/>
+      <c r="E4" s="26" t="n">
         <f aca="false">(C4-B4)/B4</f>
         <v>0.746308734724211</v>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="9" t="n">
         <f aca="false">(D4-C4)/C4</f>
         <v>-1</v>
       </c>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="N4" s="9"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="23" t="n">
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="77"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="25" t="n">
         <v>25781.81</v>
       </c>
-      <c r="C5" s="40" t="n">
+      <c r="C5" s="44" t="n">
         <v>25839</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24" t="n">
+      <c r="D5" s="25"/>
+      <c r="E5" s="26" t="n">
         <f aca="false">(C5-B5)/B5</f>
         <v>0.00221823060522123</v>
       </c>
-      <c r="F5" s="8" t="n">
+      <c r="F5" s="9" t="n">
         <f aca="false">(D5-C5)/C5</f>
         <v>-1</v>
       </c>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="N5" s="9"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="23" t="n">
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="77"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="25" t="n">
         <v>13432.28</v>
       </c>
-      <c r="C6" s="40" t="n">
+      <c r="C6" s="44" t="n">
         <v>12769</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24" t="n">
+      <c r="D6" s="25"/>
+      <c r="E6" s="26" t="n">
         <f aca="false">(C6-B6)/B6</f>
         <v>-0.0493795543273369</v>
       </c>
-      <c r="F6" s="8" t="n">
+      <c r="F6" s="9" t="n">
         <f aca="false">(D6-C6)/C6</f>
         <v>-1</v>
       </c>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="N6" s="9"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="23" t="n">
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="77"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="25" t="n">
         <v>15430.56</v>
       </c>
-      <c r="C7" s="40" t="n">
+      <c r="C7" s="44" t="n">
         <v>10444</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24" t="n">
+      <c r="D7" s="25"/>
+      <c r="E7" s="26" t="n">
         <f aca="false">(C7-B7)/B7</f>
         <v>-0.323161311060648</v>
       </c>
-      <c r="F7" s="8" t="n">
+      <c r="F7" s="9" t="n">
         <f aca="false">(D7-C7)/C7</f>
         <v>-1</v>
       </c>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="N7" s="9"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="23" t="n">
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="77"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="25" t="n">
         <v>7210.53</v>
       </c>
-      <c r="C8" s="23" t="n">
+      <c r="C8" s="25" t="n">
         <v>9191</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24" t="n">
+      <c r="D8" s="25"/>
+      <c r="E8" s="26" t="n">
         <f aca="false">(C8-B8)/B8</f>
         <v>0.274663582288681</v>
       </c>
-      <c r="F8" s="8" t="n">
+      <c r="F8" s="9" t="n">
         <f aca="false">(D8-C8)/C8</f>
         <v>-1</v>
       </c>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="N8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="23" t="n">
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="57"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="77"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="25" t="n">
         <v>7045.99</v>
       </c>
-      <c r="C9" s="23" t="n">
+      <c r="C9" s="25" t="n">
         <v>11379</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24" t="n">
+      <c r="D9" s="25"/>
+      <c r="E9" s="26" t="n">
         <f aca="false">(C9-B9)/B9</f>
         <v>0.614961133921564</v>
       </c>
-      <c r="F9" s="8" t="n">
+      <c r="F9" s="9" t="n">
         <f aca="false">(D9-C9)/C9</f>
         <v>-1</v>
       </c>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="N9" s="9"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="25" t="n">
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="77"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="69" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="27" t="n">
         <v>23032</v>
       </c>
-      <c r="C10" s="23" t="n">
+      <c r="C10" s="25" t="n">
         <v>11779</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="27" t="n">
+      <c r="D10" s="25"/>
+      <c r="E10" s="29" t="n">
         <f aca="false">(C10-B10)/B10</f>
         <v>-0.488581104550191</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="N10" s="9"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="25" t="n">
+      <c r="F10" s="9"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="77"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="69" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="27" t="n">
         <v>36770</v>
       </c>
-      <c r="C11" s="23" t="n">
+      <c r="C11" s="25" t="n">
         <v>23418</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="27" t="n">
+      <c r="D11" s="25"/>
+      <c r="E11" s="29" t="n">
         <f aca="false">(C11-B11)/B11</f>
         <v>-0.3631221104161</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="N11" s="9"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="25" t="n">
+      <c r="F11" s="9"/>
+      <c r="G11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="77"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="27" t="n">
         <v>40381</v>
       </c>
-      <c r="C12" s="23" t="n">
+      <c r="C12" s="25" t="n">
         <v>34717</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="27" t="n">
+      <c r="D12" s="25"/>
+      <c r="E12" s="29" t="n">
         <f aca="false">(C12-B12)/B12</f>
         <v>-0.140263985537753</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="N12" s="9"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="76" t="n">
+      <c r="F12" s="9"/>
+      <c r="G12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="77"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="79" t="n">
         <v>34355</v>
       </c>
-      <c r="C13" s="23" t="n">
+      <c r="C13" s="25" t="n">
         <v>36455</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24" t="n">
+      <c r="D13" s="25"/>
+      <c r="E13" s="26" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>0.0611264735846311</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="N13" s="9"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="61" t="n">
+      <c r="F13" s="9"/>
+      <c r="G13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="77"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="65" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>307130.98</v>
       </c>
-      <c r="C14" s="61" t="n">
+      <c r="C14" s="65" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>313121</v>
       </c>
-      <c r="D14" s="30" t="n">
+      <c r="D14" s="32" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>79585</v>
       </c>
-      <c r="E14" s="31" t="n">
+      <c r="E14" s="33" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>0.0195031448797514</v>
       </c>
-      <c r="F14" s="32" t="n">
+      <c r="F14" s="34" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>-0.779009071973123</v>
       </c>
-      <c r="G14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="N14" s="9"/>
-    </row>
-    <row r="15" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="77"/>
-      <c r="B15" s="78" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="78" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="78"/>
-      <c r="E15" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="79"/>
-      <c r="G15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="N15" s="9"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="77"/>
-      <c r="B16" s="80" t="n">
+      <c r="G14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="77"/>
+    </row>
+    <row r="15" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="80"/>
+      <c r="B15" s="81" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="81" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="81"/>
+      <c r="E15" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="82"/>
+      <c r="G15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="77"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="80"/>
+      <c r="B16" s="83" t="n">
         <v>331445.11</v>
       </c>
-      <c r="C16" s="80" t="n">
+      <c r="C16" s="83" t="n">
         <v>272775.98</v>
       </c>
-      <c r="D16" s="78"/>
-      <c r="E16" s="8" t="n">
+      <c r="D16" s="81"/>
+      <c r="E16" s="9" t="n">
         <f aca="false">(C16-B16)/C16</f>
         <v>-0.215081731170025</v>
       </c>
-      <c r="F16" s="79"/>
-      <c r="G16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="N16" s="9"/>
+      <c r="F16" s="82"/>
+      <c r="G16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="77"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N17" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N18" s="9" t="s">
-        <v>59</v>
-      </c>
+      <c r="M17" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M18" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3831,9 +3986,12 @@
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
-  <mergeCells count="2">
+  <mergeCells count="5">
+    <mergeCell ref="M2:M16"/>
     <mergeCell ref="N2:N16"/>
     <mergeCell ref="G3:K3"/>
+    <mergeCell ref="M17:R17"/>
+    <mergeCell ref="M18:R18"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Move charts to the top of the slide
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Waste" sheetId="1" state="visible" r:id="rId2"/>
@@ -725,7 +725,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="63">
   <si>
     <t xml:space="preserve">Waste</t>
   </si>
@@ -811,6 +811,9 @@
     <t xml:space="preserve">Top tip!</t>
   </si>
   <si>
+    <t xml:space="preserve">Cabot Circus uses state-of-the-art rainwater harvesting technology, which helps reduce water waste!</t>
+  </si>
+  <si>
     <t xml:space="preserve">2015 Water</t>
   </si>
   <si>
@@ -823,9 +826,6 @@
     <t xml:space="preserve">Nothing to report? Try using this comment for the water slide:</t>
   </si>
   <si>
-    <t xml:space="preserve">Cabot Circus uses state-of-the-art rainwater harvesting technology, which helps reduce water waste!</t>
-  </si>
-  <si>
     <t xml:space="preserve">Landlord Water only</t>
   </si>
   <si>
@@ -901,10 +901,7 @@
     <t xml:space="preserve">Gas 2019 (kWh)</t>
   </si>
   <si>
-    <t xml:space="preserve">This month, we’re up.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We always strive to be transparent with our customers. This month, we’re up for our gas usage. We will try better next time.</t>
+    <t xml:space="preserve">Using a machine known as an anaerobic digester, we convert tons of food waste back into energy!</t>
   </si>
   <si>
     <t xml:space="preserve">Reporting on invoice consumption not meter reads.</t>
@@ -917,9 +914,6 @@
   </si>
   <si>
     <t xml:space="preserve">Nothing to report? Try using this comment for the gas slide:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using a machine known as an anaerobic digester, we convert tons of food waste back into energy!</t>
   </si>
 </sst>
 </file>
@@ -936,7 +930,7 @@
     <numFmt numFmtId="170" formatCode="0.00%"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -994,6 +988,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1195,7 +1195,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1304,6 +1304,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -1316,11 +1320,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1328,7 +1332,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1340,11 +1344,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1385,7 +1389,7 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1412,7 +1416,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1424,7 +1428,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1436,7 +1440,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1444,11 +1448,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1456,7 +1460,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1504,7 +1508,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1520,7 +1524,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1608,7 +1612,7 @@
   </sheetPr>
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I32" activeCellId="0" sqref="I32"/>
     </sheetView>
   </sheetViews>
@@ -1902,7 +1906,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1961,8 +1965,8 @@
       <c r="M2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="10" t="s">
-        <v>8</v>
+      <c r="N2" s="27" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1987,7 +1991,7 @@
         <v>-0.0658448150833938</v>
       </c>
       <c r="M3" s="5"/>
-      <c r="N3" s="10"/>
+      <c r="N3" s="27"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
@@ -2009,7 +2013,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M4" s="5"/>
-      <c r="N4" s="10"/>
+      <c r="N4" s="27"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
@@ -2031,7 +2035,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M5" s="5"/>
-      <c r="N5" s="10"/>
+      <c r="N5" s="27"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
@@ -2040,7 +2044,7 @@
       <c r="B6" s="24" t="n">
         <v>6577</v>
       </c>
-      <c r="C6" s="27" t="n">
+      <c r="C6" s="28" t="n">
         <v>10387</v>
       </c>
       <c r="D6" s="25"/>
@@ -2053,7 +2057,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M6" s="5"/>
-      <c r="N6" s="10"/>
+      <c r="N6" s="27"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
@@ -2062,7 +2066,7 @@
       <c r="B7" s="24" t="n">
         <v>7009</v>
       </c>
-      <c r="C7" s="27" t="n">
+      <c r="C7" s="28" t="n">
         <v>8235</v>
       </c>
       <c r="D7" s="25"/>
@@ -2075,7 +2079,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M7" s="5"/>
-      <c r="N7" s="10"/>
+      <c r="N7" s="27"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
@@ -2097,7 +2101,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M8" s="5"/>
-      <c r="N8" s="10"/>
+      <c r="N8" s="27"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
@@ -2119,7 +2123,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M9" s="5"/>
-      <c r="N9" s="10"/>
+      <c r="N9" s="27"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
@@ -2141,7 +2145,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M10" s="5"/>
-      <c r="N10" s="10"/>
+      <c r="N10" s="27"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
@@ -2160,7 +2164,7 @@
       </c>
       <c r="F11" s="9"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="10"/>
+      <c r="N11" s="27"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19" t="s">
@@ -2179,71 +2183,71 @@
       </c>
       <c r="F12" s="9"/>
       <c r="M12" s="5"/>
-      <c r="N12" s="10"/>
+      <c r="N12" s="27"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="28" t="n">
+      <c r="B13" s="29" t="n">
         <v>8881</v>
       </c>
       <c r="C13" s="25" t="n">
         <v>6912</v>
       </c>
       <c r="D13" s="25"/>
-      <c r="E13" s="29" t="n">
+      <c r="E13" s="30" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>-0.22170926697444</v>
       </c>
       <c r="F13" s="9"/>
       <c r="M13" s="5"/>
-      <c r="N13" s="10"/>
+      <c r="N13" s="27"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="31" t="n">
+      <c r="B14" s="32" t="n">
         <v>77704</v>
       </c>
-      <c r="C14" s="32" t="n">
+      <c r="C14" s="33" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>96849</v>
       </c>
-      <c r="D14" s="32" t="n">
+      <c r="D14" s="33" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>14960</v>
       </c>
-      <c r="E14" s="33" t="n">
+      <c r="E14" s="34" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>0.24638371255019</v>
       </c>
-      <c r="F14" s="34" t="e">
+      <c r="F14" s="35" t="e">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M14" s="5"/>
-      <c r="N14" s="10"/>
+      <c r="N14" s="27"/>
     </row>
     <row r="15" customFormat="false" ht="43.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="19"/>
       <c r="B15" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" s="19"/>
-      <c r="E15" s="35" t="s">
-        <v>30</v>
+      <c r="E15" s="36" t="s">
+        <v>31</v>
       </c>
       <c r="F15" s="19"/>
       <c r="M15" s="5"/>
-      <c r="N15" s="10"/>
+      <c r="N15" s="27"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="35"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="25" t="n">
         <v>81734</v>
       </c>
@@ -2251,17 +2255,17 @@
         <v>77704</v>
       </c>
       <c r="D16" s="19"/>
-      <c r="E16" s="36" t="n">
+      <c r="E16" s="37" t="n">
         <f aca="false">(C16-B16)/B16</f>
         <v>-0.0493062862456261</v>
       </c>
-      <c r="F16" s="37"/>
+      <c r="F16" s="38"/>
       <c r="M16" s="5"/>
-      <c r="N16" s="10"/>
+      <c r="N16" s="27"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M17" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N17" s="17"/>
       <c r="O17" s="17"/>
@@ -2271,15 +2275,15 @@
       <c r="S17" s="17"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M18" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="N18" s="38"/>
-      <c r="O18" s="38"/>
-      <c r="P18" s="38"/>
-      <c r="Q18" s="38"/>
-      <c r="R18" s="38"/>
-      <c r="S18" s="38"/>
+      <c r="M18" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" s="39"/>
+      <c r="O18" s="39"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="39"/>
+      <c r="R18" s="39"/>
+      <c r="S18" s="39"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2334,37 +2338,37 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="43"/>
+      <c r="N1" s="44"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="44" t="n">
+      <c r="B2" s="45" t="n">
         <v>1217</v>
       </c>
-      <c r="C2" s="44" t="n">
+      <c r="C2" s="45" t="n">
         <v>224</v>
       </c>
       <c r="D2" s="9" t="n">
@@ -2382,16 +2386,16 @@
         <f aca="false">(E2-B2)/B2</f>
         <v>0.226787181594084</v>
       </c>
-      <c r="N2" s="45"/>
+      <c r="N2" s="46"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="44" t="n">
+      <c r="B3" s="45" t="n">
         <v>1518.25</v>
       </c>
-      <c r="C3" s="44" t="n">
+      <c r="C3" s="45" t="n">
         <v>221</v>
       </c>
       <c r="D3" s="9" t="n">
@@ -2409,16 +2413,16 @@
         <f aca="false">(E3-B3)/B3</f>
         <v>-0.126626049728306</v>
       </c>
-      <c r="N3" s="46"/>
+      <c r="N3" s="47"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="44" t="n">
+      <c r="B4" s="45" t="n">
         <v>1203.4</v>
       </c>
-      <c r="C4" s="44" t="n">
+      <c r="C4" s="45" t="n">
         <v>203</v>
       </c>
       <c r="D4" s="9" t="n">
@@ -2436,7 +2440,7 @@
         <f aca="false">(E4-B4)/B4</f>
         <v>-0.15738740235998</v>
       </c>
-      <c r="N4" s="46"/>
+      <c r="N4" s="47"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
@@ -2463,7 +2467,7 @@
         <f aca="false">(E5-B5)/B5</f>
         <v>0.892045454545455</v>
       </c>
-      <c r="N5" s="46"/>
+      <c r="N5" s="47"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
@@ -2479,7 +2483,7 @@
         <f aca="false">(C6-B6)/B6</f>
         <v>0.375791139240506</v>
       </c>
-      <c r="E6" s="27" t="n">
+      <c r="E6" s="28" t="n">
         <v>3212</v>
       </c>
       <c r="F6" s="9" t="n">
@@ -2490,7 +2494,7 @@
         <f aca="false">(E6-B6)/B6</f>
         <v>1.54113924050633</v>
       </c>
-      <c r="N6" s="46"/>
+      <c r="N6" s="47"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
@@ -2506,10 +2510,10 @@
         <f aca="false">(C7-B7)/B7</f>
         <v>0.626865671641791</v>
       </c>
-      <c r="E7" s="27" t="n">
+      <c r="E7" s="28" t="n">
         <v>2547</v>
       </c>
-      <c r="F7" s="47" t="n">
+      <c r="F7" s="48" t="n">
         <f aca="false">(E7-C7)/C7</f>
         <v>0.374527792768483</v>
       </c>
@@ -2517,7 +2521,7 @@
         <f aca="false">(E7-B7)/B7</f>
         <v>1.23617208077261</v>
       </c>
-      <c r="N7" s="46"/>
+      <c r="N7" s="47"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
@@ -2534,9 +2538,9 @@
         <v>-0.143830128205128</v>
       </c>
       <c r="E8" s="25"/>
-      <c r="F8" s="48"/>
+      <c r="F8" s="49"/>
       <c r="G8" s="9"/>
-      <c r="N8" s="46"/>
+      <c r="N8" s="47"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
@@ -2553,9 +2557,9 @@
         <v>0.236727589208007</v>
       </c>
       <c r="E9" s="25"/>
-      <c r="F9" s="48"/>
+      <c r="F9" s="49"/>
       <c r="G9" s="9"/>
-      <c r="N9" s="46"/>
+      <c r="N9" s="47"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
@@ -2572,9 +2576,9 @@
         <v>0.354838709677419</v>
       </c>
       <c r="E10" s="25"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="49"/>
-      <c r="N10" s="46"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="50"/>
+      <c r="N10" s="47"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
@@ -2591,9 +2595,9 @@
         <v>0.394584997780737</v>
       </c>
       <c r="E11" s="25"/>
-      <c r="F11" s="48"/>
+      <c r="F11" s="49"/>
       <c r="G11" s="9"/>
-      <c r="N11" s="46"/>
+      <c r="N11" s="47"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19" t="s">
@@ -2610,91 +2614,91 @@
         <v>0.143394934976044</v>
       </c>
       <c r="E12" s="25"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="50"/>
-      <c r="N12" s="46"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="51"/>
+      <c r="N12" s="47"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="27" t="n">
+      <c r="B13" s="28" t="n">
         <v>4402</v>
       </c>
-      <c r="C13" s="27" t="n">
+      <c r="C13" s="28" t="n">
         <v>3233</v>
       </c>
-      <c r="D13" s="51" t="n">
+      <c r="D13" s="52" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>-0.265561108587006</v>
       </c>
       <c r="E13" s="25"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="50"/>
-      <c r="N13" s="46"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="51"/>
+      <c r="N13" s="47"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="32" t="n">
+      <c r="B14" s="33" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>24383.65</v>
       </c>
-      <c r="C14" s="32" t="n">
+      <c r="C14" s="33" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>23517</v>
       </c>
-      <c r="D14" s="34" t="n">
+      <c r="D14" s="35" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>-0.0355422588496801</v>
       </c>
-      <c r="E14" s="32" t="n">
+      <c r="E14" s="33" t="n">
         <f aca="false">SUM(E2:E13)</f>
         <v>12256</v>
       </c>
-      <c r="F14" s="54" t="n">
+      <c r="F14" s="55" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>2.77317912006462</v>
       </c>
-      <c r="G14" s="54" t="n">
+      <c r="G14" s="55" t="n">
         <f aca="false">AVERAGE(G2:G13)</f>
         <v>0.602021750888365</v>
       </c>
-      <c r="N14" s="46"/>
+      <c r="N14" s="47"/>
     </row>
     <row r="15" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="55"/>
-      <c r="B15" s="56" t="s">
+      <c r="A15" s="56"/>
+      <c r="B15" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="57"/>
-      <c r="N15" s="46"/>
+      <c r="D15" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="58"/>
+      <c r="N15" s="47"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="55"/>
-      <c r="B16" s="58" t="n">
+      <c r="A16" s="56"/>
+      <c r="B16" s="59" t="n">
         <v>23383</v>
       </c>
-      <c r="C16" s="58" t="n">
+      <c r="C16" s="59" t="n">
         <v>23517</v>
       </c>
-      <c r="D16" s="59" t="n">
+      <c r="D16" s="60" t="n">
         <f aca="false">(C16-B16)/B16</f>
         <v>0.00573065902578797</v>
       </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="57"/>
-      <c r="N16" s="46"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="58"/>
+      <c r="N16" s="47"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
@@ -2736,22 +2740,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="50.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19"/>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="F1" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="62"/>
+      <c r="G1" s="63"/>
       <c r="M1" s="5" t="s">
         <v>4</v>
       </c>
@@ -2763,7 +2767,7 @@
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="63" t="n">
+      <c r="B2" s="64" t="n">
         <v>381400</v>
       </c>
       <c r="C2" s="25" t="n">
@@ -2780,7 +2784,7 @@
         <f aca="false">(D2-C2)/C2</f>
         <v>-0.185643516053403</v>
       </c>
-      <c r="G2" s="62"/>
+      <c r="G2" s="63"/>
       <c r="M2" s="5" t="s">
         <v>7</v>
       </c>
@@ -2792,7 +2796,7 @@
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="63" t="n">
+      <c r="B3" s="64" t="n">
         <v>338378</v>
       </c>
       <c r="C3" s="25" t="n">
@@ -2809,7 +2813,7 @@
         <f aca="false">(D3-C3)/C3</f>
         <v>-0.19602138676483</v>
       </c>
-      <c r="G3" s="62"/>
+      <c r="G3" s="63"/>
       <c r="M3" s="5"/>
       <c r="N3" s="10"/>
     </row>
@@ -2817,7 +2821,7 @@
       <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="63" t="n">
+      <c r="B4" s="64" t="n">
         <v>354957</v>
       </c>
       <c r="C4" s="25" t="n">
@@ -2832,7 +2836,7 @@
         <f aca="false">(D4-C4)/C4</f>
         <v>-1</v>
       </c>
-      <c r="G4" s="62"/>
+      <c r="G4" s="63"/>
       <c r="M4" s="5"/>
       <c r="N4" s="10"/>
     </row>
@@ -2840,7 +2844,7 @@
       <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="63" t="n">
+      <c r="B5" s="64" t="n">
         <v>329975</v>
       </c>
       <c r="C5" s="25" t="n">
@@ -2855,7 +2859,7 @@
         <f aca="false">(D5-C5)/C5</f>
         <v>-1</v>
       </c>
-      <c r="G5" s="62"/>
+      <c r="G5" s="63"/>
       <c r="M5" s="5"/>
       <c r="N5" s="10"/>
     </row>
@@ -2863,7 +2867,7 @@
       <c r="A6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="63" t="n">
+      <c r="B6" s="64" t="n">
         <v>333225</v>
       </c>
       <c r="C6" s="25" t="n">
@@ -2878,7 +2882,7 @@
         <f aca="false">(D6-C6)/C6</f>
         <v>-1</v>
       </c>
-      <c r="G6" s="62"/>
+      <c r="G6" s="63"/>
       <c r="M6" s="5"/>
       <c r="N6" s="10"/>
     </row>
@@ -2886,7 +2890,7 @@
       <c r="A7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="63" t="n">
+      <c r="B7" s="64" t="n">
         <v>319566</v>
       </c>
       <c r="C7" s="25" t="n">
@@ -2901,7 +2905,7 @@
         <f aca="false">(D7-C7)/C7</f>
         <v>-1</v>
       </c>
-      <c r="G7" s="62"/>
+      <c r="G7" s="63"/>
       <c r="M7" s="5"/>
       <c r="N7" s="10"/>
     </row>
@@ -2909,7 +2913,7 @@
       <c r="A8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="63" t="n">
+      <c r="B8" s="64" t="n">
         <v>345523</v>
       </c>
       <c r="C8" s="25" t="n">
@@ -2924,7 +2928,7 @@
         <f aca="false">(D8-C8)/C8</f>
         <v>-1</v>
       </c>
-      <c r="G8" s="62"/>
+      <c r="G8" s="63"/>
       <c r="M8" s="5"/>
       <c r="N8" s="10"/>
     </row>
@@ -2932,7 +2936,7 @@
       <c r="A9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="63" t="n">
+      <c r="B9" s="64" t="n">
         <v>344469</v>
       </c>
       <c r="C9" s="25" t="n">
@@ -2947,7 +2951,7 @@
         <f aca="false">(D9-C9)/C9</f>
         <v>-1</v>
       </c>
-      <c r="G9" s="62"/>
+      <c r="G9" s="63"/>
       <c r="M9" s="5"/>
       <c r="N9" s="10"/>
     </row>
@@ -2967,7 +2971,7 @@
         <v>-0.122928168726083</v>
       </c>
       <c r="F10" s="26"/>
-      <c r="G10" s="62"/>
+      <c r="G10" s="63"/>
       <c r="M10" s="5"/>
       <c r="N10" s="10"/>
     </row>
@@ -2987,7 +2991,7 @@
         <v>-0.17446078378055</v>
       </c>
       <c r="F11" s="26"/>
-      <c r="G11" s="62"/>
+      <c r="G11" s="63"/>
       <c r="M11" s="5"/>
       <c r="N11" s="10"/>
     </row>
@@ -3007,7 +3011,7 @@
         <v>-0.234098236878622</v>
       </c>
       <c r="F12" s="26"/>
-      <c r="G12" s="62"/>
+      <c r="G12" s="63"/>
       <c r="M12" s="5"/>
       <c r="N12" s="10"/>
     </row>
@@ -3015,7 +3019,7 @@
       <c r="A13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="64" t="n">
+      <c r="B13" s="65" t="n">
         <v>415125</v>
       </c>
       <c r="C13" s="25" t="n">
@@ -3027,57 +3031,57 @@
         <v>-0.236952725082806</v>
       </c>
       <c r="F13" s="26"/>
-      <c r="G13" s="62"/>
+      <c r="G13" s="63"/>
       <c r="M13" s="5"/>
       <c r="N13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="65" t="n">
+      <c r="B14" s="66" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>4264736</v>
       </c>
-      <c r="C14" s="65" t="n">
+      <c r="C14" s="66" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>3745369</v>
       </c>
-      <c r="D14" s="65" t="n">
+      <c r="D14" s="66" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>549399</v>
       </c>
-      <c r="E14" s="33" t="n">
+      <c r="E14" s="34" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>-0.121781746865457</v>
       </c>
-      <c r="F14" s="33" t="n">
+      <c r="F14" s="34" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>-0.797708112852279</v>
       </c>
-      <c r="G14" s="62"/>
+      <c r="G14" s="63"/>
       <c r="M14" s="5"/>
       <c r="N14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="30.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="66"/>
+      <c r="A15" s="67"/>
       <c r="B15" s="19" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="67"/>
-      <c r="E15" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="68"/>
-      <c r="G15" s="62"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="69"/>
+      <c r="G15" s="63"/>
       <c r="M15" s="5"/>
       <c r="N15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="66"/>
+      <c r="A16" s="67"/>
       <c r="B16" s="25" t="n">
         <v>4382326</v>
       </c>
@@ -3091,7 +3095,7 @@
         <v>-0.170065219208041</v>
       </c>
       <c r="F16" s="26"/>
-      <c r="G16" s="62"/>
+      <c r="G16" s="63"/>
       <c r="M16" s="5"/>
       <c r="N16" s="10"/>
     </row>
@@ -3180,37 +3184,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19"/>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="E1" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="43"/>
+      <c r="N1" s="44"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="71" t="n">
+      <c r="B2" s="72" t="n">
         <v>166018</v>
       </c>
-      <c r="C2" s="71" t="n">
+      <c r="C2" s="72" t="n">
         <v>154290</v>
       </c>
       <c r="D2" s="25" t="n">
         <v>137349</v>
       </c>
-      <c r="E2" s="72" t="n">
+      <c r="E2" s="73" t="n">
         <f aca="false">(C2-B2)/B2</f>
         <v>-0.0706429423315544</v>
       </c>
@@ -3218,22 +3222,22 @@
         <f aca="false">(D2-C2)/C2</f>
         <v>-0.109799727785339</v>
       </c>
-      <c r="N2" s="45"/>
+      <c r="N2" s="46"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="73" t="n">
+      <c r="B3" s="74" t="n">
         <v>153234</v>
       </c>
-      <c r="C3" s="71" t="n">
+      <c r="C3" s="72" t="n">
         <v>139138</v>
       </c>
       <c r="D3" s="25" t="n">
         <v>126757</v>
       </c>
-      <c r="E3" s="72" t="n">
+      <c r="E3" s="73" t="n">
         <f aca="false">(C3-B3)/B3</f>
         <v>-0.091990028322696</v>
       </c>
@@ -3241,22 +3245,22 @@
         <f aca="false">(D3-C3)/C3</f>
         <v>-0.0889835990168035</v>
       </c>
-      <c r="N3" s="46"/>
+      <c r="N3" s="47"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="71" t="n">
+      <c r="B4" s="72" t="n">
         <v>149129</v>
       </c>
-      <c r="C4" s="71" t="n">
+      <c r="C4" s="72" t="n">
         <v>139609</v>
       </c>
       <c r="D4" s="25" t="n">
         <v>117550</v>
       </c>
-      <c r="E4" s="72" t="n">
+      <c r="E4" s="73" t="n">
         <f aca="false">(C4-B4)/B4</f>
         <v>-0.0638373488724527</v>
       </c>
@@ -3264,22 +3268,22 @@
         <f aca="false">(D4-C4)/C4</f>
         <v>-0.158005572706631</v>
       </c>
-      <c r="N4" s="46"/>
+      <c r="N4" s="47"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="71" t="n">
+      <c r="B5" s="72" t="n">
         <v>146506</v>
       </c>
-      <c r="C5" s="71" t="n">
+      <c r="C5" s="72" t="n">
         <v>126227</v>
       </c>
       <c r="D5" s="25" t="n">
         <v>113477</v>
       </c>
-      <c r="E5" s="72" t="n">
+      <c r="E5" s="73" t="n">
         <f aca="false">(C5-B5)/B5</f>
         <v>-0.138417539213411</v>
       </c>
@@ -3287,22 +3291,22 @@
         <f aca="false">(D5-C5)/C5</f>
         <v>-0.101008500558518</v>
       </c>
-      <c r="N5" s="46"/>
+      <c r="N5" s="47"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="71" t="n">
+      <c r="B6" s="72" t="n">
         <v>122937</v>
       </c>
-      <c r="C6" s="71" t="n">
+      <c r="C6" s="72" t="n">
         <v>128749</v>
       </c>
       <c r="D6" s="25" t="n">
         <v>108336</v>
       </c>
-      <c r="E6" s="72" t="n">
+      <c r="E6" s="73" t="n">
         <f aca="false">(C6-B6)/B6</f>
         <v>0.0472762471835168</v>
       </c>
@@ -3310,22 +3314,22 @@
         <f aca="false">(D6-C6)/C6</f>
         <v>-0.158548804262557</v>
       </c>
-      <c r="N6" s="46"/>
+      <c r="N6" s="47"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="71" t="n">
+      <c r="B7" s="72" t="n">
         <v>113710</v>
       </c>
-      <c r="C7" s="71" t="n">
+      <c r="C7" s="72" t="n">
         <v>125671</v>
       </c>
       <c r="D7" s="25" t="n">
         <v>98523</v>
       </c>
-      <c r="E7" s="72" t="n">
+      <c r="E7" s="73" t="n">
         <f aca="false">(C7-B7)/B7</f>
         <v>0.10518863776273</v>
       </c>
@@ -3333,22 +3337,22 @@
         <f aca="false">(D7-C7)/C7</f>
         <v>-0.216024381122136</v>
       </c>
-      <c r="N7" s="46"/>
+      <c r="N7" s="47"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="71" t="n">
+      <c r="B8" s="72" t="n">
         <v>117122</v>
       </c>
-      <c r="C8" s="71" t="n">
+      <c r="C8" s="72" t="n">
         <v>147302</v>
       </c>
       <c r="D8" s="25" t="n">
         <v>103029</v>
       </c>
-      <c r="E8" s="72" t="n">
+      <c r="E8" s="73" t="n">
         <f aca="false">(C8-B8)/B8</f>
         <v>0.257680025955841</v>
       </c>
@@ -3356,22 +3360,22 @@
         <f aca="false">(D8-C8)/C8</f>
         <v>-0.300559394984454</v>
       </c>
-      <c r="N8" s="46"/>
+      <c r="N8" s="47"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="71" t="n">
+      <c r="B9" s="72" t="n">
         <v>126623</v>
       </c>
-      <c r="C9" s="71" t="n">
+      <c r="C9" s="72" t="n">
         <v>145461</v>
       </c>
       <c r="D9" s="25" t="n">
         <v>115694</v>
       </c>
-      <c r="E9" s="72" t="n">
+      <c r="E9" s="73" t="n">
         <f aca="false">(C9-B9)/B9</f>
         <v>0.148772339938242</v>
       </c>
@@ -3379,105 +3383,105 @@
         <f aca="false">(D9-C9)/C9</f>
         <v>-0.204639044142416</v>
       </c>
-      <c r="N9" s="46"/>
+      <c r="N9" s="47"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="71" t="n">
+      <c r="B10" s="72" t="n">
         <v>122360</v>
       </c>
-      <c r="C10" s="71" t="n">
+      <c r="C10" s="72" t="n">
         <v>149470</v>
       </c>
       <c r="D10" s="25"/>
-      <c r="E10" s="72" t="n">
+      <c r="E10" s="73" t="n">
         <f aca="false">(C10-B10)/B10</f>
         <v>0.221559333115397</v>
       </c>
       <c r="F10" s="26"/>
-      <c r="N10" s="46"/>
+      <c r="N10" s="47"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="71" t="n">
+      <c r="B11" s="72" t="n">
         <v>132280</v>
       </c>
-      <c r="C11" s="71" t="n">
+      <c r="C11" s="72" t="n">
         <v>165507</v>
       </c>
       <c r="D11" s="25"/>
-      <c r="E11" s="72" t="n">
+      <c r="E11" s="73" t="n">
         <f aca="false">(C11-B11)/B11</f>
         <v>0.251186876322951</v>
       </c>
       <c r="F11" s="26"/>
-      <c r="N11" s="46"/>
+      <c r="N11" s="47"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="71" t="n">
+      <c r="B12" s="72" t="n">
         <v>128303</v>
       </c>
-      <c r="C12" s="71" t="n">
+      <c r="C12" s="72" t="n">
         <v>162736</v>
       </c>
       <c r="D12" s="25"/>
-      <c r="E12" s="72" t="n">
+      <c r="E12" s="73" t="n">
         <f aca="false">(C12-B12)/B12</f>
         <v>0.268372524414862</v>
       </c>
       <c r="F12" s="26"/>
-      <c r="N12" s="46"/>
+      <c r="N12" s="47"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="71" t="n">
+      <c r="B13" s="72" t="n">
         <v>132120</v>
       </c>
-      <c r="C13" s="71" t="n">
+      <c r="C13" s="72" t="n">
         <v>165619</v>
       </c>
       <c r="D13" s="25"/>
-      <c r="E13" s="72" t="n">
+      <c r="E13" s="73" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>0.253549803209204</v>
       </c>
       <c r="F13" s="26"/>
-      <c r="N13" s="46"/>
+      <c r="N13" s="47"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="65" t="n">
+      <c r="B14" s="66" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>1610342</v>
       </c>
-      <c r="C14" s="65" t="n">
+      <c r="C14" s="66" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>1749779</v>
       </c>
-      <c r="D14" s="65" t="n">
+      <c r="D14" s="66" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>920715</v>
       </c>
-      <c r="E14" s="33" t="n">
+      <c r="E14" s="34" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>0.0865884389775588</v>
       </c>
-      <c r="F14" s="33" t="n">
+      <c r="F14" s="34" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>-0.167196128072357</v>
       </c>
-      <c r="N14" s="46"/>
+      <c r="N14" s="47"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3501,8 +3505,8 @@
   </sheetPr>
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M18" activeCellId="0" sqref="M18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3522,31 +3526,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="30.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19"/>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="76" t="s">
+      <c r="E1" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="75" t="s">
+      <c r="F1" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
       <c r="M1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3570,16 +3574,16 @@
         <f aca="false">(D2-C2)/C2</f>
         <v>0.104134835752483</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
       <c r="M2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="10" t="s">
-        <v>59</v>
+      <c r="N2" s="27" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3589,7 +3593,7 @@
       <c r="B3" s="25" t="n">
         <v>37545</v>
       </c>
-      <c r="C3" s="44" t="n">
+      <c r="C3" s="45" t="n">
         <v>50219</v>
       </c>
       <c r="D3" s="25" t="n">
@@ -3603,15 +3607,15 @@
         <f aca="false">(D3-C3)/C3</f>
         <v>-0.336207411537466</v>
       </c>
-      <c r="G3" s="77" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
+      <c r="G3" s="78" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="10"/>
+      <c r="N3" s="27"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
@@ -3620,7 +3624,7 @@
       <c r="B4" s="25" t="n">
         <v>25781.81</v>
       </c>
-      <c r="C4" s="44" t="n">
+      <c r="C4" s="45" t="n">
         <v>45023</v>
       </c>
       <c r="D4" s="25"/>
@@ -3632,13 +3636,13 @@
         <f aca="false">(D4-C4)/C4</f>
         <v>-1</v>
       </c>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="10"/>
+      <c r="N4" s="27"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
@@ -3647,7 +3651,7 @@
       <c r="B5" s="25" t="n">
         <v>25781.81</v>
       </c>
-      <c r="C5" s="44" t="n">
+      <c r="C5" s="45" t="n">
         <v>25839</v>
       </c>
       <c r="D5" s="25"/>
@@ -3659,13 +3663,13 @@
         <f aca="false">(D5-C5)/C5</f>
         <v>-1</v>
       </c>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="10"/>
+      <c r="N5" s="27"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
@@ -3674,7 +3678,7 @@
       <c r="B6" s="25" t="n">
         <v>13432.28</v>
       </c>
-      <c r="C6" s="44" t="n">
+      <c r="C6" s="45" t="n">
         <v>12769</v>
       </c>
       <c r="D6" s="25"/>
@@ -3686,13 +3690,13 @@
         <f aca="false">(D6-C6)/C6</f>
         <v>-1</v>
       </c>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="10"/>
+      <c r="N6" s="27"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
@@ -3701,7 +3705,7 @@
       <c r="B7" s="25" t="n">
         <v>15430.56</v>
       </c>
-      <c r="C7" s="44" t="n">
+      <c r="C7" s="45" t="n">
         <v>10444</v>
       </c>
       <c r="D7" s="25"/>
@@ -3713,13 +3717,13 @@
         <f aca="false">(D7-C7)/C7</f>
         <v>-1</v>
       </c>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="10"/>
+      <c r="N7" s="27"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
@@ -3740,13 +3744,13 @@
         <f aca="false">(D8-C8)/C8</f>
         <v>-1</v>
       </c>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57"/>
-      <c r="K8" s="57"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="10"/>
+      <c r="N8" s="27"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
@@ -3767,89 +3771,89 @@
         <f aca="false">(D9-C9)/C9</f>
         <v>-1</v>
       </c>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="10"/>
+      <c r="N9" s="27"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="27" t="n">
+      <c r="B10" s="28" t="n">
         <v>23032</v>
       </c>
       <c r="C10" s="25" t="n">
         <v>11779</v>
       </c>
       <c r="D10" s="25"/>
-      <c r="E10" s="29" t="n">
+      <c r="E10" s="30" t="n">
         <f aca="false">(C10-B10)/B10</f>
         <v>-0.488581104550191</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="10"/>
+      <c r="N10" s="27"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="27" t="n">
+      <c r="B11" s="28" t="n">
         <v>36770</v>
       </c>
       <c r="C11" s="25" t="n">
         <v>23418</v>
       </c>
       <c r="D11" s="25"/>
-      <c r="E11" s="29" t="n">
+      <c r="E11" s="30" t="n">
         <f aca="false">(C11-B11)/B11</f>
         <v>-0.3631221104161</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
+      <c r="G11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="10"/>
+      <c r="N11" s="27"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="69" t="s">
+      <c r="A12" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="27" t="n">
+      <c r="B12" s="28" t="n">
         <v>40381</v>
       </c>
       <c r="C12" s="25" t="n">
         <v>34717</v>
       </c>
       <c r="D12" s="25"/>
-      <c r="E12" s="29" t="n">
+      <c r="E12" s="30" t="n">
         <f aca="false">(C12-B12)/B12</f>
         <v>-0.140263985537753</v>
       </c>
       <c r="F12" s="9"/>
-      <c r="G12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
+      <c r="G12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
       <c r="M12" s="5"/>
-      <c r="N12" s="10"/>
+      <c r="N12" s="27"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="78" t="n">
+      <c r="B13" s="79" t="n">
         <v>34355</v>
       </c>
       <c r="C13" s="25" t="n">
@@ -3861,88 +3865,88 @@
         <v>0.0611264735846311</v>
       </c>
       <c r="F13" s="9"/>
-      <c r="G13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
+      <c r="G13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
       <c r="M13" s="5"/>
-      <c r="N13" s="10"/>
+      <c r="N13" s="27"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="65" t="n">
+      <c r="B14" s="66" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>307130.98</v>
       </c>
-      <c r="C14" s="65" t="n">
+      <c r="C14" s="66" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>313121</v>
       </c>
-      <c r="D14" s="32" t="n">
+      <c r="D14" s="33" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>79585</v>
       </c>
-      <c r="E14" s="33" t="n">
+      <c r="E14" s="34" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>0.0195031448797514</v>
       </c>
-      <c r="F14" s="34" t="n">
+      <c r="F14" s="35" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>-0.779009071973123</v>
       </c>
-      <c r="G14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
+      <c r="G14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
       <c r="M14" s="5"/>
-      <c r="N14" s="10"/>
+      <c r="N14" s="27"/>
     </row>
     <row r="15" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="79"/>
-      <c r="B15" s="80" t="s">
+      <c r="A15" s="80"/>
+      <c r="B15" s="81" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="80" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="80"/>
-      <c r="E15" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="81"/>
-      <c r="G15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="82"/>
+      <c r="G15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="58"/>
       <c r="M15" s="5"/>
-      <c r="N15" s="10"/>
+      <c r="N15" s="27"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="79"/>
-      <c r="B16" s="82" t="n">
+      <c r="A16" s="80"/>
+      <c r="B16" s="83" t="n">
         <v>331445.11</v>
       </c>
-      <c r="C16" s="82" t="n">
+      <c r="C16" s="83" t="n">
         <v>272775.98</v>
       </c>
-      <c r="D16" s="80"/>
+      <c r="D16" s="81"/>
       <c r="E16" s="9" t="n">
         <f aca="false">(C16-B16)/C16</f>
         <v>-0.215081731170025</v>
       </c>
-      <c r="F16" s="81"/>
-      <c r="G16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
+      <c r="F16" s="82"/>
+      <c r="G16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
       <c r="M16" s="5"/>
-      <c r="N16" s="10"/>
+      <c r="N16" s="27"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M17" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N17" s="17"/>
       <c r="O17" s="17"/>
@@ -3952,7 +3956,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M18" s="18" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="N18" s="18"/>
       <c r="O18" s="18"/>

</xml_diff>

<commit_message>
Remove outdated directories and files
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Waste" sheetId="1" state="visible" r:id="rId2"/>
@@ -933,7 +933,7 @@
     <numFmt numFmtId="170" formatCode="0.00%"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -991,12 +991,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1198,7 +1192,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1307,10 +1301,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -1323,11 +1313,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1335,7 +1325,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1347,11 +1337,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1392,7 +1382,7 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="12" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1419,7 +1409,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1431,7 +1421,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1443,7 +1433,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1451,11 +1441,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1463,7 +1453,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1511,7 +1501,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1527,7 +1517,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1615,7 +1605,7 @@
   </sheetPr>
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
     </sheetView>
   </sheetViews>
@@ -1908,8 +1898,8 @@
   </sheetPr>
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1968,7 +1958,7 @@
       <c r="M2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="27" t="s">
+      <c r="N2" s="10" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1994,7 +1984,7 @@
         <v>-0.0658448150833938</v>
       </c>
       <c r="M3" s="5"/>
-      <c r="N3" s="27"/>
+      <c r="N3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
@@ -2016,7 +2006,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M4" s="5"/>
-      <c r="N4" s="27"/>
+      <c r="N4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
@@ -2038,7 +2028,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M5" s="5"/>
-      <c r="N5" s="27"/>
+      <c r="N5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
@@ -2047,7 +2037,7 @@
       <c r="B6" s="24" t="n">
         <v>6577</v>
       </c>
-      <c r="C6" s="28" t="n">
+      <c r="C6" s="27" t="n">
         <v>10387</v>
       </c>
       <c r="D6" s="25"/>
@@ -2060,7 +2050,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M6" s="5"/>
-      <c r="N6" s="27"/>
+      <c r="N6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
@@ -2069,7 +2059,7 @@
       <c r="B7" s="24" t="n">
         <v>7009</v>
       </c>
-      <c r="C7" s="28" t="n">
+      <c r="C7" s="27" t="n">
         <v>8235</v>
       </c>
       <c r="D7" s="25"/>
@@ -2082,7 +2072,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M7" s="5"/>
-      <c r="N7" s="27"/>
+      <c r="N7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
@@ -2104,7 +2094,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M8" s="5"/>
-      <c r="N8" s="27"/>
+      <c r="N8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
@@ -2126,7 +2116,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M9" s="5"/>
-      <c r="N9" s="27"/>
+      <c r="N9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
@@ -2148,7 +2138,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M10" s="5"/>
-      <c r="N10" s="27"/>
+      <c r="N10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
@@ -2167,7 +2157,7 @@
       </c>
       <c r="F11" s="9"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="27"/>
+      <c r="N11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19" t="s">
@@ -2186,52 +2176,52 @@
       </c>
       <c r="F12" s="9"/>
       <c r="M12" s="5"/>
-      <c r="N12" s="27"/>
+      <c r="N12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="29" t="n">
+      <c r="B13" s="28" t="n">
         <v>8881</v>
       </c>
       <c r="C13" s="25" t="n">
         <v>6912</v>
       </c>
       <c r="D13" s="25"/>
-      <c r="E13" s="30" t="n">
+      <c r="E13" s="29" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>-0.22170926697444</v>
       </c>
       <c r="F13" s="9"/>
       <c r="M13" s="5"/>
-      <c r="N13" s="27"/>
+      <c r="N13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="32" t="n">
+      <c r="B14" s="31" t="n">
         <v>77704</v>
       </c>
-      <c r="C14" s="33" t="n">
+      <c r="C14" s="32" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>96849</v>
       </c>
-      <c r="D14" s="33" t="n">
+      <c r="D14" s="32" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>14960</v>
       </c>
-      <c r="E14" s="34" t="n">
+      <c r="E14" s="33" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>0.24638371255019</v>
       </c>
-      <c r="F14" s="35" t="e">
+      <c r="F14" s="34" t="e">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M14" s="5"/>
-      <c r="N14" s="27"/>
+      <c r="N14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="43.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="19"/>
@@ -2242,15 +2232,15 @@
         <v>30</v>
       </c>
       <c r="D15" s="19"/>
-      <c r="E15" s="36" t="s">
+      <c r="E15" s="35" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="19"/>
       <c r="M15" s="5"/>
-      <c r="N15" s="27"/>
+      <c r="N15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="36"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="25" t="n">
         <v>81734</v>
       </c>
@@ -2258,13 +2248,13 @@
         <v>77704</v>
       </c>
       <c r="D16" s="19"/>
-      <c r="E16" s="37" t="n">
+      <c r="E16" s="36" t="n">
         <f aca="false">(C16-B16)/B16</f>
         <v>-0.0493062862456261</v>
       </c>
-      <c r="F16" s="38"/>
+      <c r="F16" s="37"/>
       <c r="M16" s="5"/>
-      <c r="N16" s="27"/>
+      <c r="N16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M17" s="17" t="s">
@@ -2278,15 +2268,15 @@
       <c r="S17" s="17"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M18" s="39" t="s">
+      <c r="M18" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="39"/>
-      <c r="R18" s="39"/>
-      <c r="S18" s="39"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="38"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2341,37 +2331,37 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="44"/>
+      <c r="N1" s="43"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="45" t="n">
+      <c r="B2" s="44" t="n">
         <v>1217</v>
       </c>
-      <c r="C2" s="45" t="n">
+      <c r="C2" s="44" t="n">
         <v>224</v>
       </c>
       <c r="D2" s="9" t="n">
@@ -2389,16 +2379,16 @@
         <f aca="false">(E2-B2)/B2</f>
         <v>0.226787181594084</v>
       </c>
-      <c r="N2" s="46"/>
+      <c r="N2" s="45"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="45" t="n">
+      <c r="B3" s="44" t="n">
         <v>1518.25</v>
       </c>
-      <c r="C3" s="45" t="n">
+      <c r="C3" s="44" t="n">
         <v>221</v>
       </c>
       <c r="D3" s="9" t="n">
@@ -2416,16 +2406,16 @@
         <f aca="false">(E3-B3)/B3</f>
         <v>-0.126626049728306</v>
       </c>
-      <c r="N3" s="47"/>
+      <c r="N3" s="46"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="45" t="n">
+      <c r="B4" s="44" t="n">
         <v>1203.4</v>
       </c>
-      <c r="C4" s="45" t="n">
+      <c r="C4" s="44" t="n">
         <v>203</v>
       </c>
       <c r="D4" s="9" t="n">
@@ -2443,7 +2433,7 @@
         <f aca="false">(E4-B4)/B4</f>
         <v>-0.15738740235998</v>
       </c>
-      <c r="N4" s="47"/>
+      <c r="N4" s="46"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
@@ -2470,7 +2460,7 @@
         <f aca="false">(E5-B5)/B5</f>
         <v>0.892045454545455</v>
       </c>
-      <c r="N5" s="47"/>
+      <c r="N5" s="46"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
@@ -2486,7 +2476,7 @@
         <f aca="false">(C6-B6)/B6</f>
         <v>0.375791139240506</v>
       </c>
-      <c r="E6" s="28" t="n">
+      <c r="E6" s="27" t="n">
         <v>3212</v>
       </c>
       <c r="F6" s="9" t="n">
@@ -2497,7 +2487,7 @@
         <f aca="false">(E6-B6)/B6</f>
         <v>1.54113924050633</v>
       </c>
-      <c r="N6" s="47"/>
+      <c r="N6" s="46"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
@@ -2513,10 +2503,10 @@
         <f aca="false">(C7-B7)/B7</f>
         <v>0.626865671641791</v>
       </c>
-      <c r="E7" s="28" t="n">
+      <c r="E7" s="27" t="n">
         <v>2547</v>
       </c>
-      <c r="F7" s="48" t="n">
+      <c r="F7" s="47" t="n">
         <f aca="false">(E7-C7)/C7</f>
         <v>0.374527792768483</v>
       </c>
@@ -2524,7 +2514,7 @@
         <f aca="false">(E7-B7)/B7</f>
         <v>1.23617208077261</v>
       </c>
-      <c r="N7" s="47"/>
+      <c r="N7" s="46"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
@@ -2541,9 +2531,9 @@
         <v>-0.143830128205128</v>
       </c>
       <c r="E8" s="25"/>
-      <c r="F8" s="49"/>
+      <c r="F8" s="48"/>
       <c r="G8" s="9"/>
-      <c r="N8" s="47"/>
+      <c r="N8" s="46"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
@@ -2560,9 +2550,9 @@
         <v>0.236727589208007</v>
       </c>
       <c r="E9" s="25"/>
-      <c r="F9" s="49"/>
+      <c r="F9" s="48"/>
       <c r="G9" s="9"/>
-      <c r="N9" s="47"/>
+      <c r="N9" s="46"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
@@ -2579,9 +2569,9 @@
         <v>0.354838709677419</v>
       </c>
       <c r="E10" s="25"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="50"/>
-      <c r="N10" s="47"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="49"/>
+      <c r="N10" s="46"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
@@ -2598,9 +2588,9 @@
         <v>0.394584997780737</v>
       </c>
       <c r="E11" s="25"/>
-      <c r="F11" s="49"/>
+      <c r="F11" s="48"/>
       <c r="G11" s="9"/>
-      <c r="N11" s="47"/>
+      <c r="N11" s="46"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19" t="s">
@@ -2617,91 +2607,91 @@
         <v>0.143394934976044</v>
       </c>
       <c r="E12" s="25"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="51"/>
-      <c r="N12" s="47"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="50"/>
+      <c r="N12" s="46"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="28" t="n">
+      <c r="B13" s="27" t="n">
         <v>4402</v>
       </c>
-      <c r="C13" s="28" t="n">
+      <c r="C13" s="27" t="n">
         <v>3233</v>
       </c>
-      <c r="D13" s="52" t="n">
+      <c r="D13" s="51" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>-0.265561108587006</v>
       </c>
       <c r="E13" s="25"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="51"/>
-      <c r="N13" s="47"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="50"/>
+      <c r="N13" s="46"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="33" t="n">
+      <c r="B14" s="32" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>24383.65</v>
       </c>
-      <c r="C14" s="33" t="n">
+      <c r="C14" s="32" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>23517</v>
       </c>
-      <c r="D14" s="35" t="n">
+      <c r="D14" s="34" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>-0.0355422588496801</v>
       </c>
-      <c r="E14" s="33" t="n">
+      <c r="E14" s="32" t="n">
         <f aca="false">SUM(E2:E13)</f>
         <v>12256</v>
       </c>
-      <c r="F14" s="55" t="n">
+      <c r="F14" s="54" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>2.77317912006462</v>
       </c>
-      <c r="G14" s="55" t="n">
+      <c r="G14" s="54" t="n">
         <f aca="false">AVERAGE(G2:G13)</f>
         <v>0.602021750888365</v>
       </c>
-      <c r="N14" s="47"/>
+      <c r="N14" s="46"/>
     </row>
     <row r="15" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="56"/>
-      <c r="B15" s="57" t="s">
+      <c r="A15" s="55"/>
+      <c r="B15" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="57" t="s">
+      <c r="C15" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="58"/>
-      <c r="N15" s="47"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="57"/>
+      <c r="N15" s="46"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="56"/>
-      <c r="B16" s="59" t="n">
+      <c r="A16" s="55"/>
+      <c r="B16" s="58" t="n">
         <v>23383</v>
       </c>
-      <c r="C16" s="59" t="n">
+      <c r="C16" s="58" t="n">
         <v>23517</v>
       </c>
-      <c r="D16" s="60" t="n">
+      <c r="D16" s="59" t="n">
         <f aca="false">(C16-B16)/B16</f>
         <v>0.00573065902578797</v>
       </c>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="58"/>
-      <c r="N16" s="47"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="57"/>
+      <c r="N16" s="46"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
@@ -2743,22 +2733,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="50.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="63"/>
+      <c r="G1" s="62"/>
       <c r="M1" s="5" t="s">
         <v>4</v>
       </c>
@@ -2770,7 +2760,7 @@
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="64" t="n">
+      <c r="B2" s="63" t="n">
         <v>381400</v>
       </c>
       <c r="C2" s="25" t="n">
@@ -2787,7 +2777,7 @@
         <f aca="false">(D2-C2)/C2</f>
         <v>-0.185643516053403</v>
       </c>
-      <c r="G2" s="63"/>
+      <c r="G2" s="62"/>
       <c r="M2" s="5" t="s">
         <v>7</v>
       </c>
@@ -2799,7 +2789,7 @@
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="64" t="n">
+      <c r="B3" s="63" t="n">
         <v>338378</v>
       </c>
       <c r="C3" s="25" t="n">
@@ -2816,7 +2806,7 @@
         <f aca="false">(D3-C3)/C3</f>
         <v>-0.19602138676483</v>
       </c>
-      <c r="G3" s="63"/>
+      <c r="G3" s="62"/>
       <c r="M3" s="5"/>
       <c r="N3" s="10"/>
     </row>
@@ -2824,7 +2814,7 @@
       <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="64" t="n">
+      <c r="B4" s="63" t="n">
         <v>354957</v>
       </c>
       <c r="C4" s="25" t="n">
@@ -2839,7 +2829,7 @@
         <f aca="false">(D4-C4)/C4</f>
         <v>-1</v>
       </c>
-      <c r="G4" s="63"/>
+      <c r="G4" s="62"/>
       <c r="M4" s="5"/>
       <c r="N4" s="10"/>
     </row>
@@ -2847,7 +2837,7 @@
       <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="64" t="n">
+      <c r="B5" s="63" t="n">
         <v>329975</v>
       </c>
       <c r="C5" s="25" t="n">
@@ -2862,7 +2852,7 @@
         <f aca="false">(D5-C5)/C5</f>
         <v>-1</v>
       </c>
-      <c r="G5" s="63"/>
+      <c r="G5" s="62"/>
       <c r="M5" s="5"/>
       <c r="N5" s="10"/>
     </row>
@@ -2870,7 +2860,7 @@
       <c r="A6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="64" t="n">
+      <c r="B6" s="63" t="n">
         <v>333225</v>
       </c>
       <c r="C6" s="25" t="n">
@@ -2885,7 +2875,7 @@
         <f aca="false">(D6-C6)/C6</f>
         <v>-1</v>
       </c>
-      <c r="G6" s="63"/>
+      <c r="G6" s="62"/>
       <c r="M6" s="5"/>
       <c r="N6" s="10"/>
     </row>
@@ -2893,7 +2883,7 @@
       <c r="A7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="64" t="n">
+      <c r="B7" s="63" t="n">
         <v>319566</v>
       </c>
       <c r="C7" s="25" t="n">
@@ -2908,7 +2898,7 @@
         <f aca="false">(D7-C7)/C7</f>
         <v>-1</v>
       </c>
-      <c r="G7" s="63"/>
+      <c r="G7" s="62"/>
       <c r="M7" s="5"/>
       <c r="N7" s="10"/>
     </row>
@@ -2916,7 +2906,7 @@
       <c r="A8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="64" t="n">
+      <c r="B8" s="63" t="n">
         <v>345523</v>
       </c>
       <c r="C8" s="25" t="n">
@@ -2931,7 +2921,7 @@
         <f aca="false">(D8-C8)/C8</f>
         <v>-1</v>
       </c>
-      <c r="G8" s="63"/>
+      <c r="G8" s="62"/>
       <c r="M8" s="5"/>
       <c r="N8" s="10"/>
     </row>
@@ -2939,7 +2929,7 @@
       <c r="A9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="64" t="n">
+      <c r="B9" s="63" t="n">
         <v>344469</v>
       </c>
       <c r="C9" s="25" t="n">
@@ -2954,7 +2944,7 @@
         <f aca="false">(D9-C9)/C9</f>
         <v>-1</v>
       </c>
-      <c r="G9" s="63"/>
+      <c r="G9" s="62"/>
       <c r="M9" s="5"/>
       <c r="N9" s="10"/>
     </row>
@@ -2974,7 +2964,7 @@
         <v>-0.122928168726083</v>
       </c>
       <c r="F10" s="26"/>
-      <c r="G10" s="63"/>
+      <c r="G10" s="62"/>
       <c r="M10" s="5"/>
       <c r="N10" s="10"/>
     </row>
@@ -2994,7 +2984,7 @@
         <v>-0.17446078378055</v>
       </c>
       <c r="F11" s="26"/>
-      <c r="G11" s="63"/>
+      <c r="G11" s="62"/>
       <c r="M11" s="5"/>
       <c r="N11" s="10"/>
     </row>
@@ -3014,7 +3004,7 @@
         <v>-0.234098236878622</v>
       </c>
       <c r="F12" s="26"/>
-      <c r="G12" s="63"/>
+      <c r="G12" s="62"/>
       <c r="M12" s="5"/>
       <c r="N12" s="10"/>
     </row>
@@ -3022,7 +3012,7 @@
       <c r="A13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="65" t="n">
+      <c r="B13" s="64" t="n">
         <v>415125</v>
       </c>
       <c r="C13" s="25" t="n">
@@ -3034,57 +3024,57 @@
         <v>-0.236952725082806</v>
       </c>
       <c r="F13" s="26"/>
-      <c r="G13" s="63"/>
+      <c r="G13" s="62"/>
       <c r="M13" s="5"/>
       <c r="N13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="66" t="n">
+      <c r="B14" s="65" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>4264736</v>
       </c>
-      <c r="C14" s="66" t="n">
+      <c r="C14" s="65" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>3745369</v>
       </c>
-      <c r="D14" s="66" t="n">
+      <c r="D14" s="65" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>549399</v>
       </c>
-      <c r="E14" s="34" t="n">
+      <c r="E14" s="33" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>-0.121781746865457</v>
       </c>
-      <c r="F14" s="34" t="n">
+      <c r="F14" s="33" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>-0.797708112852279</v>
       </c>
-      <c r="G14" s="63"/>
+      <c r="G14" s="62"/>
       <c r="M14" s="5"/>
       <c r="N14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="30.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="67"/>
+      <c r="A15" s="66"/>
       <c r="B15" s="19" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="68"/>
-      <c r="E15" s="69" t="s">
+      <c r="D15" s="67"/>
+      <c r="E15" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="69"/>
-      <c r="G15" s="63"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="62"/>
       <c r="M15" s="5"/>
       <c r="N15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="67"/>
+      <c r="A16" s="66"/>
       <c r="B16" s="25" t="n">
         <v>4382326</v>
       </c>
@@ -3098,7 +3088,7 @@
         <v>-0.170065219208041</v>
       </c>
       <c r="F16" s="26"/>
-      <c r="G16" s="63"/>
+      <c r="G16" s="62"/>
       <c r="M16" s="5"/>
       <c r="N16" s="10"/>
     </row>
@@ -3187,37 +3177,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19"/>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="44"/>
+      <c r="N1" s="43"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="72" t="n">
+      <c r="B2" s="71" t="n">
         <v>166018</v>
       </c>
-      <c r="C2" s="72" t="n">
+      <c r="C2" s="71" t="n">
         <v>154290</v>
       </c>
       <c r="D2" s="25" t="n">
         <v>137349</v>
       </c>
-      <c r="E2" s="73" t="n">
+      <c r="E2" s="72" t="n">
         <f aca="false">(C2-B2)/B2</f>
         <v>-0.0706429423315544</v>
       </c>
@@ -3225,22 +3215,22 @@
         <f aca="false">(D2-C2)/C2</f>
         <v>-0.109799727785339</v>
       </c>
-      <c r="N2" s="46"/>
+      <c r="N2" s="45"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="74" t="n">
+      <c r="B3" s="73" t="n">
         <v>153234</v>
       </c>
-      <c r="C3" s="72" t="n">
+      <c r="C3" s="71" t="n">
         <v>139138</v>
       </c>
       <c r="D3" s="25" t="n">
         <v>126757</v>
       </c>
-      <c r="E3" s="73" t="n">
+      <c r="E3" s="72" t="n">
         <f aca="false">(C3-B3)/B3</f>
         <v>-0.091990028322696</v>
       </c>
@@ -3248,22 +3238,22 @@
         <f aca="false">(D3-C3)/C3</f>
         <v>-0.0889835990168035</v>
       </c>
-      <c r="N3" s="47"/>
+      <c r="N3" s="46"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="72" t="n">
+      <c r="B4" s="71" t="n">
         <v>149129</v>
       </c>
-      <c r="C4" s="72" t="n">
+      <c r="C4" s="71" t="n">
         <v>139609</v>
       </c>
       <c r="D4" s="25" t="n">
         <v>117550</v>
       </c>
-      <c r="E4" s="73" t="n">
+      <c r="E4" s="72" t="n">
         <f aca="false">(C4-B4)/B4</f>
         <v>-0.0638373488724527</v>
       </c>
@@ -3271,22 +3261,22 @@
         <f aca="false">(D4-C4)/C4</f>
         <v>-0.158005572706631</v>
       </c>
-      <c r="N4" s="47"/>
+      <c r="N4" s="46"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="72" t="n">
+      <c r="B5" s="71" t="n">
         <v>146506</v>
       </c>
-      <c r="C5" s="72" t="n">
+      <c r="C5" s="71" t="n">
         <v>126227</v>
       </c>
       <c r="D5" s="25" t="n">
         <v>113477</v>
       </c>
-      <c r="E5" s="73" t="n">
+      <c r="E5" s="72" t="n">
         <f aca="false">(C5-B5)/B5</f>
         <v>-0.138417539213411</v>
       </c>
@@ -3294,22 +3284,22 @@
         <f aca="false">(D5-C5)/C5</f>
         <v>-0.101008500558518</v>
       </c>
-      <c r="N5" s="47"/>
+      <c r="N5" s="46"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="72" t="n">
+      <c r="B6" s="71" t="n">
         <v>122937</v>
       </c>
-      <c r="C6" s="72" t="n">
+      <c r="C6" s="71" t="n">
         <v>128749</v>
       </c>
       <c r="D6" s="25" t="n">
         <v>108336</v>
       </c>
-      <c r="E6" s="73" t="n">
+      <c r="E6" s="72" t="n">
         <f aca="false">(C6-B6)/B6</f>
         <v>0.0472762471835168</v>
       </c>
@@ -3317,22 +3307,22 @@
         <f aca="false">(D6-C6)/C6</f>
         <v>-0.158548804262557</v>
       </c>
-      <c r="N6" s="47"/>
+      <c r="N6" s="46"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="72" t="n">
+      <c r="B7" s="71" t="n">
         <v>113710</v>
       </c>
-      <c r="C7" s="72" t="n">
+      <c r="C7" s="71" t="n">
         <v>125671</v>
       </c>
       <c r="D7" s="25" t="n">
         <v>98523</v>
       </c>
-      <c r="E7" s="73" t="n">
+      <c r="E7" s="72" t="n">
         <f aca="false">(C7-B7)/B7</f>
         <v>0.10518863776273</v>
       </c>
@@ -3340,22 +3330,22 @@
         <f aca="false">(D7-C7)/C7</f>
         <v>-0.216024381122136</v>
       </c>
-      <c r="N7" s="47"/>
+      <c r="N7" s="46"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="72" t="n">
+      <c r="B8" s="71" t="n">
         <v>117122</v>
       </c>
-      <c r="C8" s="72" t="n">
+      <c r="C8" s="71" t="n">
         <v>147302</v>
       </c>
       <c r="D8" s="25" t="n">
         <v>103029</v>
       </c>
-      <c r="E8" s="73" t="n">
+      <c r="E8" s="72" t="n">
         <f aca="false">(C8-B8)/B8</f>
         <v>0.257680025955841</v>
       </c>
@@ -3363,22 +3353,22 @@
         <f aca="false">(D8-C8)/C8</f>
         <v>-0.300559394984454</v>
       </c>
-      <c r="N8" s="47"/>
+      <c r="N8" s="46"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="72" t="n">
+      <c r="B9" s="71" t="n">
         <v>126623</v>
       </c>
-      <c r="C9" s="72" t="n">
+      <c r="C9" s="71" t="n">
         <v>145461</v>
       </c>
       <c r="D9" s="25" t="n">
         <v>115694</v>
       </c>
-      <c r="E9" s="73" t="n">
+      <c r="E9" s="72" t="n">
         <f aca="false">(C9-B9)/B9</f>
         <v>0.148772339938242</v>
       </c>
@@ -3386,105 +3376,105 @@
         <f aca="false">(D9-C9)/C9</f>
         <v>-0.204639044142416</v>
       </c>
-      <c r="N9" s="47"/>
+      <c r="N9" s="46"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="72" t="n">
+      <c r="B10" s="71" t="n">
         <v>122360</v>
       </c>
-      <c r="C10" s="72" t="n">
+      <c r="C10" s="71" t="n">
         <v>149470</v>
       </c>
       <c r="D10" s="25"/>
-      <c r="E10" s="73" t="n">
+      <c r="E10" s="72" t="n">
         <f aca="false">(C10-B10)/B10</f>
         <v>0.221559333115397</v>
       </c>
       <c r="F10" s="26"/>
-      <c r="N10" s="47"/>
+      <c r="N10" s="46"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="72" t="n">
+      <c r="B11" s="71" t="n">
         <v>132280</v>
       </c>
-      <c r="C11" s="72" t="n">
+      <c r="C11" s="71" t="n">
         <v>165507</v>
       </c>
       <c r="D11" s="25"/>
-      <c r="E11" s="73" t="n">
+      <c r="E11" s="72" t="n">
         <f aca="false">(C11-B11)/B11</f>
         <v>0.251186876322951</v>
       </c>
       <c r="F11" s="26"/>
-      <c r="N11" s="47"/>
+      <c r="N11" s="46"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="72" t="n">
+      <c r="B12" s="71" t="n">
         <v>128303</v>
       </c>
-      <c r="C12" s="72" t="n">
+      <c r="C12" s="71" t="n">
         <v>162736</v>
       </c>
       <c r="D12" s="25"/>
-      <c r="E12" s="73" t="n">
+      <c r="E12" s="72" t="n">
         <f aca="false">(C12-B12)/B12</f>
         <v>0.268372524414862</v>
       </c>
       <c r="F12" s="26"/>
-      <c r="N12" s="47"/>
+      <c r="N12" s="46"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="72" t="n">
+      <c r="B13" s="71" t="n">
         <v>132120</v>
       </c>
-      <c r="C13" s="72" t="n">
+      <c r="C13" s="71" t="n">
         <v>165619</v>
       </c>
       <c r="D13" s="25"/>
-      <c r="E13" s="73" t="n">
+      <c r="E13" s="72" t="n">
         <f aca="false">(C13-B13)/B13</f>
         <v>0.253549803209204</v>
       </c>
       <c r="F13" s="26"/>
-      <c r="N13" s="47"/>
+      <c r="N13" s="46"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="66" t="n">
+      <c r="B14" s="65" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>1610342</v>
       </c>
-      <c r="C14" s="66" t="n">
+      <c r="C14" s="65" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>1749779</v>
       </c>
-      <c r="D14" s="66" t="n">
+      <c r="D14" s="65" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>920715</v>
       </c>
-      <c r="E14" s="34" t="n">
+      <c r="E14" s="33" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>0.0865884389775588</v>
       </c>
-      <c r="F14" s="34" t="n">
+      <c r="F14" s="33" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>-0.167196128072357</v>
       </c>
-      <c r="N14" s="47"/>
+      <c r="N14" s="46"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3529,26 +3519,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="30.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19"/>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="76" t="s">
+      <c r="F1" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
       <c r="M1" s="5" t="s">
         <v>4</v>
       </c>
@@ -3577,15 +3567,15 @@
         <f aca="false">(D2-C2)/C2</f>
         <v>0.104134835752483</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
       <c r="M2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="27" t="s">
+      <c r="N2" s="10" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3596,7 +3586,7 @@
       <c r="B3" s="25" t="n">
         <v>37545</v>
       </c>
-      <c r="C3" s="45" t="n">
+      <c r="C3" s="44" t="n">
         <v>50219</v>
       </c>
       <c r="D3" s="25" t="n">
@@ -3610,15 +3600,15 @@
         <f aca="false">(D3-C3)/C3</f>
         <v>-0.336207411537466</v>
       </c>
-      <c r="G3" s="78" t="s">
+      <c r="G3" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="27"/>
+      <c r="N3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
@@ -3627,7 +3617,7 @@
       <c r="B4" s="25" t="n">
         <v>25781.81</v>
       </c>
-      <c r="C4" s="45" t="n">
+      <c r="C4" s="44" t="n">
         <v>45023</v>
       </c>
       <c r="D4" s="25"/>
@@ -3639,13 +3629,13 @@
         <f aca="false">(D4-C4)/C4</f>
         <v>-1</v>
       </c>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="27"/>
+      <c r="N4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
@@ -3654,7 +3644,7 @@
       <c r="B5" s="25" t="n">
         <v>25781.81</v>
       </c>
-      <c r="C5" s="45" t="n">
+      <c r="C5" s="44" t="n">
         <v>25839</v>
       </c>
       <c r="D5" s="25"/>
@@ -3666,13 +3656,13 @@
         <f aca="false">(D5-C5)/C5</f>
         <v>-1</v>
       </c>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="27"/>
+      <c r="N5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
@@ -3681,7 +3671,7 @@
       <c r="B6" s="25" t="n">
         <v>13432.28</v>
       </c>
-      <c r="C6" s="45" t="n">
+      <c r="C6" s="44" t="n">
         <v>12769</v>
       </c>
       <c r="D6" s="25"/>
@@ -3693,13 +3683,13 @@
         <f aca="false">(D6-C6)/C6</f>
         <v>-1</v>
       </c>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="27"/>
+      <c r="N6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
@@ -3708,7 +3698,7 @@
       <c r="B7" s="25" t="n">
         <v>15430.56</v>
       </c>
-      <c r="C7" s="45" t="n">
+      <c r="C7" s="44" t="n">
         <v>10444</v>
       </c>
       <c r="D7" s="25"/>
@@ -3720,13 +3710,13 @@
         <f aca="false">(D7-C7)/C7</f>
         <v>-1</v>
       </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="27"/>
+      <c r="N7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
@@ -3747,13 +3737,13 @@
         <f aca="false">(D8-C8)/C8</f>
         <v>-1</v>
       </c>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="58"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="57"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="27"/>
+      <c r="N8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
@@ -3774,89 +3764,89 @@
         <f aca="false">(D9-C9)/C9</f>
         <v>-1</v>
       </c>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="27"/>
+      <c r="N9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="70" t="s">
+      <c r="A10" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="28" t="n">
+      <c r="B10" s="27" t="n">
         <v>23032</v>
       </c>
       <c r="C10" s="25" t="n">
         <v>11779</v>
       </c>
       <c r="D10" s="25"/>
-      <c r="E10" s="30" t="n">
+      <c r="E10" s="29" t="n">
         <f aca="false">(C10-B10)/B10</f>
         <v>-0.488581104550191</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="27"/>
+      <c r="N10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="28" t="n">
+      <c r="B11" s="27" t="n">
         <v>36770</v>
       </c>
       <c r="C11" s="25" t="n">
         <v>23418</v>
       </c>
       <c r="D11" s="25"/>
-      <c r="E11" s="30" t="n">
+      <c r="E11" s="29" t="n">
         <f aca="false">(C11-B11)/B11</f>
         <v>-0.3631221104161</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="58"/>
+      <c r="G11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="27"/>
+      <c r="N11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="70" t="s">
+      <c r="A12" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="28" t="n">
+      <c r="B12" s="27" t="n">
         <v>40381</v>
       </c>
       <c r="C12" s="25" t="n">
         <v>34717</v>
       </c>
       <c r="D12" s="25"/>
-      <c r="E12" s="30" t="n">
+      <c r="E12" s="29" t="n">
         <f aca="false">(C12-B12)/B12</f>
         <v>-0.140263985537753</v>
       </c>
       <c r="F12" s="9"/>
-      <c r="G12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="58"/>
+      <c r="G12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
       <c r="M12" s="5"/>
-      <c r="N12" s="27"/>
+      <c r="N12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="79" t="n">
+      <c r="B13" s="78" t="n">
         <v>34355</v>
       </c>
       <c r="C13" s="25" t="n">
@@ -3868,84 +3858,84 @@
         <v>0.0611264735846311</v>
       </c>
       <c r="F13" s="9"/>
-      <c r="G13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="58"/>
+      <c r="G13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
       <c r="M13" s="5"/>
-      <c r="N13" s="27"/>
+      <c r="N13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="66" t="n">
+      <c r="B14" s="65" t="n">
         <f aca="false">SUM(B2:B13)</f>
         <v>307130.98</v>
       </c>
-      <c r="C14" s="66" t="n">
+      <c r="C14" s="65" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>313121</v>
       </c>
-      <c r="D14" s="33" t="n">
+      <c r="D14" s="32" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>79585</v>
       </c>
-      <c r="E14" s="34" t="n">
+      <c r="E14" s="33" t="n">
         <f aca="false">(C14-B14)/B14</f>
         <v>0.0195031448797514</v>
       </c>
-      <c r="F14" s="35" t="n">
+      <c r="F14" s="34" t="n">
         <f aca="false">AVERAGE(F2:F13)</f>
         <v>-0.779009071973123</v>
       </c>
-      <c r="G14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="58"/>
+      <c r="G14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
       <c r="M14" s="5"/>
-      <c r="N14" s="27"/>
+      <c r="N14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="80"/>
-      <c r="B15" s="81" t="s">
+      <c r="A15" s="79"/>
+      <c r="B15" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="81" t="s">
+      <c r="C15" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="81"/>
-      <c r="E15" s="40" t="s">
+      <c r="D15" s="80"/>
+      <c r="E15" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="82"/>
-      <c r="G15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="58"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
       <c r="M15" s="5"/>
-      <c r="N15" s="27"/>
+      <c r="N15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="80"/>
-      <c r="B16" s="83" t="n">
+      <c r="A16" s="79"/>
+      <c r="B16" s="82" t="n">
         <v>331445.11</v>
       </c>
-      <c r="C16" s="83" t="n">
+      <c r="C16" s="82" t="n">
         <v>272775.98</v>
       </c>
-      <c r="D16" s="81"/>
+      <c r="D16" s="80"/>
       <c r="E16" s="9" t="n">
         <f aca="false">(C16-B16)/C16</f>
         <v>-0.215081731170025</v>
       </c>
-      <c r="F16" s="82"/>
-      <c r="G16" s="58"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="58"/>
-      <c r="K16" s="58"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
       <c r="M16" s="5"/>
-      <c r="N16" s="27"/>
+      <c r="N16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M17" s="17" t="s">

</xml_diff>